<commit_message>
Fix error in programs and modified documents
</commit_message>
<xml_diff>
--- a/planificacion/planificacion.xlsx
+++ b/planificacion/planificacion.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D60751-34A9-4567-A8AA-0C1224F42692}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CB51A4-E6CB-4011-AAA9-67D0BF9FF3A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6810" yWindow="3810" windowWidth="15330" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version actual" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
   <si>
     <t>Tareas</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>Analizar caso de estudio y sacar conclusiones</t>
+  </si>
+  <si>
+    <t>Iteración 6</t>
   </si>
 </sst>
 </file>
@@ -730,6 +733,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -763,17 +777,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1062,8 +1065,8 @@
   <dimension ref="A1:BG129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AW114" sqref="AW114:AZ114"/>
+      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BA116" sqref="BA116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,88 +1082,88 @@
   <sheetData>
     <row r="1" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1"/>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="48" t="s">
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="49" t="s">
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="48" t="s">
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="53" t="s">
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="56" t="s">
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="57" t="s">
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
-      <c r="AG1" s="58"/>
-      <c r="AH1" s="48" t="s">
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="69"/>
+      <c r="AH1" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="AI1" s="49"/>
-      <c r="AJ1" s="49"/>
-      <c r="AK1" s="49"/>
-      <c r="AL1" s="50"/>
-      <c r="AM1" s="48" t="s">
+      <c r="AI1" s="60"/>
+      <c r="AJ1" s="60"/>
+      <c r="AK1" s="60"/>
+      <c r="AL1" s="61"/>
+      <c r="AM1" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="AN1" s="49"/>
-      <c r="AO1" s="49"/>
-      <c r="AP1" s="50"/>
-      <c r="AQ1" s="48" t="s">
+      <c r="AN1" s="60"/>
+      <c r="AO1" s="60"/>
+      <c r="AP1" s="61"/>
+      <c r="AQ1" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="AR1" s="49"/>
-      <c r="AS1" s="49"/>
-      <c r="AT1" s="50"/>
-      <c r="AU1" s="48" t="s">
+      <c r="AR1" s="60"/>
+      <c r="AS1" s="60"/>
+      <c r="AT1" s="61"/>
+      <c r="AU1" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="AV1" s="49"/>
-      <c r="AW1" s="49"/>
-      <c r="AX1" s="49"/>
-      <c r="AY1" s="50"/>
-      <c r="AZ1" s="48" t="s">
+      <c r="AV1" s="60"/>
+      <c r="AW1" s="60"/>
+      <c r="AX1" s="60"/>
+      <c r="AY1" s="61"/>
+      <c r="AZ1" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="BA1" s="49"/>
-      <c r="BB1" s="49"/>
-      <c r="BC1" s="50"/>
-      <c r="BD1" s="48" t="s">
+      <c r="BA1" s="60"/>
+      <c r="BB1" s="60"/>
+      <c r="BC1" s="61"/>
+      <c r="BD1" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="BE1" s="49"/>
-      <c r="BF1" s="49"/>
-      <c r="BG1" s="50"/>
+      <c r="BE1" s="60"/>
+      <c r="BF1" s="60"/>
+      <c r="BG1" s="61"/>
     </row>
     <row r="2" spans="1:59" ht="69.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1467,7 +1470,7 @@
       <c r="BF4" s="15"/>
       <c r="BG4" s="15"/>
     </row>
-    <row r="5" spans="1:59" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="11" t="s">
         <v>35</v>
@@ -1483,7 +1486,6 @@
       <c r="K5" s="13"/>
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
-      <c r="N5" s="17"/>
       <c r="O5" s="15"/>
       <c r="P5" s="15"/>
       <c r="Q5" s="15"/>
@@ -1504,7 +1506,7 @@
       <c r="AF5" s="10"/>
       <c r="AG5" s="31"/>
       <c r="AH5" s="25"/>
-      <c r="AI5" s="15"/>
+      <c r="AI5" s="17"/>
       <c r="AJ5" s="15"/>
       <c r="AK5" s="15"/>
       <c r="AL5" s="15"/>
@@ -3793,10 +3795,10 @@
       <c r="M42" s="1"/>
       <c r="N42" s="18"/>
       <c r="O42" s="18"/>
-      <c r="P42" s="59"/>
-      <c r="Q42" s="59"/>
-      <c r="R42" s="59"/>
-      <c r="S42" s="59"/>
+      <c r="P42" s="48"/>
+      <c r="Q42" s="48"/>
+      <c r="R42" s="48"/>
+      <c r="S42" s="48"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
@@ -3855,10 +3857,10 @@
       <c r="M43" s="1"/>
       <c r="N43" s="18"/>
       <c r="O43" s="18"/>
-      <c r="P43" s="59"/>
-      <c r="Q43" s="59"/>
-      <c r="R43" s="59"/>
-      <c r="S43" s="59"/>
+      <c r="P43" s="48"/>
+      <c r="Q43" s="48"/>
+      <c r="R43" s="48"/>
+      <c r="S43" s="48"/>
       <c r="U43" s="1"/>
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
@@ -4040,8 +4042,8 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
-      <c r="S46" s="59"/>
-      <c r="U46" s="59"/>
+      <c r="S46" s="48"/>
+      <c r="U46" s="48"/>
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
       <c r="X46" s="34"/>
@@ -4103,8 +4105,8 @@
       <c r="O47" s="1"/>
       <c r="P47" s="18"/>
       <c r="Q47" s="18"/>
-      <c r="R47" s="59"/>
-      <c r="U47" s="59"/>
+      <c r="R47" s="48"/>
+      <c r="U47" s="48"/>
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
       <c r="X47" s="34"/>
@@ -4164,8 +4166,8 @@
       <c r="O48" s="1"/>
       <c r="P48" s="18"/>
       <c r="Q48" s="18"/>
-      <c r="R48" s="59"/>
-      <c r="U48" s="59"/>
+      <c r="R48" s="48"/>
+      <c r="U48" s="48"/>
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
       <c r="X48" s="34"/>
@@ -4223,8 +4225,8 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
-      <c r="R49" s="59"/>
-      <c r="U49" s="59"/>
+      <c r="R49" s="48"/>
+      <c r="U49" s="48"/>
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
       <c r="X49" s="34"/>
@@ -4537,7 +4539,7 @@
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
       <c r="V54" s="4"/>
-      <c r="W54" s="60"/>
+      <c r="W54" s="49"/>
       <c r="X54" s="9"/>
       <c r="Y54" s="6"/>
       <c r="Z54" s="4"/>
@@ -4600,7 +4602,7 @@
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
       <c r="V55" s="4"/>
-      <c r="W55" s="60"/>
+      <c r="W55" s="49"/>
       <c r="X55" s="9"/>
       <c r="Y55" s="6"/>
       <c r="Z55" s="4"/>
@@ -4663,7 +4665,7 @@
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
       <c r="V56" s="4"/>
-      <c r="W56" s="60"/>
+      <c r="W56" s="49"/>
       <c r="X56" s="9"/>
       <c r="Y56" s="6"/>
       <c r="Z56" s="4"/>
@@ -4724,7 +4726,7 @@
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
       <c r="V57" s="4"/>
-      <c r="W57" s="60"/>
+      <c r="W57" s="49"/>
       <c r="X57" s="9"/>
       <c r="Y57" s="6"/>
       <c r="Z57" s="4"/>
@@ -4785,7 +4787,7 @@
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
       <c r="V58" s="4"/>
-      <c r="W58" s="60"/>
+      <c r="W58" s="49"/>
       <c r="X58" s="9"/>
       <c r="Y58" s="6"/>
       <c r="Z58" s="4"/>
@@ -4850,7 +4852,7 @@
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
       <c r="V59" s="4"/>
-      <c r="W59" s="60"/>
+      <c r="W59" s="49"/>
       <c r="X59" s="9"/>
       <c r="Y59" s="6"/>
       <c r="Z59" s="4"/>
@@ -4913,7 +4915,7 @@
       <c r="T60" s="1"/>
       <c r="U60" s="1"/>
       <c r="V60" s="4"/>
-      <c r="W60" s="60"/>
+      <c r="W60" s="49"/>
       <c r="X60" s="9"/>
       <c r="Y60" s="6"/>
       <c r="Z60" s="4"/>
@@ -4975,28 +4977,28 @@
       <c r="U61" s="1"/>
       <c r="V61" s="4"/>
       <c r="W61" s="35"/>
-      <c r="X61" s="61"/>
-      <c r="Y61" s="62"/>
+      <c r="X61" s="50"/>
+      <c r="Y61" s="51"/>
       <c r="Z61" s="4"/>
       <c r="AA61" s="4"/>
       <c r="AB61" s="4"/>
       <c r="AC61" s="4"/>
       <c r="AD61" s="4"/>
       <c r="AE61" s="4"/>
-      <c r="AF61" s="59"/>
-      <c r="AG61" s="66"/>
-      <c r="AH61" s="68"/>
-      <c r="AI61" s="59"/>
-      <c r="AJ61" s="59"/>
-      <c r="AK61" s="59"/>
-      <c r="AL61" s="59"/>
-      <c r="AM61" s="59"/>
-      <c r="AN61" s="59"/>
-      <c r="AO61" s="59"/>
-      <c r="AP61" s="59"/>
-      <c r="AQ61" s="59"/>
-      <c r="AR61" s="59"/>
-      <c r="AS61" s="59"/>
+      <c r="AF61" s="48"/>
+      <c r="AG61" s="55"/>
+      <c r="AH61" s="57"/>
+      <c r="AI61" s="48"/>
+      <c r="AJ61" s="48"/>
+      <c r="AK61" s="48"/>
+      <c r="AL61" s="48"/>
+      <c r="AM61" s="48"/>
+      <c r="AN61" s="48"/>
+      <c r="AO61" s="48"/>
+      <c r="AP61" s="48"/>
+      <c r="AQ61" s="48"/>
+      <c r="AR61" s="48"/>
+      <c r="AS61" s="48"/>
       <c r="AT61" s="4"/>
       <c r="AU61" s="4"/>
       <c r="AV61" s="4"/>
@@ -5036,28 +5038,28 @@
       <c r="U62" s="1"/>
       <c r="V62" s="4"/>
       <c r="W62" s="35"/>
-      <c r="X62" s="63"/>
-      <c r="Y62" s="64"/>
-      <c r="Z62" s="65"/>
+      <c r="X62" s="52"/>
+      <c r="Y62" s="53"/>
+      <c r="Z62" s="54"/>
       <c r="AA62" s="4"/>
       <c r="AB62" s="4"/>
       <c r="AC62" s="4"/>
       <c r="AD62" s="4"/>
       <c r="AE62" s="4"/>
-      <c r="AF62" s="59"/>
-      <c r="AG62" s="66"/>
-      <c r="AH62" s="68"/>
-      <c r="AI62" s="59"/>
-      <c r="AJ62" s="59"/>
-      <c r="AK62" s="59"/>
-      <c r="AL62" s="59"/>
-      <c r="AM62" s="59"/>
-      <c r="AN62" s="59"/>
-      <c r="AO62" s="59"/>
-      <c r="AP62" s="59"/>
-      <c r="AQ62" s="59"/>
-      <c r="AR62" s="59"/>
-      <c r="AS62" s="59"/>
+      <c r="AF62" s="48"/>
+      <c r="AG62" s="55"/>
+      <c r="AH62" s="57"/>
+      <c r="AI62" s="48"/>
+      <c r="AJ62" s="48"/>
+      <c r="AK62" s="48"/>
+      <c r="AL62" s="48"/>
+      <c r="AM62" s="48"/>
+      <c r="AN62" s="48"/>
+      <c r="AO62" s="48"/>
+      <c r="AP62" s="48"/>
+      <c r="AQ62" s="48"/>
+      <c r="AR62" s="48"/>
+      <c r="AS62" s="48"/>
       <c r="AT62" s="4"/>
       <c r="AU62" s="4"/>
       <c r="AV62" s="4"/>
@@ -5101,28 +5103,28 @@
       <c r="U63" s="1"/>
       <c r="V63" s="4"/>
       <c r="W63" s="35"/>
-      <c r="X63" s="63"/>
-      <c r="Y63" s="64"/>
-      <c r="Z63" s="65"/>
+      <c r="X63" s="52"/>
+      <c r="Y63" s="53"/>
+      <c r="Z63" s="54"/>
       <c r="AA63" s="4"/>
       <c r="AB63" s="4"/>
       <c r="AC63" s="4"/>
       <c r="AD63" s="4"/>
       <c r="AE63" s="4"/>
-      <c r="AF63" s="59"/>
-      <c r="AG63" s="66"/>
-      <c r="AH63" s="69"/>
-      <c r="AI63" s="59"/>
-      <c r="AJ63" s="59"/>
-      <c r="AK63" s="59"/>
-      <c r="AL63" s="59"/>
-      <c r="AM63" s="59"/>
-      <c r="AN63" s="59"/>
-      <c r="AO63" s="59"/>
-      <c r="AP63" s="59"/>
-      <c r="AQ63" s="59"/>
-      <c r="AR63" s="59"/>
-      <c r="AS63" s="59"/>
+      <c r="AF63" s="48"/>
+      <c r="AG63" s="55"/>
+      <c r="AH63" s="58"/>
+      <c r="AI63" s="48"/>
+      <c r="AJ63" s="48"/>
+      <c r="AK63" s="48"/>
+      <c r="AL63" s="48"/>
+      <c r="AM63" s="48"/>
+      <c r="AN63" s="48"/>
+      <c r="AO63" s="48"/>
+      <c r="AP63" s="48"/>
+      <c r="AQ63" s="48"/>
+      <c r="AR63" s="48"/>
+      <c r="AS63" s="48"/>
       <c r="AT63" s="4"/>
       <c r="AU63" s="4"/>
       <c r="AV63" s="4"/>
@@ -5164,28 +5166,28 @@
       <c r="U64" s="4"/>
       <c r="V64" s="4"/>
       <c r="W64" s="35"/>
-      <c r="X64" s="63"/>
-      <c r="Y64" s="65"/>
-      <c r="Z64" s="65"/>
+      <c r="X64" s="52"/>
+      <c r="Y64" s="54"/>
+      <c r="Z64" s="54"/>
       <c r="AA64" s="4"/>
       <c r="AB64" s="4"/>
       <c r="AC64" s="4"/>
       <c r="AD64" s="4"/>
       <c r="AE64" s="4"/>
-      <c r="AF64" s="59"/>
-      <c r="AG64" s="66"/>
-      <c r="AH64" s="68"/>
-      <c r="AI64" s="59"/>
-      <c r="AJ64" s="59"/>
-      <c r="AK64" s="59"/>
-      <c r="AL64" s="59"/>
-      <c r="AM64" s="59"/>
-      <c r="AN64" s="59"/>
-      <c r="AO64" s="59"/>
-      <c r="AP64" s="59"/>
-      <c r="AQ64" s="59"/>
-      <c r="AR64" s="59"/>
-      <c r="AS64" s="59"/>
+      <c r="AF64" s="48"/>
+      <c r="AG64" s="55"/>
+      <c r="AH64" s="57"/>
+      <c r="AI64" s="48"/>
+      <c r="AJ64" s="48"/>
+      <c r="AK64" s="48"/>
+      <c r="AL64" s="48"/>
+      <c r="AM64" s="48"/>
+      <c r="AN64" s="48"/>
+      <c r="AO64" s="48"/>
+      <c r="AP64" s="48"/>
+      <c r="AQ64" s="48"/>
+      <c r="AR64" s="48"/>
+      <c r="AS64" s="48"/>
       <c r="AT64" s="4"/>
       <c r="AU64" s="4"/>
       <c r="AV64" s="4"/>
@@ -5233,20 +5235,20 @@
       <c r="AC65" s="4"/>
       <c r="AD65" s="4"/>
       <c r="AE65" s="4"/>
-      <c r="AF65" s="59"/>
-      <c r="AG65" s="66"/>
-      <c r="AH65" s="67"/>
-      <c r="AI65" s="59"/>
-      <c r="AJ65" s="59"/>
-      <c r="AK65" s="59"/>
-      <c r="AL65" s="59"/>
-      <c r="AM65" s="59"/>
-      <c r="AN65" s="59"/>
-      <c r="AO65" s="59"/>
-      <c r="AP65" s="59"/>
-      <c r="AQ65" s="59"/>
-      <c r="AR65" s="59"/>
-      <c r="AS65" s="59"/>
+      <c r="AF65" s="48"/>
+      <c r="AG65" s="55"/>
+      <c r="AH65" s="56"/>
+      <c r="AI65" s="48"/>
+      <c r="AJ65" s="48"/>
+      <c r="AK65" s="48"/>
+      <c r="AL65" s="48"/>
+      <c r="AM65" s="48"/>
+      <c r="AN65" s="48"/>
+      <c r="AO65" s="48"/>
+      <c r="AP65" s="48"/>
+      <c r="AQ65" s="48"/>
+      <c r="AR65" s="48"/>
+      <c r="AS65" s="48"/>
       <c r="AT65" s="4"/>
       <c r="AU65" s="4"/>
       <c r="AV65" s="4"/>
@@ -5298,20 +5300,20 @@
       <c r="AC66" s="4"/>
       <c r="AD66" s="4"/>
       <c r="AE66" s="4"/>
-      <c r="AF66" s="59"/>
-      <c r="AG66" s="66"/>
-      <c r="AH66" s="67"/>
-      <c r="AI66" s="59"/>
-      <c r="AJ66" s="59"/>
-      <c r="AK66" s="59"/>
-      <c r="AL66" s="59"/>
-      <c r="AM66" s="59"/>
-      <c r="AN66" s="59"/>
-      <c r="AO66" s="59"/>
-      <c r="AP66" s="59"/>
-      <c r="AQ66" s="59"/>
-      <c r="AR66" s="59"/>
-      <c r="AS66" s="59"/>
+      <c r="AF66" s="48"/>
+      <c r="AG66" s="55"/>
+      <c r="AH66" s="56"/>
+      <c r="AI66" s="48"/>
+      <c r="AJ66" s="48"/>
+      <c r="AK66" s="48"/>
+      <c r="AL66" s="48"/>
+      <c r="AM66" s="48"/>
+      <c r="AN66" s="48"/>
+      <c r="AO66" s="48"/>
+      <c r="AP66" s="48"/>
+      <c r="AQ66" s="48"/>
+      <c r="AR66" s="48"/>
+      <c r="AS66" s="48"/>
       <c r="AT66" s="4"/>
       <c r="AU66" s="4"/>
       <c r="AV66" s="4"/>
@@ -5361,20 +5363,20 @@
       <c r="AC67" s="4"/>
       <c r="AD67" s="4"/>
       <c r="AE67" s="4"/>
-      <c r="AF67" s="59"/>
-      <c r="AG67" s="66"/>
-      <c r="AH67" s="67"/>
-      <c r="AI67" s="59"/>
-      <c r="AJ67" s="59"/>
-      <c r="AK67" s="59"/>
-      <c r="AL67" s="59"/>
-      <c r="AM67" s="59"/>
-      <c r="AN67" s="59"/>
-      <c r="AO67" s="59"/>
-      <c r="AP67" s="59"/>
-      <c r="AQ67" s="59"/>
-      <c r="AR67" s="59"/>
-      <c r="AS67" s="59"/>
+      <c r="AF67" s="48"/>
+      <c r="AG67" s="55"/>
+      <c r="AH67" s="56"/>
+      <c r="AI67" s="48"/>
+      <c r="AJ67" s="48"/>
+      <c r="AK67" s="48"/>
+      <c r="AL67" s="48"/>
+      <c r="AM67" s="48"/>
+      <c r="AN67" s="48"/>
+      <c r="AO67" s="48"/>
+      <c r="AP67" s="48"/>
+      <c r="AQ67" s="48"/>
+      <c r="AR67" s="48"/>
+      <c r="AS67" s="48"/>
       <c r="AT67" s="4"/>
       <c r="AU67" s="4"/>
       <c r="AV67" s="4"/>
@@ -5421,20 +5423,20 @@
       <c r="AC68" s="4"/>
       <c r="AD68" s="4"/>
       <c r="AE68" s="4"/>
-      <c r="AF68" s="59"/>
-      <c r="AG68" s="66"/>
-      <c r="AH68" s="67"/>
-      <c r="AI68" s="59"/>
-      <c r="AJ68" s="59"/>
-      <c r="AK68" s="59"/>
-      <c r="AL68" s="59"/>
-      <c r="AM68" s="59"/>
-      <c r="AN68" s="59"/>
-      <c r="AO68" s="59"/>
-      <c r="AP68" s="59"/>
-      <c r="AQ68" s="59"/>
-      <c r="AR68" s="59"/>
-      <c r="AS68" s="59"/>
+      <c r="AF68" s="48"/>
+      <c r="AG68" s="55"/>
+      <c r="AH68" s="56"/>
+      <c r="AI68" s="48"/>
+      <c r="AJ68" s="48"/>
+      <c r="AK68" s="48"/>
+      <c r="AL68" s="48"/>
+      <c r="AM68" s="48"/>
+      <c r="AN68" s="48"/>
+      <c r="AO68" s="48"/>
+      <c r="AP68" s="48"/>
+      <c r="AQ68" s="48"/>
+      <c r="AR68" s="48"/>
+      <c r="AS68" s="48"/>
       <c r="AT68" s="4"/>
       <c r="AU68" s="4"/>
       <c r="AV68" s="4"/>
@@ -5484,20 +5486,20 @@
       <c r="AC69" s="4"/>
       <c r="AD69" s="4"/>
       <c r="AE69" s="4"/>
-      <c r="AF69" s="59"/>
-      <c r="AG69" s="66"/>
-      <c r="AH69" s="67"/>
-      <c r="AI69" s="59"/>
-      <c r="AJ69" s="59"/>
-      <c r="AK69" s="59"/>
-      <c r="AL69" s="59"/>
-      <c r="AM69" s="59"/>
-      <c r="AN69" s="59"/>
-      <c r="AO69" s="59"/>
-      <c r="AP69" s="59"/>
-      <c r="AQ69" s="59"/>
-      <c r="AR69" s="59"/>
-      <c r="AS69" s="59"/>
+      <c r="AF69" s="48"/>
+      <c r="AG69" s="55"/>
+      <c r="AH69" s="56"/>
+      <c r="AI69" s="48"/>
+      <c r="AJ69" s="48"/>
+      <c r="AK69" s="48"/>
+      <c r="AL69" s="48"/>
+      <c r="AM69" s="48"/>
+      <c r="AN69" s="48"/>
+      <c r="AO69" s="48"/>
+      <c r="AP69" s="48"/>
+      <c r="AQ69" s="48"/>
+      <c r="AR69" s="48"/>
+      <c r="AS69" s="48"/>
       <c r="AT69" s="4"/>
       <c r="AU69" s="4"/>
       <c r="AV69" s="4"/>
@@ -5622,23 +5624,23 @@
       <c r="AK71" s="4"/>
       <c r="AL71" s="4"/>
       <c r="AM71" s="4"/>
-      <c r="AN71" s="59"/>
-      <c r="AO71" s="59"/>
-      <c r="AP71" s="59"/>
-      <c r="AQ71" s="59"/>
-      <c r="AR71" s="59"/>
-      <c r="AS71" s="59"/>
-      <c r="AT71" s="59"/>
-      <c r="AU71" s="59"/>
-      <c r="AV71" s="59"/>
-      <c r="AW71" s="59"/>
-      <c r="AX71" s="59"/>
-      <c r="AY71" s="59"/>
-      <c r="AZ71" s="59"/>
+      <c r="AN71" s="48"/>
+      <c r="AO71" s="48"/>
+      <c r="AP71" s="48"/>
+      <c r="AQ71" s="48"/>
+      <c r="AR71" s="48"/>
+      <c r="AS71" s="48"/>
+      <c r="AT71" s="48"/>
+      <c r="AU71" s="48"/>
+      <c r="AV71" s="48"/>
+      <c r="AW71" s="48"/>
+      <c r="AX71" s="48"/>
+      <c r="AY71" s="48"/>
+      <c r="AZ71" s="48"/>
       <c r="BA71" s="4"/>
       <c r="BB71" s="4"/>
       <c r="BC71" s="4"/>
-      <c r="BD71" s="59"/>
+      <c r="BD71" s="48"/>
       <c r="BE71" s="4"/>
       <c r="BF71" s="4"/>
       <c r="BG71" s="4"/>
@@ -5685,23 +5687,23 @@
       <c r="AK72" s="4"/>
       <c r="AL72" s="4"/>
       <c r="AM72" s="4"/>
-      <c r="AN72" s="59"/>
-      <c r="AO72" s="59"/>
-      <c r="AP72" s="59"/>
-      <c r="AQ72" s="59"/>
-      <c r="AR72" s="59"/>
-      <c r="AS72" s="59"/>
-      <c r="AT72" s="59"/>
-      <c r="AU72" s="59"/>
-      <c r="AV72" s="59"/>
-      <c r="AW72" s="59"/>
-      <c r="AX72" s="59"/>
-      <c r="AY72" s="59"/>
-      <c r="AZ72" s="59"/>
+      <c r="AN72" s="48"/>
+      <c r="AO72" s="48"/>
+      <c r="AP72" s="48"/>
+      <c r="AQ72" s="48"/>
+      <c r="AR72" s="48"/>
+      <c r="AS72" s="48"/>
+      <c r="AT72" s="48"/>
+      <c r="AU72" s="48"/>
+      <c r="AV72" s="48"/>
+      <c r="AW72" s="48"/>
+      <c r="AX72" s="48"/>
+      <c r="AY72" s="48"/>
+      <c r="AZ72" s="48"/>
       <c r="BA72" s="4"/>
       <c r="BB72" s="4"/>
       <c r="BC72" s="4"/>
-      <c r="BD72" s="59"/>
+      <c r="BD72" s="48"/>
       <c r="BE72" s="4"/>
       <c r="BF72" s="4"/>
       <c r="BG72" s="4"/>
@@ -5748,23 +5750,23 @@
       <c r="AK73" s="4"/>
       <c r="AL73" s="4"/>
       <c r="AM73" s="4"/>
-      <c r="AN73" s="59"/>
-      <c r="AO73" s="59"/>
-      <c r="AP73" s="59"/>
-      <c r="AQ73" s="59"/>
-      <c r="AR73" s="59"/>
-      <c r="AS73" s="59"/>
-      <c r="AT73" s="59"/>
-      <c r="AU73" s="59"/>
-      <c r="AV73" s="59"/>
-      <c r="AW73" s="59"/>
-      <c r="AX73" s="59"/>
-      <c r="AY73" s="59"/>
-      <c r="AZ73" s="59"/>
+      <c r="AN73" s="48"/>
+      <c r="AO73" s="48"/>
+      <c r="AP73" s="48"/>
+      <c r="AQ73" s="48"/>
+      <c r="AR73" s="48"/>
+      <c r="AS73" s="48"/>
+      <c r="AT73" s="48"/>
+      <c r="AU73" s="48"/>
+      <c r="AV73" s="48"/>
+      <c r="AW73" s="48"/>
+      <c r="AX73" s="48"/>
+      <c r="AY73" s="48"/>
+      <c r="AZ73" s="48"/>
       <c r="BA73" s="4"/>
       <c r="BB73" s="4"/>
       <c r="BC73" s="4"/>
-      <c r="BD73" s="59"/>
+      <c r="BD73" s="48"/>
       <c r="BE73" s="4"/>
       <c r="BF73" s="4"/>
       <c r="BG73" s="4"/>
@@ -5789,7 +5791,7 @@
       <c r="Q74" s="4"/>
       <c r="R74" s="4"/>
       <c r="S74" s="4"/>
-      <c r="T74" s="59"/>
+      <c r="T74" s="48"/>
       <c r="U74" s="4"/>
       <c r="V74" s="4"/>
       <c r="W74" s="6"/>
@@ -5809,23 +5811,23 @@
       <c r="AK74" s="4"/>
       <c r="AL74" s="4"/>
       <c r="AM74" s="4"/>
-      <c r="AN74" s="59"/>
-      <c r="AO74" s="59"/>
-      <c r="AP74" s="59"/>
-      <c r="AQ74" s="59"/>
-      <c r="AR74" s="59"/>
-      <c r="AS74" s="59"/>
-      <c r="AT74" s="59"/>
-      <c r="AU74" s="59"/>
-      <c r="AV74" s="59"/>
-      <c r="AW74" s="59"/>
-      <c r="AX74" s="59"/>
-      <c r="AY74" s="59"/>
-      <c r="AZ74" s="59"/>
+      <c r="AN74" s="48"/>
+      <c r="AO74" s="48"/>
+      <c r="AP74" s="48"/>
+      <c r="AQ74" s="48"/>
+      <c r="AR74" s="48"/>
+      <c r="AS74" s="48"/>
+      <c r="AT74" s="48"/>
+      <c r="AU74" s="48"/>
+      <c r="AV74" s="48"/>
+      <c r="AW74" s="48"/>
+      <c r="AX74" s="48"/>
+      <c r="AY74" s="48"/>
+      <c r="AZ74" s="48"/>
       <c r="BA74" s="4"/>
       <c r="BB74" s="4"/>
       <c r="BC74" s="4"/>
-      <c r="BD74" s="59"/>
+      <c r="BD74" s="48"/>
       <c r="BE74" s="4"/>
       <c r="BF74" s="4"/>
       <c r="BG74" s="4"/>
@@ -5870,23 +5872,23 @@
       <c r="AK75" s="4"/>
       <c r="AL75" s="4"/>
       <c r="AM75" s="4"/>
-      <c r="AN75" s="59"/>
-      <c r="AO75" s="59"/>
-      <c r="AP75" s="59"/>
-      <c r="AQ75" s="59"/>
-      <c r="AR75" s="59"/>
-      <c r="AS75" s="59"/>
-      <c r="AT75" s="59"/>
-      <c r="AU75" s="59"/>
-      <c r="AV75" s="59"/>
-      <c r="AW75" s="59"/>
-      <c r="AX75" s="59"/>
-      <c r="AY75" s="59"/>
-      <c r="AZ75" s="59"/>
+      <c r="AN75" s="48"/>
+      <c r="AO75" s="48"/>
+      <c r="AP75" s="48"/>
+      <c r="AQ75" s="48"/>
+      <c r="AR75" s="48"/>
+      <c r="AS75" s="48"/>
+      <c r="AT75" s="48"/>
+      <c r="AU75" s="48"/>
+      <c r="AV75" s="48"/>
+      <c r="AW75" s="48"/>
+      <c r="AX75" s="48"/>
+      <c r="AY75" s="48"/>
+      <c r="AZ75" s="48"/>
       <c r="BA75" s="4"/>
       <c r="BB75" s="4"/>
       <c r="BC75" s="4"/>
-      <c r="BD75" s="59"/>
+      <c r="BD75" s="48"/>
       <c r="BE75" s="4"/>
       <c r="BF75" s="4"/>
       <c r="BG75" s="4"/>
@@ -5935,23 +5937,23 @@
       <c r="AK76" s="4"/>
       <c r="AL76" s="4"/>
       <c r="AM76" s="4"/>
-      <c r="AN76" s="59"/>
-      <c r="AO76" s="59"/>
-      <c r="AP76" s="59"/>
-      <c r="AQ76" s="59"/>
-      <c r="AR76" s="59"/>
-      <c r="AS76" s="59"/>
-      <c r="AT76" s="59"/>
-      <c r="AU76" s="59"/>
-      <c r="AV76" s="59"/>
-      <c r="AW76" s="59"/>
-      <c r="AX76" s="59"/>
-      <c r="AY76" s="59"/>
-      <c r="AZ76" s="59"/>
+      <c r="AN76" s="48"/>
+      <c r="AO76" s="48"/>
+      <c r="AP76" s="48"/>
+      <c r="AQ76" s="48"/>
+      <c r="AR76" s="48"/>
+      <c r="AS76" s="48"/>
+      <c r="AT76" s="48"/>
+      <c r="AU76" s="48"/>
+      <c r="AV76" s="48"/>
+      <c r="AW76" s="48"/>
+      <c r="AX76" s="48"/>
+      <c r="AY76" s="48"/>
+      <c r="AZ76" s="48"/>
       <c r="BA76" s="4"/>
       <c r="BB76" s="4"/>
       <c r="BC76" s="4"/>
-      <c r="BD76" s="59"/>
+      <c r="BD76" s="48"/>
       <c r="BE76" s="4"/>
       <c r="BF76" s="4"/>
       <c r="BG76" s="4"/>
@@ -5998,23 +6000,23 @@
       <c r="AK77" s="4"/>
       <c r="AL77" s="4"/>
       <c r="AM77" s="4"/>
-      <c r="AN77" s="59"/>
-      <c r="AO77" s="59"/>
-      <c r="AP77" s="59"/>
-      <c r="AQ77" s="59"/>
-      <c r="AR77" s="59"/>
-      <c r="AS77" s="59"/>
-      <c r="AT77" s="59"/>
-      <c r="AU77" s="59"/>
-      <c r="AV77" s="59"/>
-      <c r="AW77" s="59"/>
-      <c r="AX77" s="59"/>
-      <c r="AY77" s="59"/>
-      <c r="AZ77" s="59"/>
+      <c r="AN77" s="48"/>
+      <c r="AO77" s="48"/>
+      <c r="AP77" s="48"/>
+      <c r="AQ77" s="48"/>
+      <c r="AR77" s="48"/>
+      <c r="AS77" s="48"/>
+      <c r="AT77" s="48"/>
+      <c r="AU77" s="48"/>
+      <c r="AV77" s="48"/>
+      <c r="AW77" s="48"/>
+      <c r="AX77" s="48"/>
+      <c r="AY77" s="48"/>
+      <c r="AZ77" s="48"/>
       <c r="BA77" s="4"/>
       <c r="BB77" s="4"/>
       <c r="BC77" s="4"/>
-      <c r="BD77" s="59"/>
+      <c r="BD77" s="48"/>
       <c r="BE77" s="4"/>
       <c r="BF77" s="4"/>
       <c r="BG77" s="4"/>
@@ -6059,23 +6061,23 @@
       <c r="AK78" s="4"/>
       <c r="AL78" s="4"/>
       <c r="AM78" s="4"/>
-      <c r="AN78" s="59"/>
-      <c r="AO78" s="59"/>
-      <c r="AP78" s="59"/>
-      <c r="AQ78" s="59"/>
-      <c r="AR78" s="59"/>
-      <c r="AS78" s="59"/>
-      <c r="AT78" s="59"/>
-      <c r="AU78" s="59"/>
-      <c r="AV78" s="59"/>
-      <c r="AW78" s="59"/>
-      <c r="AX78" s="59"/>
-      <c r="AY78" s="59"/>
-      <c r="AZ78" s="59"/>
+      <c r="AN78" s="48"/>
+      <c r="AO78" s="48"/>
+      <c r="AP78" s="48"/>
+      <c r="AQ78" s="48"/>
+      <c r="AR78" s="48"/>
+      <c r="AS78" s="48"/>
+      <c r="AT78" s="48"/>
+      <c r="AU78" s="48"/>
+      <c r="AV78" s="48"/>
+      <c r="AW78" s="48"/>
+      <c r="AX78" s="48"/>
+      <c r="AY78" s="48"/>
+      <c r="AZ78" s="48"/>
       <c r="BA78" s="4"/>
       <c r="BB78" s="4"/>
       <c r="BC78" s="4"/>
-      <c r="BD78" s="59"/>
+      <c r="BD78" s="48"/>
       <c r="BE78" s="4"/>
       <c r="BF78" s="4"/>
       <c r="BG78" s="4"/>
@@ -6124,23 +6126,23 @@
       <c r="AK79" s="4"/>
       <c r="AL79" s="4"/>
       <c r="AM79" s="4"/>
-      <c r="AN79" s="59"/>
-      <c r="AO79" s="59"/>
-      <c r="AP79" s="59"/>
-      <c r="AQ79" s="59"/>
-      <c r="AR79" s="59"/>
-      <c r="AS79" s="59"/>
-      <c r="AT79" s="59"/>
-      <c r="AU79" s="59"/>
-      <c r="AV79" s="59"/>
-      <c r="AW79" s="59"/>
-      <c r="AX79" s="59"/>
-      <c r="AY79" s="59"/>
-      <c r="AZ79" s="59"/>
+      <c r="AN79" s="48"/>
+      <c r="AO79" s="48"/>
+      <c r="AP79" s="48"/>
+      <c r="AQ79" s="48"/>
+      <c r="AR79" s="48"/>
+      <c r="AS79" s="48"/>
+      <c r="AT79" s="48"/>
+      <c r="AU79" s="48"/>
+      <c r="AV79" s="48"/>
+      <c r="AW79" s="48"/>
+      <c r="AX79" s="48"/>
+      <c r="AY79" s="48"/>
+      <c r="AZ79" s="48"/>
       <c r="BA79" s="4"/>
       <c r="BB79" s="4"/>
       <c r="BC79" s="4"/>
-      <c r="BD79" s="59"/>
+      <c r="BD79" s="48"/>
       <c r="BE79" s="4"/>
       <c r="BF79" s="4"/>
       <c r="BG79" s="4"/>
@@ -6187,23 +6189,23 @@
       <c r="AK80" s="4"/>
       <c r="AL80" s="4"/>
       <c r="AM80" s="4"/>
-      <c r="AN80" s="59"/>
-      <c r="AO80" s="59"/>
-      <c r="AP80" s="59"/>
-      <c r="AQ80" s="59"/>
-      <c r="AR80" s="59"/>
-      <c r="AS80" s="59"/>
-      <c r="AT80" s="59"/>
-      <c r="AU80" s="59"/>
-      <c r="AV80" s="59"/>
-      <c r="AW80" s="59"/>
-      <c r="AX80" s="59"/>
-      <c r="AY80" s="59"/>
-      <c r="AZ80" s="59"/>
+      <c r="AN80" s="48"/>
+      <c r="AO80" s="48"/>
+      <c r="AP80" s="48"/>
+      <c r="AQ80" s="48"/>
+      <c r="AR80" s="48"/>
+      <c r="AS80" s="48"/>
+      <c r="AT80" s="48"/>
+      <c r="AU80" s="48"/>
+      <c r="AV80" s="48"/>
+      <c r="AW80" s="48"/>
+      <c r="AX80" s="48"/>
+      <c r="AY80" s="48"/>
+      <c r="AZ80" s="48"/>
       <c r="BA80" s="4"/>
       <c r="BB80" s="4"/>
       <c r="BC80" s="4"/>
-      <c r="BD80" s="59"/>
+      <c r="BD80" s="48"/>
       <c r="BE80" s="4"/>
       <c r="BF80" s="4"/>
       <c r="BG80" s="4"/>
@@ -6250,23 +6252,23 @@
       <c r="AK81" s="4"/>
       <c r="AL81" s="4"/>
       <c r="AM81" s="4"/>
-      <c r="AN81" s="59"/>
-      <c r="AO81" s="59"/>
-      <c r="AP81" s="59"/>
-      <c r="AQ81" s="59"/>
-      <c r="AR81" s="59"/>
-      <c r="AS81" s="59"/>
-      <c r="AT81" s="59"/>
-      <c r="AU81" s="59"/>
-      <c r="AV81" s="59"/>
-      <c r="AW81" s="59"/>
-      <c r="AX81" s="59"/>
-      <c r="AY81" s="59"/>
-      <c r="AZ81" s="59"/>
+      <c r="AN81" s="48"/>
+      <c r="AO81" s="48"/>
+      <c r="AP81" s="48"/>
+      <c r="AQ81" s="48"/>
+      <c r="AR81" s="48"/>
+      <c r="AS81" s="48"/>
+      <c r="AT81" s="48"/>
+      <c r="AU81" s="48"/>
+      <c r="AV81" s="48"/>
+      <c r="AW81" s="48"/>
+      <c r="AX81" s="48"/>
+      <c r="AY81" s="48"/>
+      <c r="AZ81" s="48"/>
       <c r="BA81" s="4"/>
       <c r="BB81" s="4"/>
       <c r="BC81" s="4"/>
-      <c r="BD81" s="59"/>
+      <c r="BD81" s="48"/>
       <c r="BE81" s="4"/>
       <c r="BF81" s="4"/>
       <c r="BG81" s="4"/>
@@ -6313,23 +6315,23 @@
       <c r="AK82" s="4"/>
       <c r="AL82" s="4"/>
       <c r="AM82" s="4"/>
-      <c r="AN82" s="59"/>
-      <c r="AO82" s="59"/>
-      <c r="AP82" s="59"/>
-      <c r="AQ82" s="59"/>
-      <c r="AR82" s="59"/>
-      <c r="AS82" s="59"/>
-      <c r="AT82" s="59"/>
-      <c r="AU82" s="59"/>
-      <c r="AV82" s="59"/>
-      <c r="AW82" s="59"/>
-      <c r="AX82" s="59"/>
-      <c r="AY82" s="59"/>
-      <c r="AZ82" s="59"/>
+      <c r="AN82" s="48"/>
+      <c r="AO82" s="48"/>
+      <c r="AP82" s="48"/>
+      <c r="AQ82" s="48"/>
+      <c r="AR82" s="48"/>
+      <c r="AS82" s="48"/>
+      <c r="AT82" s="48"/>
+      <c r="AU82" s="48"/>
+      <c r="AV82" s="48"/>
+      <c r="AW82" s="48"/>
+      <c r="AX82" s="48"/>
+      <c r="AY82" s="48"/>
+      <c r="AZ82" s="48"/>
       <c r="BA82" s="4"/>
       <c r="BB82" s="4"/>
       <c r="BC82" s="4"/>
-      <c r="BD82" s="59"/>
+      <c r="BD82" s="48"/>
       <c r="BE82" s="4"/>
       <c r="BF82" s="4"/>
       <c r="BG82" s="4"/>
@@ -6376,23 +6378,23 @@
       <c r="AK83" s="4"/>
       <c r="AL83" s="4"/>
       <c r="AM83" s="4"/>
-      <c r="AN83" s="59"/>
-      <c r="AO83" s="59"/>
-      <c r="AP83" s="59"/>
-      <c r="AQ83" s="59"/>
-      <c r="AR83" s="59"/>
-      <c r="AS83" s="59"/>
-      <c r="AT83" s="59"/>
-      <c r="AU83" s="59"/>
-      <c r="AV83" s="59"/>
-      <c r="AW83" s="59"/>
-      <c r="AX83" s="59"/>
-      <c r="AY83" s="59"/>
-      <c r="AZ83" s="59"/>
+      <c r="AN83" s="48"/>
+      <c r="AO83" s="48"/>
+      <c r="AP83" s="48"/>
+      <c r="AQ83" s="48"/>
+      <c r="AR83" s="48"/>
+      <c r="AS83" s="48"/>
+      <c r="AT83" s="48"/>
+      <c r="AU83" s="48"/>
+      <c r="AV83" s="48"/>
+      <c r="AW83" s="48"/>
+      <c r="AX83" s="48"/>
+      <c r="AY83" s="48"/>
+      <c r="AZ83" s="48"/>
       <c r="BA83" s="4"/>
       <c r="BB83" s="4"/>
       <c r="BC83" s="4"/>
-      <c r="BD83" s="59"/>
+      <c r="BD83" s="48"/>
       <c r="BE83" s="4"/>
       <c r="BF83" s="4"/>
       <c r="BG83" s="4"/>
@@ -6439,23 +6441,23 @@
       <c r="AK84" s="4"/>
       <c r="AL84" s="4"/>
       <c r="AM84" s="4"/>
-      <c r="AN84" s="59"/>
-      <c r="AO84" s="59"/>
-      <c r="AP84" s="59"/>
-      <c r="AQ84" s="59"/>
-      <c r="AR84" s="59"/>
-      <c r="AS84" s="59"/>
-      <c r="AT84" s="59"/>
-      <c r="AU84" s="59"/>
-      <c r="AV84" s="59"/>
-      <c r="AW84" s="59"/>
-      <c r="AX84" s="59"/>
-      <c r="AY84" s="59"/>
-      <c r="AZ84" s="59"/>
+      <c r="AN84" s="48"/>
+      <c r="AO84" s="48"/>
+      <c r="AP84" s="48"/>
+      <c r="AQ84" s="48"/>
+      <c r="AR84" s="48"/>
+      <c r="AS84" s="48"/>
+      <c r="AT84" s="48"/>
+      <c r="AU84" s="48"/>
+      <c r="AV84" s="48"/>
+      <c r="AW84" s="48"/>
+      <c r="AX84" s="48"/>
+      <c r="AY84" s="48"/>
+      <c r="AZ84" s="48"/>
       <c r="BA84" s="4"/>
       <c r="BB84" s="4"/>
       <c r="BC84" s="4"/>
-      <c r="BD84" s="59"/>
+      <c r="BD84" s="48"/>
       <c r="BE84" s="4"/>
       <c r="BF84" s="4"/>
       <c r="BG84" s="4"/>
@@ -6500,23 +6502,23 @@
       <c r="AK85" s="4"/>
       <c r="AL85" s="4"/>
       <c r="AM85" s="4"/>
-      <c r="AN85" s="59"/>
-      <c r="AO85" s="59"/>
-      <c r="AP85" s="59"/>
-      <c r="AQ85" s="59"/>
-      <c r="AR85" s="59"/>
-      <c r="AS85" s="59"/>
-      <c r="AT85" s="59"/>
-      <c r="AU85" s="59"/>
-      <c r="AV85" s="59"/>
-      <c r="AW85" s="59"/>
-      <c r="AX85" s="59"/>
-      <c r="AY85" s="59"/>
-      <c r="AZ85" s="59"/>
+      <c r="AN85" s="48"/>
+      <c r="AO85" s="48"/>
+      <c r="AP85" s="48"/>
+      <c r="AQ85" s="48"/>
+      <c r="AR85" s="48"/>
+      <c r="AS85" s="48"/>
+      <c r="AT85" s="48"/>
+      <c r="AU85" s="48"/>
+      <c r="AV85" s="48"/>
+      <c r="AW85" s="48"/>
+      <c r="AX85" s="48"/>
+      <c r="AY85" s="48"/>
+      <c r="AZ85" s="48"/>
       <c r="BA85" s="4"/>
       <c r="BB85" s="4"/>
       <c r="BC85" s="4"/>
-      <c r="BD85" s="59"/>
+      <c r="BD85" s="48"/>
       <c r="BE85" s="4"/>
       <c r="BF85" s="4"/>
       <c r="BG85" s="4"/>
@@ -6561,23 +6563,23 @@
       <c r="AK86" s="4"/>
       <c r="AL86" s="4"/>
       <c r="AM86" s="4"/>
-      <c r="AN86" s="59"/>
-      <c r="AO86" s="59"/>
-      <c r="AP86" s="59"/>
-      <c r="AQ86" s="59"/>
-      <c r="AR86" s="59"/>
-      <c r="AS86" s="59"/>
-      <c r="AT86" s="59"/>
-      <c r="AU86" s="59"/>
-      <c r="AV86" s="59"/>
-      <c r="AW86" s="59"/>
-      <c r="AX86" s="59"/>
-      <c r="AY86" s="59"/>
-      <c r="AZ86" s="59"/>
+      <c r="AN86" s="48"/>
+      <c r="AO86" s="48"/>
+      <c r="AP86" s="48"/>
+      <c r="AQ86" s="48"/>
+      <c r="AR86" s="48"/>
+      <c r="AS86" s="48"/>
+      <c r="AT86" s="48"/>
+      <c r="AU86" s="48"/>
+      <c r="AV86" s="48"/>
+      <c r="AW86" s="48"/>
+      <c r="AX86" s="48"/>
+      <c r="AY86" s="48"/>
+      <c r="AZ86" s="48"/>
       <c r="BA86" s="4"/>
       <c r="BB86" s="4"/>
       <c r="BC86" s="4"/>
-      <c r="BD86" s="59"/>
+      <c r="BD86" s="48"/>
       <c r="BE86" s="4"/>
       <c r="BF86" s="4"/>
       <c r="BG86" s="4"/>
@@ -6626,23 +6628,23 @@
       <c r="AK87" s="4"/>
       <c r="AL87" s="4"/>
       <c r="AM87" s="4"/>
-      <c r="AN87" s="59"/>
-      <c r="AO87" s="59"/>
-      <c r="AP87" s="59"/>
-      <c r="AQ87" s="59"/>
-      <c r="AR87" s="59"/>
-      <c r="AS87" s="59"/>
-      <c r="AT87" s="59"/>
-      <c r="AU87" s="59"/>
-      <c r="AV87" s="59"/>
-      <c r="AW87" s="59"/>
-      <c r="AX87" s="59"/>
-      <c r="AY87" s="59"/>
-      <c r="AZ87" s="59"/>
+      <c r="AN87" s="48"/>
+      <c r="AO87" s="48"/>
+      <c r="AP87" s="48"/>
+      <c r="AQ87" s="48"/>
+      <c r="AR87" s="48"/>
+      <c r="AS87" s="48"/>
+      <c r="AT87" s="48"/>
+      <c r="AU87" s="48"/>
+      <c r="AV87" s="48"/>
+      <c r="AW87" s="48"/>
+      <c r="AX87" s="48"/>
+      <c r="AY87" s="48"/>
+      <c r="AZ87" s="48"/>
       <c r="BA87" s="4"/>
       <c r="BB87" s="4"/>
       <c r="BC87" s="4"/>
-      <c r="BD87" s="59"/>
+      <c r="BD87" s="48"/>
       <c r="BE87" s="4"/>
       <c r="BF87" s="4"/>
       <c r="BG87" s="4"/>
@@ -6689,23 +6691,23 @@
       <c r="AK88" s="4"/>
       <c r="AL88" s="4"/>
       <c r="AM88" s="4"/>
-      <c r="AN88" s="59"/>
-      <c r="AO88" s="59"/>
-      <c r="AP88" s="59"/>
-      <c r="AQ88" s="59"/>
-      <c r="AR88" s="59"/>
-      <c r="AS88" s="59"/>
-      <c r="AT88" s="59"/>
-      <c r="AU88" s="59"/>
-      <c r="AV88" s="59"/>
-      <c r="AW88" s="59"/>
-      <c r="AX88" s="59"/>
-      <c r="AY88" s="59"/>
-      <c r="AZ88" s="59"/>
+      <c r="AN88" s="48"/>
+      <c r="AO88" s="48"/>
+      <c r="AP88" s="48"/>
+      <c r="AQ88" s="48"/>
+      <c r="AR88" s="48"/>
+      <c r="AS88" s="48"/>
+      <c r="AT88" s="48"/>
+      <c r="AU88" s="48"/>
+      <c r="AV88" s="48"/>
+      <c r="AW88" s="48"/>
+      <c r="AX88" s="48"/>
+      <c r="AY88" s="48"/>
+      <c r="AZ88" s="48"/>
       <c r="BA88" s="4"/>
       <c r="BB88" s="4"/>
       <c r="BC88" s="4"/>
-      <c r="BD88" s="59"/>
+      <c r="BD88" s="48"/>
       <c r="BE88" s="4"/>
       <c r="BF88" s="4"/>
       <c r="BG88" s="4"/>
@@ -6819,23 +6821,23 @@
       <c r="AK90" s="4"/>
       <c r="AL90" s="4"/>
       <c r="AM90" s="4"/>
-      <c r="AN90" s="59"/>
-      <c r="AO90" s="59"/>
-      <c r="AP90" s="59"/>
-      <c r="AQ90" s="59"/>
-      <c r="AR90" s="59"/>
-      <c r="AS90" s="59"/>
-      <c r="AT90" s="59"/>
-      <c r="AU90" s="59"/>
-      <c r="AV90" s="59"/>
-      <c r="AW90" s="59"/>
-      <c r="AX90" s="59"/>
-      <c r="AY90" s="59"/>
-      <c r="AZ90" s="59"/>
+      <c r="AN90" s="48"/>
+      <c r="AO90" s="48"/>
+      <c r="AP90" s="48"/>
+      <c r="AQ90" s="48"/>
+      <c r="AR90" s="48"/>
+      <c r="AS90" s="48"/>
+      <c r="AT90" s="48"/>
+      <c r="AU90" s="48"/>
+      <c r="AV90" s="48"/>
+      <c r="AW90" s="48"/>
+      <c r="AX90" s="48"/>
+      <c r="AY90" s="48"/>
+      <c r="AZ90" s="48"/>
       <c r="BA90" s="4"/>
       <c r="BB90" s="4"/>
       <c r="BC90" s="4"/>
-      <c r="BD90" s="59"/>
+      <c r="BD90" s="48"/>
       <c r="BE90" s="4"/>
       <c r="BF90" s="4"/>
       <c r="BG90" s="4"/>
@@ -6882,23 +6884,23 @@
       <c r="AK91" s="4"/>
       <c r="AL91" s="4"/>
       <c r="AM91" s="4"/>
-      <c r="AN91" s="59"/>
-      <c r="AO91" s="59"/>
-      <c r="AP91" s="59"/>
-      <c r="AQ91" s="59"/>
-      <c r="AR91" s="59"/>
-      <c r="AS91" s="59"/>
-      <c r="AT91" s="59"/>
-      <c r="AU91" s="59"/>
-      <c r="AV91" s="59"/>
-      <c r="AW91" s="59"/>
-      <c r="AX91" s="59"/>
-      <c r="AY91" s="59"/>
-      <c r="AZ91" s="59"/>
+      <c r="AN91" s="48"/>
+      <c r="AO91" s="48"/>
+      <c r="AP91" s="48"/>
+      <c r="AQ91" s="48"/>
+      <c r="AR91" s="48"/>
+      <c r="AS91" s="48"/>
+      <c r="AT91" s="48"/>
+      <c r="AU91" s="48"/>
+      <c r="AV91" s="48"/>
+      <c r="AW91" s="48"/>
+      <c r="AX91" s="48"/>
+      <c r="AY91" s="48"/>
+      <c r="AZ91" s="48"/>
       <c r="BA91" s="4"/>
       <c r="BB91" s="4"/>
       <c r="BC91" s="4"/>
-      <c r="BD91" s="59"/>
+      <c r="BD91" s="48"/>
       <c r="BE91" s="4"/>
       <c r="BF91" s="4"/>
       <c r="BG91" s="4"/>
@@ -6945,23 +6947,23 @@
       <c r="AK92" s="4"/>
       <c r="AL92" s="4"/>
       <c r="AM92" s="4"/>
-      <c r="AN92" s="59"/>
-      <c r="AO92" s="59"/>
-      <c r="AP92" s="59"/>
-      <c r="AQ92" s="59"/>
-      <c r="AR92" s="59"/>
-      <c r="AS92" s="59"/>
-      <c r="AT92" s="59"/>
-      <c r="AU92" s="59"/>
-      <c r="AV92" s="59"/>
-      <c r="AW92" s="59"/>
-      <c r="AX92" s="59"/>
-      <c r="AY92" s="59"/>
-      <c r="AZ92" s="59"/>
+      <c r="AN92" s="48"/>
+      <c r="AO92" s="48"/>
+      <c r="AP92" s="48"/>
+      <c r="AQ92" s="48"/>
+      <c r="AR92" s="48"/>
+      <c r="AS92" s="48"/>
+      <c r="AT92" s="48"/>
+      <c r="AU92" s="48"/>
+      <c r="AV92" s="48"/>
+      <c r="AW92" s="48"/>
+      <c r="AX92" s="48"/>
+      <c r="AY92" s="48"/>
+      <c r="AZ92" s="48"/>
       <c r="BA92" s="4"/>
       <c r="BB92" s="4"/>
       <c r="BC92" s="4"/>
-      <c r="BD92" s="59"/>
+      <c r="BD92" s="48"/>
       <c r="BE92" s="4"/>
       <c r="BF92" s="4"/>
       <c r="BG92" s="4"/>
@@ -7005,23 +7007,23 @@
       <c r="AK93" s="4"/>
       <c r="AL93" s="4"/>
       <c r="AM93" s="4"/>
-      <c r="AN93" s="59"/>
-      <c r="AO93" s="59"/>
-      <c r="AP93" s="59"/>
-      <c r="AQ93" s="59"/>
-      <c r="AR93" s="59"/>
-      <c r="AS93" s="59"/>
-      <c r="AT93" s="59"/>
-      <c r="AU93" s="59"/>
-      <c r="AV93" s="59"/>
-      <c r="AW93" s="59"/>
-      <c r="AX93" s="59"/>
-      <c r="AY93" s="59"/>
-      <c r="AZ93" s="59"/>
+      <c r="AN93" s="48"/>
+      <c r="AO93" s="48"/>
+      <c r="AP93" s="48"/>
+      <c r="AQ93" s="48"/>
+      <c r="AR93" s="48"/>
+      <c r="AS93" s="48"/>
+      <c r="AT93" s="48"/>
+      <c r="AU93" s="48"/>
+      <c r="AV93" s="48"/>
+      <c r="AW93" s="48"/>
+      <c r="AX93" s="48"/>
+      <c r="AY93" s="48"/>
+      <c r="AZ93" s="48"/>
       <c r="BA93" s="4"/>
       <c r="BB93" s="4"/>
       <c r="BC93" s="4"/>
-      <c r="BD93" s="59"/>
+      <c r="BD93" s="48"/>
       <c r="BE93" s="4"/>
       <c r="BF93" s="4"/>
       <c r="BG93" s="4"/>
@@ -7066,23 +7068,23 @@
       <c r="AK94" s="4"/>
       <c r="AL94" s="4"/>
       <c r="AM94" s="4"/>
-      <c r="AN94" s="59"/>
-      <c r="AO94" s="59"/>
-      <c r="AP94" s="59"/>
-      <c r="AQ94" s="59"/>
-      <c r="AR94" s="59"/>
-      <c r="AS94" s="59"/>
-      <c r="AT94" s="59"/>
-      <c r="AU94" s="59"/>
-      <c r="AV94" s="59"/>
-      <c r="AW94" s="59"/>
-      <c r="AX94" s="59"/>
-      <c r="AY94" s="59"/>
-      <c r="AZ94" s="59"/>
+      <c r="AN94" s="48"/>
+      <c r="AO94" s="48"/>
+      <c r="AP94" s="48"/>
+      <c r="AQ94" s="48"/>
+      <c r="AR94" s="48"/>
+      <c r="AS94" s="48"/>
+      <c r="AT94" s="48"/>
+      <c r="AU94" s="48"/>
+      <c r="AV94" s="48"/>
+      <c r="AW94" s="48"/>
+      <c r="AX94" s="48"/>
+      <c r="AY94" s="48"/>
+      <c r="AZ94" s="48"/>
       <c r="BA94" s="4"/>
       <c r="BB94" s="4"/>
       <c r="BC94" s="4"/>
-      <c r="BD94" s="59"/>
+      <c r="BD94" s="48"/>
       <c r="BE94" s="4"/>
       <c r="BF94" s="4"/>
       <c r="BG94" s="4"/>
@@ -7131,23 +7133,23 @@
       <c r="AK95" s="4"/>
       <c r="AL95" s="4"/>
       <c r="AM95" s="4"/>
-      <c r="AN95" s="59"/>
-      <c r="AO95" s="59"/>
-      <c r="AP95" s="59"/>
-      <c r="AQ95" s="59"/>
-      <c r="AR95" s="59"/>
-      <c r="AS95" s="59"/>
-      <c r="AT95" s="59"/>
-      <c r="AU95" s="59"/>
-      <c r="AV95" s="59"/>
-      <c r="AW95" s="59"/>
-      <c r="AX95" s="59"/>
-      <c r="AY95" s="59"/>
-      <c r="AZ95" s="59"/>
+      <c r="AN95" s="48"/>
+      <c r="AO95" s="48"/>
+      <c r="AP95" s="48"/>
+      <c r="AQ95" s="48"/>
+      <c r="AR95" s="48"/>
+      <c r="AS95" s="48"/>
+      <c r="AT95" s="48"/>
+      <c r="AU95" s="48"/>
+      <c r="AV95" s="48"/>
+      <c r="AW95" s="48"/>
+      <c r="AX95" s="48"/>
+      <c r="AY95" s="48"/>
+      <c r="AZ95" s="48"/>
       <c r="BA95" s="4"/>
       <c r="BB95" s="4"/>
       <c r="BC95" s="4"/>
-      <c r="BD95" s="59"/>
+      <c r="BD95" s="48"/>
       <c r="BE95" s="4"/>
       <c r="BF95" s="4"/>
       <c r="BG95" s="4"/>
@@ -7192,23 +7194,23 @@
       <c r="AK96" s="4"/>
       <c r="AL96" s="4"/>
       <c r="AM96" s="4"/>
-      <c r="AN96" s="59"/>
-      <c r="AO96" s="59"/>
-      <c r="AP96" s="59"/>
-      <c r="AQ96" s="59"/>
-      <c r="AR96" s="59"/>
-      <c r="AS96" s="59"/>
-      <c r="AT96" s="59"/>
-      <c r="AU96" s="59"/>
-      <c r="AV96" s="59"/>
-      <c r="AW96" s="59"/>
-      <c r="AX96" s="59"/>
-      <c r="AY96" s="59"/>
-      <c r="AZ96" s="59"/>
+      <c r="AN96" s="48"/>
+      <c r="AO96" s="48"/>
+      <c r="AP96" s="48"/>
+      <c r="AQ96" s="48"/>
+      <c r="AR96" s="48"/>
+      <c r="AS96" s="48"/>
+      <c r="AT96" s="48"/>
+      <c r="AU96" s="48"/>
+      <c r="AV96" s="48"/>
+      <c r="AW96" s="48"/>
+      <c r="AX96" s="48"/>
+      <c r="AY96" s="48"/>
+      <c r="AZ96" s="48"/>
       <c r="BA96" s="4"/>
       <c r="BB96" s="4"/>
       <c r="BC96" s="4"/>
-      <c r="BD96" s="59"/>
+      <c r="BD96" s="48"/>
       <c r="BE96" s="4"/>
       <c r="BF96" s="4"/>
       <c r="BG96" s="4"/>
@@ -7253,23 +7255,23 @@
       <c r="AK97" s="4"/>
       <c r="AL97" s="4"/>
       <c r="AM97" s="4"/>
-      <c r="AN97" s="59"/>
-      <c r="AO97" s="59"/>
-      <c r="AP97" s="59"/>
-      <c r="AQ97" s="59"/>
-      <c r="AR97" s="59"/>
-      <c r="AS97" s="59"/>
-      <c r="AT97" s="59"/>
-      <c r="AU97" s="59"/>
-      <c r="AV97" s="59"/>
-      <c r="AW97" s="59"/>
-      <c r="AX97" s="59"/>
-      <c r="AY97" s="59"/>
-      <c r="AZ97" s="59"/>
+      <c r="AN97" s="48"/>
+      <c r="AO97" s="48"/>
+      <c r="AP97" s="48"/>
+      <c r="AQ97" s="48"/>
+      <c r="AR97" s="48"/>
+      <c r="AS97" s="48"/>
+      <c r="AT97" s="48"/>
+      <c r="AU97" s="48"/>
+      <c r="AV97" s="48"/>
+      <c r="AW97" s="48"/>
+      <c r="AX97" s="48"/>
+      <c r="AY97" s="48"/>
+      <c r="AZ97" s="48"/>
       <c r="BA97" s="4"/>
       <c r="BB97" s="4"/>
       <c r="BC97" s="4"/>
-      <c r="BD97" s="59"/>
+      <c r="BD97" s="48"/>
       <c r="BE97" s="4"/>
       <c r="BF97" s="4"/>
       <c r="BG97" s="4"/>
@@ -7318,23 +7320,23 @@
       <c r="AK98" s="4"/>
       <c r="AL98" s="4"/>
       <c r="AM98" s="4"/>
-      <c r="AN98" s="59"/>
-      <c r="AO98" s="59"/>
-      <c r="AP98" s="59"/>
-      <c r="AQ98" s="59"/>
-      <c r="AR98" s="59"/>
-      <c r="AS98" s="59"/>
-      <c r="AT98" s="59"/>
-      <c r="AU98" s="59"/>
-      <c r="AV98" s="59"/>
-      <c r="AW98" s="59"/>
-      <c r="AX98" s="59"/>
-      <c r="AY98" s="59"/>
-      <c r="AZ98" s="59"/>
+      <c r="AN98" s="48"/>
+      <c r="AO98" s="48"/>
+      <c r="AP98" s="48"/>
+      <c r="AQ98" s="48"/>
+      <c r="AR98" s="48"/>
+      <c r="AS98" s="48"/>
+      <c r="AT98" s="48"/>
+      <c r="AU98" s="48"/>
+      <c r="AV98" s="48"/>
+      <c r="AW98" s="48"/>
+      <c r="AX98" s="48"/>
+      <c r="AY98" s="48"/>
+      <c r="AZ98" s="48"/>
       <c r="BA98" s="4"/>
       <c r="BB98" s="4"/>
       <c r="BC98" s="4"/>
-      <c r="BD98" s="59"/>
+      <c r="BD98" s="48"/>
       <c r="BE98" s="4"/>
       <c r="BF98" s="4"/>
       <c r="BG98" s="4"/>
@@ -7379,23 +7381,23 @@
       <c r="AK99" s="4"/>
       <c r="AL99" s="4"/>
       <c r="AM99" s="4"/>
-      <c r="AN99" s="59"/>
-      <c r="AO99" s="59"/>
-      <c r="AP99" s="59"/>
-      <c r="AQ99" s="59"/>
-      <c r="AR99" s="59"/>
-      <c r="AS99" s="59"/>
-      <c r="AT99" s="59"/>
-      <c r="AU99" s="59"/>
-      <c r="AV99" s="59"/>
-      <c r="AW99" s="59"/>
-      <c r="AX99" s="59"/>
-      <c r="AY99" s="59"/>
-      <c r="AZ99" s="59"/>
+      <c r="AN99" s="48"/>
+      <c r="AO99" s="48"/>
+      <c r="AP99" s="48"/>
+      <c r="AQ99" s="48"/>
+      <c r="AR99" s="48"/>
+      <c r="AS99" s="48"/>
+      <c r="AT99" s="48"/>
+      <c r="AU99" s="48"/>
+      <c r="AV99" s="48"/>
+      <c r="AW99" s="48"/>
+      <c r="AX99" s="48"/>
+      <c r="AY99" s="48"/>
+      <c r="AZ99" s="48"/>
       <c r="BA99" s="4"/>
       <c r="BB99" s="4"/>
       <c r="BC99" s="4"/>
-      <c r="BD99" s="59"/>
+      <c r="BD99" s="48"/>
       <c r="BE99" s="4"/>
       <c r="BF99" s="4"/>
       <c r="BG99" s="4"/>
@@ -7440,23 +7442,23 @@
       <c r="AK100" s="4"/>
       <c r="AL100" s="4"/>
       <c r="AM100" s="4"/>
-      <c r="AN100" s="59"/>
-      <c r="AO100" s="59"/>
-      <c r="AP100" s="59"/>
-      <c r="AQ100" s="59"/>
-      <c r="AR100" s="59"/>
-      <c r="AS100" s="59"/>
-      <c r="AT100" s="59"/>
-      <c r="AU100" s="59"/>
-      <c r="AV100" s="59"/>
-      <c r="AW100" s="59"/>
-      <c r="AX100" s="59"/>
-      <c r="AY100" s="59"/>
-      <c r="AZ100" s="59"/>
+      <c r="AN100" s="48"/>
+      <c r="AO100" s="48"/>
+      <c r="AP100" s="48"/>
+      <c r="AQ100" s="48"/>
+      <c r="AR100" s="48"/>
+      <c r="AS100" s="48"/>
+      <c r="AT100" s="48"/>
+      <c r="AU100" s="48"/>
+      <c r="AV100" s="48"/>
+      <c r="AW100" s="48"/>
+      <c r="AX100" s="48"/>
+      <c r="AY100" s="48"/>
+      <c r="AZ100" s="48"/>
       <c r="BA100" s="4"/>
       <c r="BB100" s="4"/>
       <c r="BC100" s="4"/>
-      <c r="BD100" s="59"/>
+      <c r="BD100" s="48"/>
       <c r="BE100" s="4"/>
       <c r="BF100" s="4"/>
       <c r="BG100" s="4"/>
@@ -7501,23 +7503,23 @@
       <c r="AK101" s="4"/>
       <c r="AL101" s="4"/>
       <c r="AM101" s="4"/>
-      <c r="AN101" s="59"/>
-      <c r="AO101" s="59"/>
-      <c r="AP101" s="59"/>
-      <c r="AQ101" s="59"/>
-      <c r="AR101" s="59"/>
-      <c r="AS101" s="59"/>
-      <c r="AT101" s="59"/>
-      <c r="AU101" s="59"/>
-      <c r="AV101" s="59"/>
-      <c r="AW101" s="59"/>
-      <c r="AX101" s="59"/>
-      <c r="AY101" s="59"/>
-      <c r="AZ101" s="59"/>
+      <c r="AN101" s="48"/>
+      <c r="AO101" s="48"/>
+      <c r="AP101" s="48"/>
+      <c r="AQ101" s="48"/>
+      <c r="AR101" s="48"/>
+      <c r="AS101" s="48"/>
+      <c r="AT101" s="48"/>
+      <c r="AU101" s="48"/>
+      <c r="AV101" s="48"/>
+      <c r="AW101" s="48"/>
+      <c r="AX101" s="48"/>
+      <c r="AY101" s="48"/>
+      <c r="AZ101" s="48"/>
       <c r="BA101" s="4"/>
       <c r="BB101" s="4"/>
       <c r="BC101" s="4"/>
-      <c r="BD101" s="59"/>
+      <c r="BD101" s="48"/>
       <c r="BE101" s="4"/>
       <c r="BF101" s="4"/>
       <c r="BG101" s="4"/>
@@ -7566,23 +7568,23 @@
       <c r="AK102" s="18"/>
       <c r="AL102" s="18"/>
       <c r="AM102" s="18"/>
-      <c r="AN102" s="59"/>
-      <c r="AO102" s="59"/>
-      <c r="AP102" s="59"/>
-      <c r="AQ102" s="59"/>
-      <c r="AR102" s="59"/>
-      <c r="AS102" s="59"/>
-      <c r="AT102" s="59"/>
-      <c r="AU102" s="59"/>
-      <c r="AV102" s="59"/>
-      <c r="AW102" s="59"/>
-      <c r="AX102" s="59"/>
-      <c r="AY102" s="59"/>
-      <c r="AZ102" s="59"/>
+      <c r="AN102" s="48"/>
+      <c r="AO102" s="48"/>
+      <c r="AP102" s="48"/>
+      <c r="AQ102" s="48"/>
+      <c r="AR102" s="48"/>
+      <c r="AS102" s="48"/>
+      <c r="AT102" s="48"/>
+      <c r="AU102" s="48"/>
+      <c r="AV102" s="48"/>
+      <c r="AW102" s="48"/>
+      <c r="AX102" s="48"/>
+      <c r="AY102" s="48"/>
+      <c r="AZ102" s="48"/>
       <c r="BA102" s="4"/>
       <c r="BB102" s="4"/>
       <c r="BC102" s="4"/>
-      <c r="BD102" s="59"/>
+      <c r="BD102" s="48"/>
       <c r="BE102" s="4"/>
       <c r="BF102" s="4"/>
       <c r="BG102" s="4"/>
@@ -7629,30 +7631,30 @@
       <c r="AK103" s="4"/>
       <c r="AL103" s="18"/>
       <c r="AM103" s="18"/>
-      <c r="AN103" s="59"/>
-      <c r="AO103" s="59"/>
-      <c r="AP103" s="59"/>
-      <c r="AQ103" s="59"/>
-      <c r="AR103" s="59"/>
-      <c r="AS103" s="59"/>
-      <c r="AT103" s="59"/>
-      <c r="AU103" s="59"/>
-      <c r="AV103" s="59"/>
-      <c r="AW103" s="59"/>
-      <c r="AX103" s="59"/>
-      <c r="AY103" s="59"/>
-      <c r="AZ103" s="59"/>
+      <c r="AN103" s="48"/>
+      <c r="AO103" s="48"/>
+      <c r="AP103" s="48"/>
+      <c r="AQ103" s="48"/>
+      <c r="AR103" s="48"/>
+      <c r="AS103" s="48"/>
+      <c r="AT103" s="48"/>
+      <c r="AU103" s="48"/>
+      <c r="AV103" s="48"/>
+      <c r="AW103" s="48"/>
+      <c r="AX103" s="48"/>
+      <c r="AY103" s="48"/>
+      <c r="AZ103" s="48"/>
       <c r="BA103" s="4"/>
       <c r="BB103" s="4"/>
       <c r="BC103" s="4"/>
-      <c r="BD103" s="59"/>
+      <c r="BD103" s="48"/>
       <c r="BE103" s="4"/>
       <c r="BF103" s="4"/>
       <c r="BG103" s="4"/>
     </row>
     <row r="104" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>66</v>
@@ -7762,20 +7764,20 @@
       <c r="AN105" s="18"/>
       <c r="AO105" s="18"/>
       <c r="AP105" s="18"/>
-      <c r="AQ105" s="59"/>
-      <c r="AR105" s="59"/>
-      <c r="AS105" s="59"/>
-      <c r="AT105" s="59"/>
-      <c r="AU105" s="59"/>
-      <c r="AV105" s="59"/>
-      <c r="AW105" s="59"/>
-      <c r="AX105" s="59"/>
-      <c r="AY105" s="59"/>
-      <c r="AZ105" s="59"/>
+      <c r="AQ105" s="48"/>
+      <c r="AR105" s="48"/>
+      <c r="AS105" s="48"/>
+      <c r="AT105" s="48"/>
+      <c r="AU105" s="48"/>
+      <c r="AV105" s="48"/>
+      <c r="AW105" s="48"/>
+      <c r="AX105" s="48"/>
+      <c r="AY105" s="48"/>
+      <c r="AZ105" s="48"/>
       <c r="BA105" s="4"/>
       <c r="BB105" s="4"/>
       <c r="BC105" s="4"/>
-      <c r="BD105" s="59"/>
+      <c r="BD105" s="48"/>
       <c r="BE105" s="4"/>
       <c r="BF105" s="4"/>
       <c r="BG105" s="4"/>
@@ -7820,23 +7822,23 @@
       <c r="AK106" s="4"/>
       <c r="AL106" s="4"/>
       <c r="AM106" s="4"/>
-      <c r="AN106" s="59"/>
-      <c r="AO106" s="59"/>
-      <c r="AP106" s="59"/>
-      <c r="AQ106" s="59"/>
-      <c r="AR106" s="59"/>
-      <c r="AS106" s="59"/>
-      <c r="AT106" s="59"/>
-      <c r="AU106" s="59"/>
-      <c r="AV106" s="59"/>
-      <c r="AW106" s="59"/>
-      <c r="AX106" s="59"/>
-      <c r="AY106" s="59"/>
-      <c r="AZ106" s="59"/>
+      <c r="AN106" s="48"/>
+      <c r="AO106" s="48"/>
+      <c r="AP106" s="48"/>
+      <c r="AQ106" s="48"/>
+      <c r="AR106" s="48"/>
+      <c r="AS106" s="48"/>
+      <c r="AT106" s="48"/>
+      <c r="AU106" s="48"/>
+      <c r="AV106" s="48"/>
+      <c r="AW106" s="48"/>
+      <c r="AX106" s="48"/>
+      <c r="AY106" s="48"/>
+      <c r="AZ106" s="48"/>
       <c r="BA106" s="4"/>
       <c r="BB106" s="4"/>
       <c r="BC106" s="4"/>
-      <c r="BD106" s="59"/>
+      <c r="BD106" s="48"/>
       <c r="BE106" s="4"/>
       <c r="BF106" s="4"/>
       <c r="BG106" s="4"/>
@@ -7881,23 +7883,23 @@
       <c r="AK107" s="4"/>
       <c r="AL107" s="4"/>
       <c r="AM107" s="4"/>
-      <c r="AN107" s="59"/>
-      <c r="AO107" s="59"/>
-      <c r="AP107" s="59"/>
-      <c r="AQ107" s="59"/>
-      <c r="AR107" s="59"/>
-      <c r="AS107" s="59"/>
-      <c r="AT107" s="59"/>
-      <c r="AU107" s="59"/>
-      <c r="AV107" s="59"/>
-      <c r="AW107" s="59"/>
-      <c r="AX107" s="59"/>
-      <c r="AY107" s="59"/>
-      <c r="AZ107" s="59"/>
+      <c r="AN107" s="48"/>
+      <c r="AO107" s="48"/>
+      <c r="AP107" s="48"/>
+      <c r="AQ107" s="48"/>
+      <c r="AR107" s="48"/>
+      <c r="AS107" s="48"/>
+      <c r="AT107" s="48"/>
+      <c r="AU107" s="48"/>
+      <c r="AV107" s="48"/>
+      <c r="AW107" s="48"/>
+      <c r="AX107" s="48"/>
+      <c r="AY107" s="48"/>
+      <c r="AZ107" s="48"/>
       <c r="BA107" s="4"/>
       <c r="BB107" s="4"/>
       <c r="BC107" s="4"/>
-      <c r="BD107" s="59"/>
+      <c r="BD107" s="48"/>
       <c r="BE107" s="4"/>
       <c r="BF107" s="4"/>
       <c r="BG107" s="4"/>
@@ -7942,23 +7944,23 @@
       <c r="AK108" s="4"/>
       <c r="AL108" s="4"/>
       <c r="AM108" s="4"/>
-      <c r="AN108" s="59"/>
-      <c r="AO108" s="59"/>
-      <c r="AP108" s="59"/>
-      <c r="AQ108" s="59"/>
-      <c r="AR108" s="59"/>
-      <c r="AS108" s="59"/>
-      <c r="AT108" s="59"/>
-      <c r="AU108" s="59"/>
-      <c r="AV108" s="59"/>
-      <c r="AW108" s="59"/>
-      <c r="AX108" s="59"/>
-      <c r="AY108" s="59"/>
-      <c r="AZ108" s="59"/>
+      <c r="AN108" s="48"/>
+      <c r="AO108" s="48"/>
+      <c r="AP108" s="48"/>
+      <c r="AQ108" s="48"/>
+      <c r="AR108" s="48"/>
+      <c r="AS108" s="48"/>
+      <c r="AT108" s="48"/>
+      <c r="AU108" s="48"/>
+      <c r="AV108" s="48"/>
+      <c r="AW108" s="48"/>
+      <c r="AX108" s="48"/>
+      <c r="AY108" s="48"/>
+      <c r="AZ108" s="48"/>
       <c r="BA108" s="4"/>
       <c r="BB108" s="4"/>
       <c r="BC108" s="4"/>
-      <c r="BD108" s="59"/>
+      <c r="BD108" s="48"/>
       <c r="BE108" s="4"/>
       <c r="BF108" s="4"/>
       <c r="BG108" s="4"/>
@@ -8003,23 +8005,23 @@
       <c r="AK109" s="4"/>
       <c r="AL109" s="4"/>
       <c r="AM109" s="4"/>
-      <c r="AN109" s="59"/>
-      <c r="AO109" s="59"/>
-      <c r="AP109" s="59"/>
-      <c r="AQ109" s="59"/>
-      <c r="AR109" s="59"/>
-      <c r="AS109" s="59"/>
-      <c r="AT109" s="59"/>
-      <c r="AU109" s="59"/>
-      <c r="AV109" s="59"/>
-      <c r="AW109" s="59"/>
-      <c r="AX109" s="59"/>
-      <c r="AY109" s="59"/>
-      <c r="AZ109" s="59"/>
+      <c r="AN109" s="48"/>
+      <c r="AO109" s="48"/>
+      <c r="AP109" s="48"/>
+      <c r="AQ109" s="48"/>
+      <c r="AR109" s="48"/>
+      <c r="AS109" s="48"/>
+      <c r="AT109" s="48"/>
+      <c r="AU109" s="48"/>
+      <c r="AV109" s="48"/>
+      <c r="AW109" s="48"/>
+      <c r="AX109" s="48"/>
+      <c r="AY109" s="48"/>
+      <c r="AZ109" s="48"/>
       <c r="BA109" s="4"/>
       <c r="BB109" s="4"/>
       <c r="BC109" s="4"/>
-      <c r="BD109" s="59"/>
+      <c r="BD109" s="48"/>
       <c r="BE109" s="4"/>
       <c r="BF109" s="4"/>
       <c r="BG109" s="4"/>
@@ -8068,23 +8070,23 @@
       <c r="AK110" s="4"/>
       <c r="AL110" s="4"/>
       <c r="AM110" s="4"/>
-      <c r="AN110" s="59"/>
+      <c r="AN110" s="48"/>
       <c r="AO110" s="18"/>
       <c r="AP110" s="18"/>
-      <c r="AQ110" s="59"/>
-      <c r="AR110" s="59"/>
-      <c r="AS110" s="59"/>
-      <c r="AT110" s="59"/>
-      <c r="AU110" s="59"/>
-      <c r="AV110" s="59"/>
-      <c r="AW110" s="59"/>
-      <c r="AX110" s="59"/>
-      <c r="AY110" s="59"/>
-      <c r="AZ110" s="59"/>
+      <c r="AQ110" s="48"/>
+      <c r="AR110" s="48"/>
+      <c r="AS110" s="48"/>
+      <c r="AT110" s="48"/>
+      <c r="AU110" s="48"/>
+      <c r="AV110" s="48"/>
+      <c r="AW110" s="48"/>
+      <c r="AX110" s="48"/>
+      <c r="AY110" s="48"/>
+      <c r="AZ110" s="48"/>
       <c r="BA110" s="4"/>
       <c r="BB110" s="4"/>
       <c r="BC110" s="4"/>
-      <c r="BD110" s="59"/>
+      <c r="BD110" s="48"/>
       <c r="BE110" s="4"/>
       <c r="BF110" s="4"/>
       <c r="BG110" s="4"/>
@@ -8129,23 +8131,23 @@
       <c r="AK111" s="4"/>
       <c r="AL111" s="4"/>
       <c r="AM111" s="4"/>
-      <c r="AN111" s="59"/>
-      <c r="AO111" s="59"/>
-      <c r="AP111" s="59"/>
-      <c r="AQ111" s="59"/>
-      <c r="AR111" s="59"/>
-      <c r="AS111" s="59"/>
-      <c r="AT111" s="59"/>
-      <c r="AU111" s="59"/>
-      <c r="AV111" s="59"/>
-      <c r="AW111" s="59"/>
-      <c r="AX111" s="59"/>
-      <c r="AY111" s="59"/>
-      <c r="AZ111" s="59"/>
+      <c r="AN111" s="48"/>
+      <c r="AO111" s="48"/>
+      <c r="AP111" s="48"/>
+      <c r="AQ111" s="48"/>
+      <c r="AR111" s="48"/>
+      <c r="AS111" s="48"/>
+      <c r="AT111" s="48"/>
+      <c r="AU111" s="48"/>
+      <c r="AV111" s="48"/>
+      <c r="AW111" s="48"/>
+      <c r="AX111" s="48"/>
+      <c r="AY111" s="48"/>
+      <c r="AZ111" s="48"/>
       <c r="BA111" s="4"/>
       <c r="BB111" s="4"/>
       <c r="BC111" s="4"/>
-      <c r="BD111" s="59"/>
+      <c r="BD111" s="48"/>
       <c r="BE111" s="4"/>
       <c r="BF111" s="4"/>
       <c r="BG111" s="4"/>
@@ -8190,23 +8192,23 @@
       <c r="AK112" s="4"/>
       <c r="AL112" s="4"/>
       <c r="AM112" s="4"/>
-      <c r="AN112" s="59"/>
-      <c r="AO112" s="59"/>
-      <c r="AP112" s="59"/>
-      <c r="AQ112" s="59"/>
-      <c r="AR112" s="59"/>
-      <c r="AS112" s="59"/>
-      <c r="AT112" s="59"/>
-      <c r="AU112" s="59"/>
-      <c r="AV112" s="59"/>
-      <c r="AW112" s="59"/>
-      <c r="AX112" s="59"/>
-      <c r="AY112" s="59"/>
-      <c r="AZ112" s="59"/>
+      <c r="AN112" s="48"/>
+      <c r="AO112" s="48"/>
+      <c r="AP112" s="48"/>
+      <c r="AQ112" s="48"/>
+      <c r="AR112" s="48"/>
+      <c r="AS112" s="48"/>
+      <c r="AT112" s="48"/>
+      <c r="AU112" s="48"/>
+      <c r="AV112" s="48"/>
+      <c r="AW112" s="48"/>
+      <c r="AX112" s="48"/>
+      <c r="AY112" s="48"/>
+      <c r="AZ112" s="48"/>
       <c r="BA112" s="4"/>
       <c r="BB112" s="4"/>
       <c r="BC112" s="4"/>
-      <c r="BD112" s="59"/>
+      <c r="BD112" s="48"/>
       <c r="BE112" s="4"/>
       <c r="BF112" s="4"/>
       <c r="BG112" s="4"/>
@@ -8255,23 +8257,23 @@
       <c r="AK113" s="4"/>
       <c r="AL113" s="4"/>
       <c r="AM113" s="4"/>
-      <c r="AN113" s="59"/>
-      <c r="AO113" s="59"/>
-      <c r="AP113" s="59"/>
+      <c r="AN113" s="48"/>
+      <c r="AO113" s="48"/>
+      <c r="AP113" s="48"/>
       <c r="AQ113" s="18"/>
       <c r="AR113" s="18"/>
       <c r="AS113" s="18"/>
       <c r="AT113" s="18"/>
       <c r="AU113" s="18"/>
       <c r="AV113" s="18"/>
-      <c r="AW113" s="59"/>
-      <c r="AX113" s="59"/>
-      <c r="AY113" s="59"/>
-      <c r="AZ113" s="59"/>
+      <c r="AW113" s="48"/>
+      <c r="AX113" s="48"/>
+      <c r="AY113" s="48"/>
+      <c r="AZ113" s="48"/>
       <c r="BA113" s="4"/>
       <c r="BB113" s="4"/>
       <c r="BC113" s="4"/>
-      <c r="BD113" s="59"/>
+      <c r="BD113" s="48"/>
       <c r="BE113" s="4"/>
       <c r="BF113" s="4"/>
       <c r="BG113" s="4"/>
@@ -8318,15 +8320,15 @@
       <c r="AK114" s="4"/>
       <c r="AL114" s="4"/>
       <c r="AM114" s="4"/>
-      <c r="AN114" s="59"/>
-      <c r="AO114" s="59"/>
-      <c r="AP114" s="59"/>
-      <c r="AQ114" s="59"/>
-      <c r="AR114" s="59"/>
-      <c r="AS114" s="59"/>
-      <c r="AT114" s="59"/>
-      <c r="AU114" s="59"/>
-      <c r="AV114" s="59"/>
+      <c r="AN114" s="48"/>
+      <c r="AO114" s="48"/>
+      <c r="AP114" s="48"/>
+      <c r="AQ114" s="48"/>
+      <c r="AR114" s="48"/>
+      <c r="AS114" s="48"/>
+      <c r="AT114" s="48"/>
+      <c r="AU114" s="48"/>
+      <c r="AV114" s="48"/>
       <c r="AW114" s="18"/>
       <c r="AX114" s="18"/>
       <c r="AY114" s="18"/>
@@ -8334,7 +8336,7 @@
       <c r="BA114" s="4"/>
       <c r="BB114" s="4"/>
       <c r="BC114" s="4"/>
-      <c r="BD114" s="59"/>
+      <c r="BD114" s="48"/>
       <c r="BE114" s="4"/>
       <c r="BF114" s="4"/>
       <c r="BG114" s="4"/>
@@ -8379,23 +8381,23 @@
       <c r="AK115" s="4"/>
       <c r="AL115" s="4"/>
       <c r="AM115" s="4"/>
-      <c r="AN115" s="59"/>
-      <c r="AO115" s="59"/>
-      <c r="AP115" s="59"/>
-      <c r="AQ115" s="59"/>
-      <c r="AR115" s="59"/>
-      <c r="AS115" s="59"/>
-      <c r="AT115" s="59"/>
-      <c r="AU115" s="59"/>
-      <c r="AV115" s="59"/>
-      <c r="AW115" s="59"/>
-      <c r="AX115" s="59"/>
-      <c r="AY115" s="59"/>
-      <c r="AZ115" s="59"/>
+      <c r="AN115" s="48"/>
+      <c r="AO115" s="48"/>
+      <c r="AP115" s="48"/>
+      <c r="AQ115" s="48"/>
+      <c r="AR115" s="48"/>
+      <c r="AS115" s="48"/>
+      <c r="AT115" s="48"/>
+      <c r="AU115" s="48"/>
+      <c r="AV115" s="48"/>
+      <c r="AW115" s="48"/>
+      <c r="AX115" s="48"/>
+      <c r="AY115" s="48"/>
+      <c r="AZ115" s="48"/>
       <c r="BA115" s="4"/>
       <c r="BB115" s="4"/>
       <c r="BC115" s="4"/>
-      <c r="BD115" s="59"/>
+      <c r="BD115" s="48"/>
       <c r="BE115" s="4"/>
       <c r="BF115" s="4"/>
       <c r="BG115" s="4"/>
@@ -8440,23 +8442,23 @@
       <c r="AK116" s="4"/>
       <c r="AL116" s="4"/>
       <c r="AM116" s="4"/>
-      <c r="AN116" s="59"/>
-      <c r="AO116" s="59"/>
-      <c r="AP116" s="59"/>
-      <c r="AQ116" s="59"/>
-      <c r="AR116" s="59"/>
-      <c r="AS116" s="59"/>
-      <c r="AT116" s="59"/>
-      <c r="AU116" s="59"/>
-      <c r="AV116" s="59"/>
-      <c r="AW116" s="59"/>
-      <c r="AX116" s="59"/>
-      <c r="AY116" s="59"/>
-      <c r="AZ116" s="59"/>
+      <c r="AN116" s="48"/>
+      <c r="AO116" s="48"/>
+      <c r="AP116" s="48"/>
+      <c r="AQ116" s="48"/>
+      <c r="AR116" s="48"/>
+      <c r="AS116" s="48"/>
+      <c r="AT116" s="48"/>
+      <c r="AU116" s="48"/>
+      <c r="AV116" s="48"/>
+      <c r="AW116" s="48"/>
+      <c r="AX116" s="48"/>
+      <c r="AY116" s="48"/>
+      <c r="AZ116" s="48"/>
       <c r="BA116" s="4"/>
       <c r="BB116" s="4"/>
       <c r="BC116" s="4"/>
-      <c r="BD116" s="59"/>
+      <c r="BD116" s="48"/>
       <c r="BE116" s="4"/>
       <c r="BF116" s="4"/>
       <c r="BG116" s="4"/>
@@ -8503,23 +8505,23 @@
       <c r="AK117" s="4"/>
       <c r="AL117" s="4"/>
       <c r="AM117" s="4"/>
-      <c r="AN117" s="59"/>
-      <c r="AO117" s="59"/>
-      <c r="AP117" s="59"/>
-      <c r="AQ117" s="59"/>
-      <c r="AR117" s="59"/>
-      <c r="AS117" s="59"/>
-      <c r="AT117" s="59"/>
-      <c r="AU117" s="59"/>
-      <c r="AV117" s="59"/>
-      <c r="AW117" s="59"/>
-      <c r="AX117" s="59"/>
-      <c r="AY117" s="59"/>
-      <c r="AZ117" s="59"/>
+      <c r="AN117" s="48"/>
+      <c r="AO117" s="48"/>
+      <c r="AP117" s="48"/>
+      <c r="AQ117" s="48"/>
+      <c r="AR117" s="48"/>
+      <c r="AS117" s="48"/>
+      <c r="AT117" s="48"/>
+      <c r="AU117" s="48"/>
+      <c r="AV117" s="48"/>
+      <c r="AW117" s="48"/>
+      <c r="AX117" s="48"/>
+      <c r="AY117" s="48"/>
+      <c r="AZ117" s="48"/>
       <c r="BA117" s="4"/>
       <c r="BB117" s="4"/>
       <c r="BC117" s="4"/>
-      <c r="BD117" s="59"/>
+      <c r="BD117" s="48"/>
       <c r="BE117" s="4"/>
       <c r="BF117" s="4"/>
       <c r="BG117" s="4"/>
@@ -8564,23 +8566,23 @@
       <c r="AK118" s="4"/>
       <c r="AL118" s="4"/>
       <c r="AM118" s="4"/>
-      <c r="AN118" s="59"/>
-      <c r="AO118" s="59"/>
-      <c r="AP118" s="59"/>
-      <c r="AQ118" s="59"/>
-      <c r="AR118" s="59"/>
-      <c r="AS118" s="59"/>
-      <c r="AT118" s="59"/>
-      <c r="AU118" s="59"/>
-      <c r="AV118" s="59"/>
-      <c r="AW118" s="59"/>
-      <c r="AX118" s="59"/>
-      <c r="AY118" s="59"/>
-      <c r="AZ118" s="59"/>
+      <c r="AN118" s="48"/>
+      <c r="AO118" s="48"/>
+      <c r="AP118" s="48"/>
+      <c r="AQ118" s="48"/>
+      <c r="AR118" s="48"/>
+      <c r="AS118" s="48"/>
+      <c r="AT118" s="48"/>
+      <c r="AU118" s="48"/>
+      <c r="AV118" s="48"/>
+      <c r="AW118" s="48"/>
+      <c r="AX118" s="48"/>
+      <c r="AY118" s="48"/>
+      <c r="AZ118" s="48"/>
       <c r="BA118" s="4"/>
       <c r="BB118" s="4"/>
       <c r="BC118" s="4"/>
-      <c r="BD118" s="59"/>
+      <c r="BD118" s="48"/>
       <c r="BE118" s="4"/>
       <c r="BF118" s="4"/>
       <c r="BG118" s="4"/>
@@ -8627,23 +8629,23 @@
       <c r="AK119" s="4"/>
       <c r="AL119" s="4"/>
       <c r="AM119" s="4"/>
-      <c r="AN119" s="59"/>
-      <c r="AO119" s="59"/>
-      <c r="AP119" s="59"/>
-      <c r="AQ119" s="59"/>
-      <c r="AR119" s="59"/>
-      <c r="AS119" s="59"/>
-      <c r="AT119" s="59"/>
-      <c r="AU119" s="59"/>
-      <c r="AV119" s="59"/>
-      <c r="AW119" s="59"/>
-      <c r="AX119" s="59"/>
-      <c r="AY119" s="59"/>
-      <c r="AZ119" s="59"/>
+      <c r="AN119" s="48"/>
+      <c r="AO119" s="48"/>
+      <c r="AP119" s="48"/>
+      <c r="AQ119" s="48"/>
+      <c r="AR119" s="48"/>
+      <c r="AS119" s="48"/>
+      <c r="AT119" s="48"/>
+      <c r="AU119" s="48"/>
+      <c r="AV119" s="48"/>
+      <c r="AW119" s="48"/>
+      <c r="AX119" s="48"/>
+      <c r="AY119" s="48"/>
+      <c r="AZ119" s="48"/>
       <c r="BA119" s="4"/>
       <c r="BB119" s="4"/>
       <c r="BC119" s="4"/>
-      <c r="BD119" s="59"/>
+      <c r="BD119" s="48"/>
       <c r="BE119" s="4"/>
       <c r="BF119" s="4"/>
       <c r="BG119" s="4"/>

</xml_diff>

<commit_message>
Fix some conditional and null pointer validation in *RunningController
</commit_message>
<xml_diff>
--- a/planificacion/planificacion.xlsx
+++ b/planificacion/planificacion.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CB51A4-E6CB-4011-AAA9-67D0BF9FF3A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624825EB-56DF-43FE-A971-A058CF2C0917}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version actual" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="74">
   <si>
     <t>Tareas</t>
   </si>
@@ -240,12 +240,21 @@
   <si>
     <t>Iteración 6</t>
   </si>
+  <si>
+    <t>Entrega de documento</t>
+  </si>
+  <si>
+    <t>Defensa:</t>
+  </si>
+  <si>
+    <t>18 de Agosto</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,8 +296,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,6 +333,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,10 +685,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -777,8 +812,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1062,11 +1105,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893B0263-59F4-40E5-9460-E43E9955B4EB}">
-  <dimension ref="A1:BG129"/>
+  <dimension ref="A1:BG130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BA116" sqref="BA116"/>
+      <pane ySplit="2" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G133" sqref="G133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1117,9 @@
     <col min="1" max="1" width="19.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="55.85546875" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" customWidth="1"/>
-    <col min="4" max="54" width="4.5703125" customWidth="1"/>
+    <col min="4" max="50" width="4.5703125" customWidth="1"/>
+    <col min="51" max="51" width="4.5703125" style="72" customWidth="1"/>
+    <col min="52" max="54" width="4.5703125" customWidth="1"/>
     <col min="55" max="55" width="6" customWidth="1"/>
     <col min="56" max="58" width="4.5703125" customWidth="1"/>
     <col min="59" max="59" width="6" customWidth="1"/>
@@ -1316,7 +1361,7 @@
       <c r="AX2" s="15">
         <v>44004</v>
       </c>
-      <c r="AY2" s="15">
+      <c r="AY2" s="70">
         <v>44011</v>
       </c>
       <c r="AZ2" s="15">
@@ -1397,7 +1442,7 @@
       <c r="AV3" s="15"/>
       <c r="AW3" s="15"/>
       <c r="AX3" s="15"/>
-      <c r="AY3" s="15"/>
+      <c r="AY3" s="70"/>
       <c r="AZ3" s="15"/>
       <c r="BA3" s="15"/>
       <c r="BB3" s="15"/>
@@ -1460,7 +1505,7 @@
       <c r="AV4" s="15"/>
       <c r="AW4" s="15"/>
       <c r="AX4" s="15"/>
-      <c r="AY4" s="15"/>
+      <c r="AY4" s="70"/>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
       <c r="BB4" s="15"/>
@@ -1522,7 +1567,7 @@
       <c r="AV5" s="15"/>
       <c r="AW5" s="15"/>
       <c r="AX5" s="15"/>
-      <c r="AY5" s="15"/>
+      <c r="AY5" s="70"/>
       <c r="AZ5" s="15"/>
       <c r="BA5" s="15"/>
       <c r="BB5" s="15"/>
@@ -1585,7 +1630,7 @@
       <c r="AV6" s="15"/>
       <c r="AW6" s="15"/>
       <c r="AX6" s="15"/>
-      <c r="AY6" s="15"/>
+      <c r="AY6" s="70"/>
       <c r="AZ6" s="15"/>
       <c r="BA6" s="15"/>
       <c r="BB6" s="15"/>
@@ -1648,7 +1693,7 @@
       <c r="AV7" s="15"/>
       <c r="AW7" s="15"/>
       <c r="AX7" s="15"/>
-      <c r="AY7" s="15"/>
+      <c r="AY7" s="70"/>
       <c r="AZ7" s="15"/>
       <c r="BA7" s="15"/>
       <c r="BB7" s="15"/>
@@ -1711,7 +1756,7 @@
       <c r="AV8" s="15"/>
       <c r="AW8" s="15"/>
       <c r="AX8" s="15"/>
-      <c r="AY8" s="15"/>
+      <c r="AY8" s="70"/>
       <c r="AZ8" s="15"/>
       <c r="BA8" s="15"/>
       <c r="BB8" s="15"/>
@@ -1773,7 +1818,7 @@
       <c r="AV9" s="15"/>
       <c r="AW9" s="15"/>
       <c r="AX9" s="15"/>
-      <c r="AY9" s="15"/>
+      <c r="AY9" s="70"/>
       <c r="AZ9" s="15"/>
       <c r="BA9" s="15"/>
       <c r="BB9" s="15"/>
@@ -1836,7 +1881,7 @@
       <c r="AV10" s="15"/>
       <c r="AW10" s="15"/>
       <c r="AX10" s="15"/>
-      <c r="AY10" s="15"/>
+      <c r="AY10" s="70"/>
       <c r="AZ10" s="15"/>
       <c r="BA10" s="15"/>
       <c r="BB10" s="15"/>
@@ -1847,139 +1892,139 @@
       <c r="BG10" s="15"/>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="39"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10"/>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="10"/>
+      <c r="AE11" s="10"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="31"/>
+      <c r="AH11" s="25"/>
+      <c r="AI11" s="15"/>
+      <c r="AJ11" s="15"/>
+      <c r="AK11" s="15"/>
+      <c r="AL11" s="15"/>
+      <c r="AM11" s="15"/>
+      <c r="AN11" s="15"/>
+      <c r="AO11" s="15"/>
+      <c r="AP11" s="15"/>
+      <c r="AQ11" s="15"/>
+      <c r="AR11" s="15"/>
+      <c r="AS11" s="15"/>
+      <c r="AT11" s="15"/>
+      <c r="AU11" s="15"/>
+      <c r="AV11" s="15"/>
+      <c r="AW11" s="15"/>
+      <c r="AX11" s="15"/>
+      <c r="AY11" s="70"/>
+      <c r="AZ11" s="15"/>
+      <c r="BA11" s="15"/>
+      <c r="BB11" s="17"/>
+      <c r="BC11" s="17"/>
+      <c r="BD11" s="15"/>
+      <c r="BE11" s="15"/>
+      <c r="BF11" s="15"/>
+      <c r="BG11" s="15"/>
+    </row>
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
-      <c r="T11" s="22"/>
-      <c r="U11" s="22"/>
-      <c r="V11" s="22"/>
-      <c r="W11" s="24"/>
-      <c r="X11" s="32"/>
-      <c r="Y11" s="22"/>
-      <c r="Z11" s="22"/>
-      <c r="AA11" s="22"/>
-      <c r="AB11" s="22"/>
-      <c r="AC11" s="22"/>
-      <c r="AD11" s="22"/>
-      <c r="AE11" s="22"/>
-      <c r="AF11" s="22"/>
-      <c r="AG11" s="33"/>
-      <c r="AH11" s="26"/>
-      <c r="AI11" s="22"/>
-      <c r="AJ11" s="5"/>
-      <c r="AK11" s="5"/>
-      <c r="AL11" s="5"/>
-      <c r="AM11" s="5"/>
-      <c r="AN11" s="5"/>
-      <c r="AO11" s="5"/>
-      <c r="AP11" s="5"/>
-      <c r="AQ11" s="5"/>
-      <c r="AR11" s="5"/>
-      <c r="AS11" s="5"/>
-      <c r="AT11" s="5"/>
-      <c r="AU11" s="5"/>
-      <c r="AV11" s="5"/>
-      <c r="AW11" s="5"/>
-      <c r="AX11" s="5"/>
-      <c r="AY11" s="5"/>
-      <c r="AZ11" s="5"/>
-      <c r="BA11" s="5"/>
-      <c r="BB11" s="5"/>
-      <c r="BC11" s="5"/>
-      <c r="BD11" s="5"/>
-      <c r="BE11" s="5"/>
-      <c r="BF11" s="5"/>
-      <c r="BG11" s="5"/>
-    </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="22"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="22"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="22"/>
+      <c r="Z12" s="22"/>
+      <c r="AA12" s="22"/>
+      <c r="AB12" s="22"/>
+      <c r="AC12" s="22"/>
+      <c r="AD12" s="22"/>
+      <c r="AE12" s="22"/>
+      <c r="AF12" s="22"/>
+      <c r="AG12" s="33"/>
+      <c r="AH12" s="26"/>
+      <c r="AI12" s="22"/>
+      <c r="AJ12" s="5"/>
+      <c r="AK12" s="5"/>
+      <c r="AL12" s="5"/>
+      <c r="AM12" s="5"/>
+      <c r="AN12" s="5"/>
+      <c r="AO12" s="5"/>
+      <c r="AP12" s="5"/>
+      <c r="AQ12" s="5"/>
+      <c r="AR12" s="5"/>
+      <c r="AS12" s="5"/>
+      <c r="AT12" s="5"/>
+      <c r="AU12" s="5"/>
+      <c r="AV12" s="5"/>
+      <c r="AW12" s="5"/>
+      <c r="AX12" s="5"/>
+      <c r="AY12" s="71"/>
+      <c r="AZ12" s="5"/>
+      <c r="BA12" s="5"/>
+      <c r="BB12" s="5"/>
+      <c r="BC12" s="5"/>
+      <c r="BD12" s="5"/>
+      <c r="BE12" s="5"/>
+      <c r="BF12" s="5"/>
+      <c r="BG12" s="5"/>
+    </row>
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="34"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
-      <c r="AB12" s="4"/>
-      <c r="AC12" s="4"/>
-      <c r="AD12" s="4"/>
-      <c r="AE12" s="4"/>
-      <c r="AF12" s="4"/>
-      <c r="AG12" s="35"/>
-      <c r="AH12" s="8"/>
-      <c r="AI12" s="1"/>
-      <c r="AJ12" s="1"/>
-      <c r="AK12" s="1"/>
-      <c r="AL12" s="1"/>
-      <c r="AM12" s="1"/>
-      <c r="AN12" s="1"/>
-      <c r="AO12" s="1"/>
-      <c r="AP12" s="1"/>
-      <c r="AQ12" s="1"/>
-      <c r="AR12" s="1"/>
-      <c r="AS12" s="1"/>
-      <c r="AT12" s="1"/>
-      <c r="AU12" s="1"/>
-      <c r="AV12" s="1"/>
-      <c r="AW12" s="1"/>
-      <c r="AX12" s="1"/>
-      <c r="AY12" s="1"/>
-      <c r="AZ12" s="1"/>
-      <c r="BA12" s="1"/>
-      <c r="BB12" s="1"/>
-      <c r="BC12" s="1"/>
-      <c r="BD12" s="1"/>
-      <c r="BE12" s="1"/>
-      <c r="BF12" s="1"/>
-      <c r="BG12" s="1"/>
-    </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2029,7 +2074,7 @@
       <c r="AV13" s="1"/>
       <c r="AW13" s="1"/>
       <c r="AX13" s="1"/>
-      <c r="AY13" s="1"/>
+      <c r="AY13" s="71"/>
       <c r="AZ13" s="1"/>
       <c r="BA13" s="1"/>
       <c r="BB13" s="1"/>
@@ -2042,12 +2087,12 @@
     <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
@@ -2092,7 +2137,7 @@
       <c r="AV14" s="1"/>
       <c r="AW14" s="1"/>
       <c r="AX14" s="1"/>
-      <c r="AY14" s="1"/>
+      <c r="AY14" s="71"/>
       <c r="AZ14" s="1"/>
       <c r="BA14" s="1"/>
       <c r="BB14" s="1"/>
@@ -2104,14 +2149,16 @@
     </row>
     <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="3"/>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -2153,7 +2200,7 @@
       <c r="AV15" s="1"/>
       <c r="AW15" s="1"/>
       <c r="AX15" s="1"/>
-      <c r="AY15" s="1"/>
+      <c r="AY15" s="71"/>
       <c r="AZ15" s="1"/>
       <c r="BA15" s="1"/>
       <c r="BB15" s="1"/>
@@ -2163,21 +2210,17 @@
       <c r="BF15" s="1"/>
       <c r="BG15" s="1"/>
     </row>
-    <row r="16" spans="1:59" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>5</v>
-      </c>
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -2218,7 +2261,7 @@
       <c r="AV16" s="1"/>
       <c r="AW16" s="1"/>
       <c r="AX16" s="1"/>
-      <c r="AY16" s="1"/>
+      <c r="AY16" s="71"/>
       <c r="AZ16" s="1"/>
       <c r="BA16" s="1"/>
       <c r="BB16" s="1"/>
@@ -2229,9 +2272,11 @@
       <c r="BG16" s="1"/>
     </row>
     <row r="17" spans="1:59" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2281,7 +2326,7 @@
       <c r="AV17" s="1"/>
       <c r="AW17" s="1"/>
       <c r="AX17" s="1"/>
-      <c r="AY17" s="1"/>
+      <c r="AY17" s="71"/>
       <c r="AZ17" s="1"/>
       <c r="BA17" s="1"/>
       <c r="BB17" s="1"/>
@@ -2293,10 +2338,10 @@
     </row>
     <row r="18" spans="1:59" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="4"/>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -2344,7 +2389,7 @@
       <c r="AV18" s="1"/>
       <c r="AW18" s="1"/>
       <c r="AX18" s="1"/>
-      <c r="AY18" s="1"/>
+      <c r="AY18" s="71"/>
       <c r="AZ18" s="1"/>
       <c r="BA18" s="1"/>
       <c r="BB18" s="1"/>
@@ -2356,16 +2401,18 @@
     </row>
     <row r="19" spans="1:59" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="B19" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="C19" s="4"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -2405,7 +2452,7 @@
       <c r="AV19" s="1"/>
       <c r="AW19" s="1"/>
       <c r="AX19" s="1"/>
-      <c r="AY19" s="1"/>
+      <c r="AY19" s="71"/>
       <c r="AZ19" s="1"/>
       <c r="BA19" s="1"/>
       <c r="BB19" s="1"/>
@@ -2415,30 +2462,26 @@
       <c r="BF19" s="1"/>
       <c r="BG19" s="1"/>
     </row>
-    <row r="20" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="1"/>
+    <row r="20" spans="1:59" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
@@ -2470,7 +2513,7 @@
       <c r="AV20" s="1"/>
       <c r="AW20" s="1"/>
       <c r="AX20" s="1"/>
-      <c r="AY20" s="1"/>
+      <c r="AY20" s="71"/>
       <c r="AZ20" s="1"/>
       <c r="BA20" s="1"/>
       <c r="BB20" s="1"/>
@@ -2481,9 +2524,11 @@
       <c r="BG20" s="1"/>
     </row>
     <row r="21" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2495,10 +2540,10 @@
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
@@ -2533,7 +2578,7 @@
       <c r="AV21" s="1"/>
       <c r="AW21" s="1"/>
       <c r="AX21" s="1"/>
-      <c r="AY21" s="1"/>
+      <c r="AY21" s="71"/>
       <c r="AZ21" s="1"/>
       <c r="BA21" s="1"/>
       <c r="BB21" s="1"/>
@@ -2545,6 +2590,9 @@
     </row>
     <row r="22" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -2552,13 +2600,13 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="1"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
@@ -2593,7 +2641,7 @@
       <c r="AV22" s="1"/>
       <c r="AW22" s="1"/>
       <c r="AX22" s="1"/>
-      <c r="AY22" s="1"/>
+      <c r="AY22" s="71"/>
       <c r="AZ22" s="1"/>
       <c r="BA22" s="1"/>
       <c r="BB22" s="1"/>
@@ -2605,7 +2653,6 @@
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -2614,17 +2661,17 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
       <c r="V23" s="1"/>
       <c r="W23" s="6"/>
       <c r="X23" s="34"/>
@@ -2654,7 +2701,7 @@
       <c r="AV23" s="1"/>
       <c r="AW23" s="1"/>
       <c r="AX23" s="1"/>
-      <c r="AY23" s="1"/>
+      <c r="AY23" s="71"/>
       <c r="AZ23" s="1"/>
       <c r="BA23" s="1"/>
       <c r="BB23" s="1"/>
@@ -2665,12 +2712,8 @@
       <c r="BG23" s="1"/>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -2679,9 +2722,9 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="4"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
@@ -2719,7 +2762,7 @@
       <c r="AV24" s="1"/>
       <c r="AW24" s="1"/>
       <c r="AX24" s="1"/>
-      <c r="AY24" s="1"/>
+      <c r="AY24" s="71"/>
       <c r="AZ24" s="1"/>
       <c r="BA24" s="1"/>
       <c r="BB24" s="1"/>
@@ -2730,9 +2773,11 @@
       <c r="BG24" s="1"/>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="4" t="s">
-        <v>43</v>
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2782,7 +2827,7 @@
       <c r="AV25" s="1"/>
       <c r="AW25" s="1"/>
       <c r="AX25" s="1"/>
-      <c r="AY25" s="1"/>
+      <c r="AY25" s="71"/>
       <c r="AZ25" s="1"/>
       <c r="BA25" s="1"/>
       <c r="BB25" s="1"/>
@@ -2794,7 +2839,9 @@
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="B26" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -2804,8 +2851,8 @@
       <c r="I26" s="1"/>
       <c r="J26" s="4"/>
       <c r="K26" s="1"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
@@ -2843,7 +2890,7 @@
       <c r="AV26" s="1"/>
       <c r="AW26" s="1"/>
       <c r="AX26" s="1"/>
-      <c r="AY26" s="1"/>
+      <c r="AY26" s="71"/>
       <c r="AZ26" s="1"/>
       <c r="BA26" s="1"/>
       <c r="BB26" s="1"/>
@@ -2867,7 +2914,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
-      <c r="N27" s="1"/>
+      <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
@@ -2904,7 +2951,7 @@
       <c r="AV27" s="1"/>
       <c r="AW27" s="1"/>
       <c r="AX27" s="1"/>
-      <c r="AY27" s="1"/>
+      <c r="AY27" s="71"/>
       <c r="AZ27" s="1"/>
       <c r="BA27" s="1"/>
       <c r="BB27" s="1"/>
@@ -2915,9 +2962,7 @@
       <c r="BG27" s="1"/>
     </row>
     <row r="28" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -2930,7 +2975,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
-      <c r="N28" s="18"/>
+      <c r="N28" s="1"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
@@ -2967,7 +3012,7 @@
       <c r="AV28" s="1"/>
       <c r="AW28" s="1"/>
       <c r="AX28" s="1"/>
-      <c r="AY28" s="1"/>
+      <c r="AY28" s="71"/>
       <c r="AZ28" s="1"/>
       <c r="BA28" s="1"/>
       <c r="BB28" s="1"/>
@@ -2978,7 +3023,9 @@
       <c r="BG28" s="1"/>
     </row>
     <row r="29" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -2988,10 +3035,10 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="K29" s="1"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
+      <c r="N29" s="18"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
@@ -3028,7 +3075,7 @@
       <c r="AV29" s="1"/>
       <c r="AW29" s="1"/>
       <c r="AX29" s="1"/>
-      <c r="AY29" s="1"/>
+      <c r="AY29" s="71"/>
       <c r="AZ29" s="1"/>
       <c r="BA29" s="1"/>
       <c r="BB29" s="1"/>
@@ -3048,18 +3095,18 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
       <c r="V30" s="1"/>
       <c r="W30" s="6"/>
       <c r="X30" s="34"/>
@@ -3089,7 +3136,7 @@
       <c r="AV30" s="1"/>
       <c r="AW30" s="1"/>
       <c r="AX30" s="1"/>
-      <c r="AY30" s="1"/>
+      <c r="AY30" s="71"/>
       <c r="AZ30" s="1"/>
       <c r="BA30" s="1"/>
       <c r="BB30" s="1"/>
@@ -3100,137 +3147,137 @@
       <c r="BG30" s="1"/>
     </row>
     <row r="31" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="34"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="4"/>
+      <c r="AB31" s="4"/>
+      <c r="AC31" s="4"/>
+      <c r="AD31" s="4"/>
+      <c r="AE31" s="4"/>
+      <c r="AF31" s="4"/>
+      <c r="AG31" s="35"/>
+      <c r="AH31" s="8"/>
+      <c r="AI31" s="1"/>
+      <c r="AJ31" s="1"/>
+      <c r="AK31" s="1"/>
+      <c r="AL31" s="1"/>
+      <c r="AM31" s="1"/>
+      <c r="AN31" s="1"/>
+      <c r="AO31" s="1"/>
+      <c r="AP31" s="1"/>
+      <c r="AQ31" s="1"/>
+      <c r="AR31" s="1"/>
+      <c r="AS31" s="1"/>
+      <c r="AT31" s="1"/>
+      <c r="AU31" s="1"/>
+      <c r="AV31" s="1"/>
+      <c r="AW31" s="1"/>
+      <c r="AX31" s="1"/>
+      <c r="AY31" s="71"/>
+      <c r="AZ31" s="1"/>
+      <c r="BA31" s="1"/>
+      <c r="BB31" s="1"/>
+      <c r="BC31" s="1"/>
+      <c r="BD31" s="1"/>
+      <c r="BE31" s="1"/>
+      <c r="BF31" s="1"/>
+      <c r="BG31" s="1"/>
+    </row>
+    <row r="32" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-      <c r="V31" s="5"/>
-      <c r="W31" s="7"/>
-      <c r="X31" s="36"/>
-      <c r="Y31" s="5"/>
-      <c r="Z31" s="5"/>
-      <c r="AA31" s="5"/>
-      <c r="AB31" s="5"/>
-      <c r="AC31" s="5"/>
-      <c r="AD31" s="5"/>
-      <c r="AE31" s="5"/>
-      <c r="AF31" s="5"/>
-      <c r="AG31" s="37"/>
-      <c r="AH31" s="21"/>
-      <c r="AI31" s="5"/>
-      <c r="AJ31" s="5"/>
-      <c r="AK31" s="5"/>
-      <c r="AL31" s="5"/>
-      <c r="AM31" s="5"/>
-      <c r="AN31" s="5"/>
-      <c r="AO31" s="5"/>
-      <c r="AP31" s="5"/>
-      <c r="AQ31" s="5"/>
-      <c r="AR31" s="5"/>
-      <c r="AS31" s="5"/>
-      <c r="AT31" s="5"/>
-      <c r="AU31" s="5"/>
-      <c r="AV31" s="5"/>
-      <c r="AW31" s="5"/>
-      <c r="AX31" s="5"/>
-      <c r="AY31" s="5"/>
-      <c r="AZ31" s="5"/>
-      <c r="BA31" s="5"/>
-      <c r="BB31" s="5"/>
-      <c r="BC31" s="5"/>
-      <c r="BD31" s="5"/>
-      <c r="BE31" s="5"/>
-      <c r="BF31" s="5"/>
-      <c r="BG31" s="5"/>
-    </row>
-    <row r="32" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="36"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="5"/>
+      <c r="AB32" s="5"/>
+      <c r="AC32" s="5"/>
+      <c r="AD32" s="5"/>
+      <c r="AE32" s="5"/>
+      <c r="AF32" s="5"/>
+      <c r="AG32" s="37"/>
+      <c r="AH32" s="21"/>
+      <c r="AI32" s="5"/>
+      <c r="AJ32" s="5"/>
+      <c r="AK32" s="5"/>
+      <c r="AL32" s="5"/>
+      <c r="AM32" s="5"/>
+      <c r="AN32" s="5"/>
+      <c r="AO32" s="5"/>
+      <c r="AP32" s="5"/>
+      <c r="AQ32" s="5"/>
+      <c r="AR32" s="5"/>
+      <c r="AS32" s="5"/>
+      <c r="AT32" s="5"/>
+      <c r="AU32" s="5"/>
+      <c r="AV32" s="5"/>
+      <c r="AW32" s="5"/>
+      <c r="AX32" s="5"/>
+      <c r="AY32" s="71"/>
+      <c r="AZ32" s="5"/>
+      <c r="BA32" s="5"/>
+      <c r="BB32" s="5"/>
+      <c r="BC32" s="5"/>
+      <c r="BD32" s="5"/>
+      <c r="BE32" s="5"/>
+      <c r="BF32" s="5"/>
+      <c r="BG32" s="5"/>
+    </row>
+    <row r="33" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-      <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="34"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
-      <c r="AA32" s="4"/>
-      <c r="AB32" s="4"/>
-      <c r="AC32" s="4"/>
-      <c r="AD32" s="4"/>
-      <c r="AE32" s="4"/>
-      <c r="AF32" s="4"/>
-      <c r="AG32" s="35"/>
-      <c r="AI32" s="4"/>
-      <c r="AJ32" s="1"/>
-      <c r="AK32" s="1"/>
-      <c r="AL32" s="1"/>
-      <c r="AM32" s="1"/>
-      <c r="AN32" s="1"/>
-      <c r="AO32" s="1"/>
-      <c r="AP32" s="1"/>
-      <c r="AQ32" s="1"/>
-      <c r="AR32" s="1"/>
-      <c r="AS32" s="1"/>
-      <c r="AT32" s="1"/>
-      <c r="AU32" s="1"/>
-      <c r="AV32" s="1"/>
-      <c r="AW32" s="1"/>
-      <c r="AX32" s="1"/>
-      <c r="AY32" s="1"/>
-      <c r="AZ32" s="1"/>
-      <c r="BA32" s="1"/>
-      <c r="BB32" s="1"/>
-      <c r="BC32" s="1"/>
-      <c r="BD32" s="1"/>
-      <c r="BE32" s="1"/>
-      <c r="BF32" s="1"/>
-      <c r="BG32" s="1"/>
-    </row>
-    <row r="33" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" t="s">
-        <v>54</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -3278,7 +3325,7 @@
       <c r="AV33" s="1"/>
       <c r="AW33" s="1"/>
       <c r="AX33" s="1"/>
-      <c r="AY33" s="1"/>
+      <c r="AY33" s="71"/>
       <c r="AZ33" s="1"/>
       <c r="BA33" s="1"/>
       <c r="BB33" s="1"/>
@@ -3290,8 +3337,8 @@
     </row>
     <row r="34" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="1" t="s">
-        <v>40</v>
+      <c r="B34" t="s">
+        <v>54</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -3312,7 +3359,7 @@
       <c r="S34" s="1"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
-      <c r="W34" s="4"/>
+      <c r="W34" s="9"/>
       <c r="X34" s="34"/>
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>
@@ -3323,7 +3370,6 @@
       <c r="AE34" s="4"/>
       <c r="AF34" s="4"/>
       <c r="AG34" s="35"/>
-      <c r="AH34" s="9"/>
       <c r="AI34" s="4"/>
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
@@ -3340,7 +3386,7 @@
       <c r="AV34" s="1"/>
       <c r="AW34" s="1"/>
       <c r="AX34" s="1"/>
-      <c r="AY34" s="1"/>
+      <c r="AY34" s="71"/>
       <c r="AZ34" s="1"/>
       <c r="BA34" s="1"/>
       <c r="BB34" s="1"/>
@@ -3352,7 +3398,9 @@
     </row>
     <row r="35" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -3364,7 +3412,7 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
+      <c r="N35" s="18"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
@@ -3400,7 +3448,7 @@
       <c r="AV35" s="1"/>
       <c r="AW35" s="1"/>
       <c r="AX35" s="1"/>
-      <c r="AY35" s="1"/>
+      <c r="AY35" s="71"/>
       <c r="AZ35" s="1"/>
       <c r="BA35" s="1"/>
       <c r="BB35" s="1"/>
@@ -3443,9 +3491,9 @@
       <c r="AE36" s="4"/>
       <c r="AF36" s="4"/>
       <c r="AG36" s="35"/>
-      <c r="AH36" s="8"/>
-      <c r="AI36" s="1"/>
-      <c r="AJ36" s="4"/>
+      <c r="AH36" s="9"/>
+      <c r="AI36" s="4"/>
+      <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
       <c r="AL36" s="1"/>
       <c r="AM36" s="1"/>
@@ -3460,7 +3508,7 @@
       <c r="AV36" s="1"/>
       <c r="AW36" s="1"/>
       <c r="AX36" s="1"/>
-      <c r="AY36" s="1"/>
+      <c r="AY36" s="71"/>
       <c r="AZ36" s="1"/>
       <c r="BA36" s="1"/>
       <c r="BB36" s="1"/>
@@ -3471,12 +3519,8 @@
       <c r="BG36" s="1"/>
     </row>
     <row r="37" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -3488,7 +3532,7 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
-      <c r="N37" s="18"/>
+      <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
@@ -3508,6 +3552,7 @@
       <c r="AF37" s="4"/>
       <c r="AG37" s="35"/>
       <c r="AH37" s="8"/>
+      <c r="AI37" s="1"/>
       <c r="AJ37" s="4"/>
       <c r="AK37" s="1"/>
       <c r="AL37" s="1"/>
@@ -3523,7 +3568,7 @@
       <c r="AV37" s="1"/>
       <c r="AW37" s="1"/>
       <c r="AX37" s="1"/>
-      <c r="AY37" s="1"/>
+      <c r="AY37" s="71"/>
       <c r="AZ37" s="1"/>
       <c r="BA37" s="1"/>
       <c r="BB37" s="1"/>
@@ -3534,9 +3579,11 @@
       <c r="BG37" s="1"/>
     </row>
     <row r="38" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
+      <c r="A38" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B38" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -3584,7 +3631,7 @@
       <c r="AV38" s="1"/>
       <c r="AW38" s="1"/>
       <c r="AX38" s="1"/>
-      <c r="AY38" s="1"/>
+      <c r="AY38" s="71"/>
       <c r="AZ38" s="1"/>
       <c r="BA38" s="1"/>
       <c r="BB38" s="1"/>
@@ -3596,8 +3643,8 @@
     </row>
     <row r="39" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="4" t="s">
-        <v>55</v>
+      <c r="B39" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -3645,7 +3692,7 @@
       <c r="AV39" s="1"/>
       <c r="AW39" s="1"/>
       <c r="AX39" s="1"/>
-      <c r="AY39" s="1"/>
+      <c r="AY39" s="71"/>
       <c r="AZ39" s="1"/>
       <c r="BA39" s="1"/>
       <c r="BB39" s="1"/>
@@ -3657,7 +3704,9 @@
     </row>
     <row r="40" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
+      <c r="B40" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -3669,7 +3718,7 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
+      <c r="N40" s="18"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
@@ -3677,7 +3726,7 @@
       <c r="S40" s="1"/>
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
-      <c r="W40" s="1"/>
+      <c r="W40" s="4"/>
       <c r="X40" s="34"/>
       <c r="Y40" s="4"/>
       <c r="Z40" s="4"/>
@@ -3689,7 +3738,6 @@
       <c r="AF40" s="4"/>
       <c r="AG40" s="35"/>
       <c r="AH40" s="8"/>
-      <c r="AI40" s="1"/>
       <c r="AJ40" s="4"/>
       <c r="AK40" s="1"/>
       <c r="AL40" s="1"/>
@@ -3705,7 +3753,7 @@
       <c r="AV40" s="1"/>
       <c r="AW40" s="1"/>
       <c r="AX40" s="1"/>
-      <c r="AY40" s="1"/>
+      <c r="AY40" s="71"/>
       <c r="AZ40" s="1"/>
       <c r="BA40" s="1"/>
       <c r="BB40" s="1"/>
@@ -3749,39 +3797,35 @@
       <c r="AF41" s="4"/>
       <c r="AG41" s="35"/>
       <c r="AH41" s="8"/>
-      <c r="AI41" s="4"/>
+      <c r="AI41" s="1"/>
       <c r="AJ41" s="4"/>
-      <c r="AK41" s="4"/>
-      <c r="AL41" s="4"/>
-      <c r="AM41" s="4"/>
-      <c r="AN41" s="4"/>
-      <c r="AO41" s="4"/>
-      <c r="AP41" s="4"/>
-      <c r="AQ41" s="4"/>
-      <c r="AR41" s="4"/>
-      <c r="AS41" s="4"/>
-      <c r="AT41" s="4"/>
-      <c r="AU41" s="4"/>
-      <c r="AV41" s="4"/>
-      <c r="AW41" s="4"/>
-      <c r="AX41" s="4"/>
-      <c r="AY41" s="4"/>
-      <c r="AZ41" s="4"/>
-      <c r="BA41" s="4"/>
+      <c r="AK41" s="1"/>
+      <c r="AL41" s="1"/>
+      <c r="AM41" s="1"/>
+      <c r="AN41" s="1"/>
+      <c r="AO41" s="1"/>
+      <c r="AP41" s="1"/>
+      <c r="AQ41" s="1"/>
+      <c r="AR41" s="1"/>
+      <c r="AS41" s="1"/>
+      <c r="AT41" s="1"/>
+      <c r="AU41" s="1"/>
+      <c r="AV41" s="1"/>
+      <c r="AW41" s="1"/>
+      <c r="AX41" s="1"/>
+      <c r="AY41" s="71"/>
+      <c r="AZ41" s="1"/>
+      <c r="BA41" s="1"/>
       <c r="BB41" s="1"/>
       <c r="BC41" s="1"/>
-      <c r="BD41" s="4"/>
-      <c r="BE41" s="4"/>
+      <c r="BD41" s="1"/>
+      <c r="BE41" s="1"/>
       <c r="BF41" s="1"/>
       <c r="BG41" s="1"/>
     </row>
     <row r="42" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -3793,12 +3837,12 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="48"/>
-      <c r="Q42" s="48"/>
-      <c r="R42" s="48"/>
-      <c r="S42" s="48"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
@@ -3829,7 +3873,7 @@
       <c r="AV42" s="4"/>
       <c r="AW42" s="4"/>
       <c r="AX42" s="4"/>
-      <c r="AY42" s="4"/>
+      <c r="AY42" s="71"/>
       <c r="AZ42" s="4"/>
       <c r="BA42" s="4"/>
       <c r="BB42" s="1"/>
@@ -3840,9 +3884,11 @@
       <c r="BG42" s="1"/>
     </row>
     <row r="43" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B43" s="1" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -3891,7 +3937,7 @@
       <c r="AV43" s="4"/>
       <c r="AW43" s="4"/>
       <c r="AX43" s="4"/>
-      <c r="AY43" s="4"/>
+      <c r="AY43" s="71"/>
       <c r="AZ43" s="4"/>
       <c r="BA43" s="4"/>
       <c r="BB43" s="1"/>
@@ -3904,7 +3950,7 @@
     <row r="44" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -3917,12 +3963,12 @@
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
+      <c r="N44" s="18"/>
       <c r="O44" s="18"/>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
-      <c r="S44" s="1"/>
+      <c r="P44" s="48"/>
+      <c r="Q44" s="48"/>
+      <c r="R44" s="48"/>
+      <c r="S44" s="48"/>
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
@@ -3953,7 +3999,7 @@
       <c r="AV44" s="4"/>
       <c r="AW44" s="4"/>
       <c r="AX44" s="4"/>
-      <c r="AY44" s="4"/>
+      <c r="AY44" s="71"/>
       <c r="AZ44" s="4"/>
       <c r="BA44" s="4"/>
       <c r="BB44" s="1"/>
@@ -3965,7 +4011,9 @@
     </row>
     <row r="45" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -3978,7 +4026,7 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
+      <c r="O45" s="18"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
@@ -4013,7 +4061,7 @@
       <c r="AV45" s="4"/>
       <c r="AW45" s="4"/>
       <c r="AX45" s="4"/>
-      <c r="AY45" s="4"/>
+      <c r="AY45" s="71"/>
       <c r="AZ45" s="4"/>
       <c r="BA45" s="4"/>
       <c r="BB45" s="1"/>
@@ -4042,8 +4090,8 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
-      <c r="S46" s="48"/>
-      <c r="U46" s="48"/>
+      <c r="S46" s="1"/>
+      <c r="U46" s="1"/>
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
       <c r="X46" s="34"/>
@@ -4073,7 +4121,7 @@
       <c r="AV46" s="4"/>
       <c r="AW46" s="4"/>
       <c r="AX46" s="4"/>
-      <c r="AY46" s="4"/>
+      <c r="AY46" s="71"/>
       <c r="AZ46" s="4"/>
       <c r="BA46" s="4"/>
       <c r="BB46" s="1"/>
@@ -4084,12 +4132,8 @@
       <c r="BG46" s="1"/>
     </row>
     <row r="47" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -4103,9 +4147,10 @@
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="48"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="48"/>
       <c r="U47" s="48"/>
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
@@ -4136,7 +4181,7 @@
       <c r="AV47" s="4"/>
       <c r="AW47" s="4"/>
       <c r="AX47" s="4"/>
-      <c r="AY47" s="4"/>
+      <c r="AY47" s="71"/>
       <c r="AZ47" s="4"/>
       <c r="BA47" s="4"/>
       <c r="BB47" s="1"/>
@@ -4147,9 +4192,11 @@
       <c r="BG47" s="1"/>
     </row>
     <row r="48" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="4" t="s">
-        <v>43</v>
+      <c r="A48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -4197,7 +4244,7 @@
       <c r="AV48" s="4"/>
       <c r="AW48" s="4"/>
       <c r="AX48" s="4"/>
-      <c r="AY48" s="4"/>
+      <c r="AY48" s="71"/>
       <c r="AZ48" s="4"/>
       <c r="BA48" s="4"/>
       <c r="BB48" s="1"/>
@@ -4209,7 +4256,9 @@
     </row>
     <row r="49" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
+      <c r="B49" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -4223,8 +4272,8 @@
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
+      <c r="P49" s="18"/>
+      <c r="Q49" s="18"/>
       <c r="R49" s="48"/>
       <c r="U49" s="48"/>
       <c r="V49" s="1"/>
@@ -4256,7 +4305,7 @@
       <c r="AV49" s="4"/>
       <c r="AW49" s="4"/>
       <c r="AX49" s="4"/>
-      <c r="AY49" s="4"/>
+      <c r="AY49" s="71"/>
       <c r="AZ49" s="4"/>
       <c r="BA49" s="4"/>
       <c r="BB49" s="1"/>
@@ -4284,9 +4333,8 @@
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
-      <c r="S50" s="1"/>
-      <c r="U50" s="1"/>
+      <c r="R50" s="48"/>
+      <c r="U50" s="48"/>
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
       <c r="X50" s="34"/>
@@ -4316,7 +4364,7 @@
       <c r="AV50" s="4"/>
       <c r="AW50" s="4"/>
       <c r="AX50" s="4"/>
-      <c r="AY50" s="4"/>
+      <c r="AY50" s="71"/>
       <c r="AZ50" s="4"/>
       <c r="BA50" s="4"/>
       <c r="BB50" s="1"/>
@@ -4327,9 +4375,7 @@
       <c r="BG50" s="1"/>
     </row>
     <row r="51" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -4346,9 +4392,10 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
-      <c r="R51" s="18"/>
+      <c r="R51" s="1"/>
       <c r="S51" s="1"/>
       <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
       <c r="W51" s="1"/>
       <c r="X51" s="34"/>
       <c r="Y51" s="4"/>
@@ -4377,7 +4424,7 @@
       <c r="AV51" s="4"/>
       <c r="AW51" s="4"/>
       <c r="AX51" s="4"/>
-      <c r="AY51" s="4"/>
+      <c r="AY51" s="71"/>
       <c r="AZ51" s="4"/>
       <c r="BA51" s="4"/>
       <c r="BB51" s="1"/>
@@ -4388,7 +4435,10 @@
       <c r="BG51" s="1"/>
     </row>
     <row r="52" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B52" s="38"/>
+      <c r="A52" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -4404,13 +4454,11 @@
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
-      <c r="R52" s="1"/>
+      <c r="R52" s="18"/>
       <c r="S52" s="1"/>
-      <c r="T52" s="1"/>
       <c r="U52" s="1"/>
-      <c r="V52" s="1"/>
-      <c r="W52" s="35"/>
-      <c r="X52" s="9"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="34"/>
       <c r="Y52" s="4"/>
       <c r="Z52" s="4"/>
       <c r="AA52" s="4"/>
@@ -4437,7 +4485,7 @@
       <c r="AV52" s="4"/>
       <c r="AW52" s="4"/>
       <c r="AX52" s="4"/>
-      <c r="AY52" s="4"/>
+      <c r="AY52" s="71"/>
       <c r="AZ52" s="4"/>
       <c r="BA52" s="4"/>
       <c r="BB52" s="1"/>
@@ -4448,139 +4496,136 @@
       <c r="BG52" s="1"/>
     </row>
     <row r="53" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+      <c r="B53" s="38"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="35"/>
+      <c r="X53" s="9"/>
+      <c r="Y53" s="4"/>
+      <c r="Z53" s="4"/>
+      <c r="AA53" s="4"/>
+      <c r="AB53" s="4"/>
+      <c r="AC53" s="4"/>
+      <c r="AD53" s="4"/>
+      <c r="AE53" s="4"/>
+      <c r="AF53" s="4"/>
+      <c r="AG53" s="35"/>
+      <c r="AH53" s="8"/>
+      <c r="AI53" s="4"/>
+      <c r="AJ53" s="4"/>
+      <c r="AK53" s="4"/>
+      <c r="AL53" s="4"/>
+      <c r="AM53" s="4"/>
+      <c r="AN53" s="4"/>
+      <c r="AO53" s="4"/>
+      <c r="AP53" s="4"/>
+      <c r="AQ53" s="4"/>
+      <c r="AR53" s="4"/>
+      <c r="AS53" s="4"/>
+      <c r="AT53" s="4"/>
+      <c r="AU53" s="4"/>
+      <c r="AV53" s="4"/>
+      <c r="AW53" s="4"/>
+      <c r="AX53" s="4"/>
+      <c r="AY53" s="71"/>
+      <c r="AZ53" s="4"/>
+      <c r="BA53" s="4"/>
+      <c r="BB53" s="1"/>
+      <c r="BC53" s="1"/>
+      <c r="BD53" s="4"/>
+      <c r="BE53" s="4"/>
+      <c r="BF53" s="1"/>
+      <c r="BG53" s="1"/>
+    </row>
+    <row r="54" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B54" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
-      <c r="P53" s="5"/>
-      <c r="Q53" s="5"/>
-      <c r="R53" s="5"/>
-      <c r="S53" s="5"/>
-      <c r="T53" s="5"/>
-      <c r="U53" s="5"/>
-      <c r="V53" s="5"/>
-      <c r="W53" s="37"/>
-      <c r="X53" s="21"/>
-      <c r="Y53" s="5"/>
-      <c r="Z53" s="5"/>
-      <c r="AA53" s="5"/>
-      <c r="AB53" s="5"/>
-      <c r="AC53" s="5"/>
-      <c r="AD53" s="5"/>
-      <c r="AE53" s="5"/>
-      <c r="AF53" s="5"/>
-      <c r="AG53" s="42"/>
-      <c r="AH53" s="21"/>
-      <c r="AI53" s="5"/>
-      <c r="AJ53" s="5"/>
-      <c r="AK53" s="5"/>
-      <c r="AL53" s="5"/>
-      <c r="AM53" s="5"/>
-      <c r="AN53" s="5"/>
-      <c r="AO53" s="5"/>
-      <c r="AP53" s="5"/>
-      <c r="AQ53" s="5"/>
-      <c r="AR53" s="5"/>
-      <c r="AS53" s="5"/>
-      <c r="AT53" s="5"/>
-      <c r="AU53" s="5"/>
-      <c r="AV53" s="5"/>
-      <c r="AW53" s="5"/>
-      <c r="AX53" s="5"/>
-      <c r="AY53" s="5"/>
-      <c r="AZ53" s="5"/>
-      <c r="BA53" s="5"/>
-      <c r="BB53" s="5"/>
-      <c r="BC53" s="5"/>
-      <c r="BD53" s="5"/>
-      <c r="BE53" s="5"/>
-      <c r="BF53" s="5"/>
-      <c r="BG53" s="5"/>
-    </row>
-    <row r="54" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5"/>
+      <c r="T54" s="5"/>
+      <c r="U54" s="5"/>
+      <c r="V54" s="5"/>
+      <c r="W54" s="37"/>
+      <c r="X54" s="21"/>
+      <c r="Y54" s="5"/>
+      <c r="Z54" s="5"/>
+      <c r="AA54" s="5"/>
+      <c r="AB54" s="5"/>
+      <c r="AC54" s="5"/>
+      <c r="AD54" s="5"/>
+      <c r="AE54" s="5"/>
+      <c r="AF54" s="5"/>
+      <c r="AG54" s="42"/>
+      <c r="AH54" s="21"/>
+      <c r="AI54" s="5"/>
+      <c r="AJ54" s="5"/>
+      <c r="AK54" s="5"/>
+      <c r="AL54" s="5"/>
+      <c r="AM54" s="5"/>
+      <c r="AN54" s="5"/>
+      <c r="AO54" s="5"/>
+      <c r="AP54" s="5"/>
+      <c r="AQ54" s="5"/>
+      <c r="AR54" s="5"/>
+      <c r="AS54" s="5"/>
+      <c r="AT54" s="5"/>
+      <c r="AU54" s="5"/>
+      <c r="AV54" s="5"/>
+      <c r="AW54" s="5"/>
+      <c r="AX54" s="5"/>
+      <c r="AY54" s="71"/>
+      <c r="AZ54" s="5"/>
+      <c r="BA54" s="5"/>
+      <c r="BB54" s="5"/>
+      <c r="BC54" s="5"/>
+      <c r="BD54" s="5"/>
+      <c r="BE54" s="5"/>
+      <c r="BF54" s="5"/>
+      <c r="BG54" s="5"/>
+    </row>
+    <row r="55" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-      <c r="P54" s="4"/>
-      <c r="Q54" s="4"/>
-      <c r="R54" s="18"/>
-      <c r="S54" s="4"/>
-      <c r="T54" s="1"/>
-      <c r="U54" s="1"/>
-      <c r="V54" s="4"/>
-      <c r="W54" s="49"/>
-      <c r="X54" s="9"/>
-      <c r="Y54" s="6"/>
-      <c r="Z54" s="4"/>
-      <c r="AA54" s="4"/>
-      <c r="AB54" s="4"/>
-      <c r="AC54" s="4"/>
-      <c r="AD54" s="4"/>
-      <c r="AE54" s="4"/>
-      <c r="AF54" s="4"/>
-      <c r="AG54" s="44"/>
-      <c r="AH54" s="9"/>
-      <c r="AI54" s="4"/>
-      <c r="AJ54" s="4"/>
-      <c r="AK54" s="4"/>
-      <c r="AL54" s="4"/>
-      <c r="AM54" s="4"/>
-      <c r="AN54" s="4"/>
-      <c r="AO54" s="4"/>
-      <c r="AP54" s="4"/>
-      <c r="AQ54" s="4"/>
-      <c r="AR54" s="4"/>
-      <c r="AS54" s="4"/>
-      <c r="AT54" s="4"/>
-      <c r="AU54" s="4"/>
-      <c r="AV54" s="4"/>
-      <c r="AW54" s="4"/>
-      <c r="AX54" s="4"/>
-      <c r="AY54" s="4"/>
-      <c r="AZ54" s="4"/>
-      <c r="BA54" s="4"/>
-      <c r="BB54" s="4"/>
-      <c r="BC54" s="4"/>
-      <c r="BD54" s="4"/>
-      <c r="BE54" s="4"/>
-      <c r="BF54" s="4"/>
-      <c r="BG54" s="4"/>
-    </row>
-    <row r="55" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" t="s">
-        <v>54</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -4630,7 +4675,7 @@
       <c r="AV55" s="4"/>
       <c r="AW55" s="4"/>
       <c r="AX55" s="4"/>
-      <c r="AY55" s="4"/>
+      <c r="AY55" s="71"/>
       <c r="AZ55" s="4"/>
       <c r="BA55" s="4"/>
       <c r="BB55" s="4"/>
@@ -4642,8 +4687,8 @@
     </row>
     <row r="56" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
-      <c r="B56" s="1" t="s">
-        <v>40</v>
+      <c r="B56" t="s">
+        <v>54</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -4693,7 +4738,7 @@
       <c r="AV56" s="4"/>
       <c r="AW56" s="4"/>
       <c r="AX56" s="4"/>
-      <c r="AY56" s="4"/>
+      <c r="AY56" s="71"/>
       <c r="AZ56" s="4"/>
       <c r="BA56" s="4"/>
       <c r="BB56" s="4"/>
@@ -4705,7 +4750,9 @@
     </row>
     <row r="57" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
+      <c r="B57" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -4721,7 +4768,7 @@
       <c r="O57" s="4"/>
       <c r="P57" s="4"/>
       <c r="Q57" s="4"/>
-      <c r="R57" s="4"/>
+      <c r="R57" s="18"/>
       <c r="S57" s="4"/>
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
@@ -4754,7 +4801,7 @@
       <c r="AV57" s="4"/>
       <c r="AW57" s="4"/>
       <c r="AX57" s="4"/>
-      <c r="AY57" s="4"/>
+      <c r="AY57" s="71"/>
       <c r="AZ57" s="4"/>
       <c r="BA57" s="4"/>
       <c r="BB57" s="4"/>
@@ -4815,7 +4862,7 @@
       <c r="AV58" s="4"/>
       <c r="AW58" s="4"/>
       <c r="AX58" s="4"/>
-      <c r="AY58" s="4"/>
+      <c r="AY58" s="71"/>
       <c r="AZ58" s="4"/>
       <c r="BA58" s="4"/>
       <c r="BB58" s="4"/>
@@ -4826,12 +4873,8 @@
       <c r="BG58" s="4"/>
     </row>
     <row r="59" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -4847,7 +4890,7 @@
       <c r="O59" s="4"/>
       <c r="P59" s="4"/>
       <c r="Q59" s="4"/>
-      <c r="R59" s="18"/>
+      <c r="R59" s="4"/>
       <c r="S59" s="4"/>
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
@@ -4880,7 +4923,7 @@
       <c r="AV59" s="4"/>
       <c r="AW59" s="4"/>
       <c r="AX59" s="4"/>
-      <c r="AY59" s="4"/>
+      <c r="AY59" s="71"/>
       <c r="AZ59" s="4"/>
       <c r="BA59" s="4"/>
       <c r="BB59" s="4"/>
@@ -4891,9 +4934,11 @@
       <c r="BG59" s="4"/>
     </row>
     <row r="60" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="4" t="s">
-        <v>55</v>
+      <c r="A60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
@@ -4943,7 +4988,7 @@
       <c r="AV60" s="4"/>
       <c r="AW60" s="4"/>
       <c r="AX60" s="4"/>
-      <c r="AY60" s="4"/>
+      <c r="AY60" s="71"/>
       <c r="AZ60" s="4"/>
       <c r="BA60" s="4"/>
       <c r="BB60" s="4"/>
@@ -4955,7 +5000,9 @@
     </row>
     <row r="61" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-      <c r="B61" s="4"/>
+      <c r="B61" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -4971,40 +5018,40 @@
       <c r="O61" s="4"/>
       <c r="P61" s="4"/>
       <c r="Q61" s="4"/>
-      <c r="R61" s="4"/>
+      <c r="R61" s="18"/>
       <c r="S61" s="4"/>
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
       <c r="V61" s="4"/>
-      <c r="W61" s="35"/>
-      <c r="X61" s="50"/>
-      <c r="Y61" s="51"/>
+      <c r="W61" s="49"/>
+      <c r="X61" s="9"/>
+      <c r="Y61" s="6"/>
       <c r="Z61" s="4"/>
       <c r="AA61" s="4"/>
       <c r="AB61" s="4"/>
       <c r="AC61" s="4"/>
       <c r="AD61" s="4"/>
       <c r="AE61" s="4"/>
-      <c r="AF61" s="48"/>
-      <c r="AG61" s="55"/>
-      <c r="AH61" s="57"/>
-      <c r="AI61" s="48"/>
-      <c r="AJ61" s="48"/>
-      <c r="AK61" s="48"/>
-      <c r="AL61" s="48"/>
-      <c r="AM61" s="48"/>
-      <c r="AN61" s="48"/>
-      <c r="AO61" s="48"/>
-      <c r="AP61" s="48"/>
-      <c r="AQ61" s="48"/>
-      <c r="AR61" s="48"/>
-      <c r="AS61" s="48"/>
+      <c r="AF61" s="4"/>
+      <c r="AG61" s="44"/>
+      <c r="AH61" s="9"/>
+      <c r="AI61" s="4"/>
+      <c r="AJ61" s="4"/>
+      <c r="AK61" s="4"/>
+      <c r="AL61" s="4"/>
+      <c r="AM61" s="4"/>
+      <c r="AN61" s="4"/>
+      <c r="AO61" s="4"/>
+      <c r="AP61" s="4"/>
+      <c r="AQ61" s="4"/>
+      <c r="AR61" s="4"/>
+      <c r="AS61" s="4"/>
       <c r="AT61" s="4"/>
       <c r="AU61" s="4"/>
       <c r="AV61" s="4"/>
       <c r="AW61" s="4"/>
       <c r="AX61" s="4"/>
-      <c r="AY61" s="4"/>
+      <c r="AY61" s="71"/>
       <c r="AZ61" s="4"/>
       <c r="BA61" s="4"/>
       <c r="BB61" s="4"/>
@@ -5038,9 +5085,9 @@
       <c r="U62" s="1"/>
       <c r="V62" s="4"/>
       <c r="W62" s="35"/>
-      <c r="X62" s="52"/>
-      <c r="Y62" s="53"/>
-      <c r="Z62" s="54"/>
+      <c r="X62" s="50"/>
+      <c r="Y62" s="51"/>
+      <c r="Z62" s="4"/>
       <c r="AA62" s="4"/>
       <c r="AB62" s="4"/>
       <c r="AC62" s="4"/>
@@ -5065,7 +5112,7 @@
       <c r="AV62" s="4"/>
       <c r="AW62" s="4"/>
       <c r="AX62" s="4"/>
-      <c r="AY62" s="4"/>
+      <c r="AY62" s="71"/>
       <c r="AZ62" s="4"/>
       <c r="BA62" s="4"/>
       <c r="BB62" s="4"/>
@@ -5076,12 +5123,8 @@
       <c r="BG62" s="4"/>
     </row>
     <row r="63" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A63" s="1"/>
+      <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -5097,7 +5140,7 @@
       <c r="O63" s="4"/>
       <c r="P63" s="4"/>
       <c r="Q63" s="4"/>
-      <c r="R63" s="18"/>
+      <c r="R63" s="4"/>
       <c r="S63" s="4"/>
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
@@ -5113,7 +5156,7 @@
       <c r="AE63" s="4"/>
       <c r="AF63" s="48"/>
       <c r="AG63" s="55"/>
-      <c r="AH63" s="58"/>
+      <c r="AH63" s="57"/>
       <c r="AI63" s="48"/>
       <c r="AJ63" s="48"/>
       <c r="AK63" s="48"/>
@@ -5130,7 +5173,7 @@
       <c r="AV63" s="4"/>
       <c r="AW63" s="4"/>
       <c r="AX63" s="4"/>
-      <c r="AY63" s="4"/>
+      <c r="AY63" s="71"/>
       <c r="AZ63" s="4"/>
       <c r="BA63" s="4"/>
       <c r="BB63" s="4"/>
@@ -5141,9 +5184,11 @@
       <c r="BG63" s="4"/>
     </row>
     <row r="64" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
+      <c r="A64" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B64" s="1" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
@@ -5161,13 +5206,13 @@
       <c r="P64" s="4"/>
       <c r="Q64" s="4"/>
       <c r="R64" s="18"/>
-      <c r="S64" s="18"/>
-      <c r="T64" s="4"/>
-      <c r="U64" s="4"/>
+      <c r="S64" s="4"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="1"/>
       <c r="V64" s="4"/>
       <c r="W64" s="35"/>
       <c r="X64" s="52"/>
-      <c r="Y64" s="54"/>
+      <c r="Y64" s="53"/>
       <c r="Z64" s="54"/>
       <c r="AA64" s="4"/>
       <c r="AB64" s="4"/>
@@ -5176,7 +5221,7 @@
       <c r="AE64" s="4"/>
       <c r="AF64" s="48"/>
       <c r="AG64" s="55"/>
-      <c r="AH64" s="57"/>
+      <c r="AH64" s="58"/>
       <c r="AI64" s="48"/>
       <c r="AJ64" s="48"/>
       <c r="AK64" s="48"/>
@@ -5193,7 +5238,7 @@
       <c r="AV64" s="4"/>
       <c r="AW64" s="4"/>
       <c r="AX64" s="4"/>
-      <c r="AY64" s="4"/>
+      <c r="AY64" s="71"/>
       <c r="AZ64" s="4"/>
       <c r="BA64" s="4"/>
       <c r="BB64" s="4"/>
@@ -5205,7 +5250,9 @@
     </row>
     <row r="65" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="B65" s="4"/>
+      <c r="B65" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
@@ -5221,15 +5268,15 @@
       <c r="O65" s="4"/>
       <c r="P65" s="4"/>
       <c r="Q65" s="4"/>
-      <c r="R65" s="4"/>
-      <c r="S65" s="4"/>
+      <c r="R65" s="18"/>
+      <c r="S65" s="18"/>
       <c r="T65" s="4"/>
       <c r="U65" s="4"/>
       <c r="V65" s="4"/>
       <c r="W65" s="35"/>
-      <c r="X65" s="9"/>
-      <c r="Y65" s="4"/>
-      <c r="Z65" s="4"/>
+      <c r="X65" s="52"/>
+      <c r="Y65" s="54"/>
+      <c r="Z65" s="54"/>
       <c r="AA65" s="4"/>
       <c r="AB65" s="4"/>
       <c r="AC65" s="4"/>
@@ -5237,7 +5284,7 @@
       <c r="AE65" s="4"/>
       <c r="AF65" s="48"/>
       <c r="AG65" s="55"/>
-      <c r="AH65" s="56"/>
+      <c r="AH65" s="57"/>
       <c r="AI65" s="48"/>
       <c r="AJ65" s="48"/>
       <c r="AK65" s="48"/>
@@ -5254,7 +5301,7 @@
       <c r="AV65" s="4"/>
       <c r="AW65" s="4"/>
       <c r="AX65" s="4"/>
-      <c r="AY65" s="4"/>
+      <c r="AY65" s="71"/>
       <c r="AZ65" s="4"/>
       <c r="BA65" s="4"/>
       <c r="BB65" s="4"/>
@@ -5265,12 +5312,8 @@
       <c r="BG65" s="4"/>
     </row>
     <row r="66" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="A66" s="1"/>
+      <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -5287,12 +5330,12 @@
       <c r="P66" s="4"/>
       <c r="Q66" s="4"/>
       <c r="R66" s="4"/>
-      <c r="S66" s="18"/>
-      <c r="T66" s="18"/>
+      <c r="S66" s="4"/>
+      <c r="T66" s="4"/>
       <c r="U66" s="4"/>
       <c r="V66" s="4"/>
-      <c r="W66" s="6"/>
-      <c r="X66" s="43"/>
+      <c r="W66" s="35"/>
+      <c r="X66" s="9"/>
       <c r="Y66" s="4"/>
       <c r="Z66" s="4"/>
       <c r="AA66" s="4"/>
@@ -5319,7 +5362,7 @@
       <c r="AV66" s="4"/>
       <c r="AW66" s="4"/>
       <c r="AX66" s="4"/>
-      <c r="AY66" s="4"/>
+      <c r="AY66" s="71"/>
       <c r="AZ66" s="4"/>
       <c r="BA66" s="4"/>
       <c r="BB66" s="4"/>
@@ -5330,9 +5373,11 @@
       <c r="BG66" s="4"/>
     </row>
     <row r="67" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="4" t="s">
-        <v>43</v>
+      <c r="A67" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
@@ -5382,7 +5427,7 @@
       <c r="AV67" s="4"/>
       <c r="AW67" s="4"/>
       <c r="AX67" s="4"/>
-      <c r="AY67" s="4"/>
+      <c r="AY67" s="71"/>
       <c r="AZ67" s="4"/>
       <c r="BA67" s="4"/>
       <c r="BB67" s="4"/>
@@ -5393,7 +5438,10 @@
       <c r="BG67" s="4"/>
     </row>
     <row r="68" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B68" s="4"/>
+      <c r="A68" s="1"/>
+      <c r="B68" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -5410,8 +5458,8 @@
       <c r="P68" s="4"/>
       <c r="Q68" s="4"/>
       <c r="R68" s="4"/>
-      <c r="S68" s="4"/>
-      <c r="T68" s="4"/>
+      <c r="S68" s="18"/>
+      <c r="T68" s="18"/>
       <c r="U68" s="4"/>
       <c r="V68" s="4"/>
       <c r="W68" s="6"/>
@@ -5442,7 +5490,7 @@
       <c r="AV68" s="4"/>
       <c r="AW68" s="4"/>
       <c r="AX68" s="4"/>
-      <c r="AY68" s="4"/>
+      <c r="AY68" s="71"/>
       <c r="AZ68" s="4"/>
       <c r="BA68" s="4"/>
       <c r="BB68" s="4"/>
@@ -5453,9 +5501,6 @@
       <c r="BG68" s="4"/>
     </row>
     <row r="69" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
@@ -5505,7 +5550,7 @@
       <c r="AV69" s="4"/>
       <c r="AW69" s="4"/>
       <c r="AX69" s="4"/>
-      <c r="AY69" s="4"/>
+      <c r="AY69" s="71"/>
       <c r="AZ69" s="4"/>
       <c r="BA69" s="4"/>
       <c r="BB69" s="4"/>
@@ -5516,139 +5561,139 @@
       <c r="BG69" s="4"/>
     </row>
     <row r="70" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4"/>
+      <c r="P70" s="4"/>
+      <c r="Q70" s="4"/>
+      <c r="R70" s="4"/>
+      <c r="S70" s="4"/>
+      <c r="T70" s="4"/>
+      <c r="U70" s="4"/>
+      <c r="V70" s="4"/>
+      <c r="W70" s="6"/>
+      <c r="X70" s="43"/>
+      <c r="Y70" s="4"/>
+      <c r="Z70" s="4"/>
+      <c r="AA70" s="4"/>
+      <c r="AB70" s="4"/>
+      <c r="AC70" s="4"/>
+      <c r="AD70" s="4"/>
+      <c r="AE70" s="4"/>
+      <c r="AF70" s="48"/>
+      <c r="AG70" s="55"/>
+      <c r="AH70" s="56"/>
+      <c r="AI70" s="48"/>
+      <c r="AJ70" s="48"/>
+      <c r="AK70" s="48"/>
+      <c r="AL70" s="48"/>
+      <c r="AM70" s="48"/>
+      <c r="AN70" s="48"/>
+      <c r="AO70" s="48"/>
+      <c r="AP70" s="48"/>
+      <c r="AQ70" s="48"/>
+      <c r="AR70" s="48"/>
+      <c r="AS70" s="48"/>
+      <c r="AT70" s="4"/>
+      <c r="AU70" s="4"/>
+      <c r="AV70" s="4"/>
+      <c r="AW70" s="4"/>
+      <c r="AX70" s="4"/>
+      <c r="AY70" s="71"/>
+      <c r="AZ70" s="4"/>
+      <c r="BA70" s="4"/>
+      <c r="BB70" s="4"/>
+      <c r="BC70" s="4"/>
+      <c r="BD70" s="4"/>
+      <c r="BE70" s="4"/>
+      <c r="BF70" s="4"/>
+      <c r="BG70" s="4"/>
+    </row>
+    <row r="71" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B71" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
-      <c r="L70" s="5"/>
-      <c r="M70" s="5"/>
-      <c r="N70" s="5"/>
-      <c r="O70" s="5"/>
-      <c r="P70" s="5"/>
-      <c r="Q70" s="5"/>
-      <c r="R70" s="5"/>
-      <c r="S70" s="5"/>
-      <c r="T70" s="5"/>
-      <c r="U70" s="5"/>
-      <c r="V70" s="5"/>
-      <c r="W70" s="7"/>
-      <c r="X70" s="41"/>
-      <c r="Y70" s="5"/>
-      <c r="Z70" s="5"/>
-      <c r="AA70" s="5"/>
-      <c r="AB70" s="5"/>
-      <c r="AC70" s="5"/>
-      <c r="AD70" s="5"/>
-      <c r="AE70" s="5"/>
-      <c r="AF70" s="5"/>
-      <c r="AG70" s="42"/>
-      <c r="AH70" s="21"/>
-      <c r="AI70" s="5"/>
-      <c r="AJ70" s="5"/>
-      <c r="AK70" s="5"/>
-      <c r="AL70" s="5"/>
-      <c r="AM70" s="5"/>
-      <c r="AN70" s="5"/>
-      <c r="AO70" s="5"/>
-      <c r="AP70" s="5"/>
-      <c r="AQ70" s="5"/>
-      <c r="AR70" s="5"/>
-      <c r="AS70" s="5"/>
-      <c r="AT70" s="5"/>
-      <c r="AU70" s="5"/>
-      <c r="AV70" s="5"/>
-      <c r="AW70" s="5"/>
-      <c r="AX70" s="5"/>
-      <c r="AY70" s="5"/>
-      <c r="AZ70" s="5"/>
-      <c r="BA70" s="5"/>
-      <c r="BB70" s="5"/>
-      <c r="BC70" s="5"/>
-      <c r="BD70" s="5"/>
-      <c r="BE70" s="5"/>
-      <c r="BF70" s="5"/>
-      <c r="BG70" s="5"/>
-    </row>
-    <row r="71" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="5"/>
+      <c r="O71" s="5"/>
+      <c r="P71" s="5"/>
+      <c r="Q71" s="5"/>
+      <c r="R71" s="5"/>
+      <c r="S71" s="5"/>
+      <c r="T71" s="5"/>
+      <c r="U71" s="5"/>
+      <c r="V71" s="5"/>
+      <c r="W71" s="7"/>
+      <c r="X71" s="41"/>
+      <c r="Y71" s="5"/>
+      <c r="Z71" s="5"/>
+      <c r="AA71" s="5"/>
+      <c r="AB71" s="5"/>
+      <c r="AC71" s="5"/>
+      <c r="AD71" s="5"/>
+      <c r="AE71" s="5"/>
+      <c r="AF71" s="5"/>
+      <c r="AG71" s="42"/>
+      <c r="AH71" s="21"/>
+      <c r="AI71" s="5"/>
+      <c r="AJ71" s="5"/>
+      <c r="AK71" s="5"/>
+      <c r="AL71" s="5"/>
+      <c r="AM71" s="5"/>
+      <c r="AN71" s="5"/>
+      <c r="AO71" s="5"/>
+      <c r="AP71" s="5"/>
+      <c r="AQ71" s="5"/>
+      <c r="AR71" s="5"/>
+      <c r="AS71" s="5"/>
+      <c r="AT71" s="5"/>
+      <c r="AU71" s="5"/>
+      <c r="AV71" s="5"/>
+      <c r="AW71" s="5"/>
+      <c r="AX71" s="5"/>
+      <c r="AY71" s="71"/>
+      <c r="AZ71" s="5"/>
+      <c r="BA71" s="5"/>
+      <c r="BB71" s="5"/>
+      <c r="BC71" s="5"/>
+      <c r="BD71" s="5"/>
+      <c r="BE71" s="5"/>
+      <c r="BF71" s="5"/>
+      <c r="BG71" s="5"/>
+    </row>
+    <row r="72" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
-      <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
-      <c r="P71" s="4"/>
-      <c r="Q71" s="4"/>
-      <c r="R71" s="4"/>
-      <c r="S71" s="4"/>
-      <c r="T71" s="18"/>
-      <c r="U71" s="4"/>
-      <c r="V71" s="4"/>
-      <c r="W71" s="6"/>
-      <c r="X71" s="43"/>
-      <c r="Y71" s="4"/>
-      <c r="Z71" s="4"/>
-      <c r="AA71" s="4"/>
-      <c r="AB71" s="4"/>
-      <c r="AC71" s="4"/>
-      <c r="AD71" s="4"/>
-      <c r="AE71" s="4"/>
-      <c r="AF71" s="4"/>
-      <c r="AG71" s="44"/>
-      <c r="AH71" s="9"/>
-      <c r="AI71" s="4"/>
-      <c r="AJ71" s="4"/>
-      <c r="AK71" s="4"/>
-      <c r="AL71" s="4"/>
-      <c r="AM71" s="4"/>
-      <c r="AN71" s="48"/>
-      <c r="AO71" s="48"/>
-      <c r="AP71" s="48"/>
-      <c r="AQ71" s="48"/>
-      <c r="AR71" s="48"/>
-      <c r="AS71" s="48"/>
-      <c r="AT71" s="48"/>
-      <c r="AU71" s="48"/>
-      <c r="AV71" s="48"/>
-      <c r="AW71" s="48"/>
-      <c r="AX71" s="48"/>
-      <c r="AY71" s="48"/>
-      <c r="AZ71" s="48"/>
-      <c r="BA71" s="4"/>
-      <c r="BB71" s="4"/>
-      <c r="BC71" s="4"/>
-      <c r="BD71" s="48"/>
-      <c r="BE71" s="4"/>
-      <c r="BF71" s="4"/>
-      <c r="BG71" s="4"/>
-    </row>
-    <row r="72" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" t="s">
-        <v>54</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
@@ -5698,7 +5743,7 @@
       <c r="AV72" s="48"/>
       <c r="AW72" s="48"/>
       <c r="AX72" s="48"/>
-      <c r="AY72" s="48"/>
+      <c r="AY72" s="71"/>
       <c r="AZ72" s="48"/>
       <c r="BA72" s="4"/>
       <c r="BB72" s="4"/>
@@ -5710,8 +5755,8 @@
     </row>
     <row r="73" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
-      <c r="B73" s="1" t="s">
-        <v>40</v>
+      <c r="B73" t="s">
+        <v>54</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
@@ -5761,7 +5806,7 @@
       <c r="AV73" s="48"/>
       <c r="AW73" s="48"/>
       <c r="AX73" s="48"/>
-      <c r="AY73" s="48"/>
+      <c r="AY73" s="71"/>
       <c r="AZ73" s="48"/>
       <c r="BA73" s="4"/>
       <c r="BB73" s="4"/>
@@ -5773,7 +5818,9 @@
     </row>
     <row r="74" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
+      <c r="B74" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -5791,7 +5838,7 @@
       <c r="Q74" s="4"/>
       <c r="R74" s="4"/>
       <c r="S74" s="4"/>
-      <c r="T74" s="48"/>
+      <c r="T74" s="18"/>
       <c r="U74" s="4"/>
       <c r="V74" s="4"/>
       <c r="W74" s="6"/>
@@ -5822,7 +5869,7 @@
       <c r="AV74" s="48"/>
       <c r="AW74" s="48"/>
       <c r="AX74" s="48"/>
-      <c r="AY74" s="48"/>
+      <c r="AY74" s="71"/>
       <c r="AZ74" s="48"/>
       <c r="BA74" s="4"/>
       <c r="BB74" s="4"/>
@@ -5852,7 +5899,7 @@
       <c r="Q75" s="4"/>
       <c r="R75" s="4"/>
       <c r="S75" s="4"/>
-      <c r="T75" s="4"/>
+      <c r="T75" s="48"/>
       <c r="U75" s="4"/>
       <c r="V75" s="4"/>
       <c r="W75" s="6"/>
@@ -5883,7 +5930,7 @@
       <c r="AV75" s="48"/>
       <c r="AW75" s="48"/>
       <c r="AX75" s="48"/>
-      <c r="AY75" s="48"/>
+      <c r="AY75" s="71"/>
       <c r="AZ75" s="48"/>
       <c r="BA75" s="4"/>
       <c r="BB75" s="4"/>
@@ -5894,12 +5941,8 @@
       <c r="BG75" s="4"/>
     </row>
     <row r="76" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -5917,7 +5960,7 @@
       <c r="Q76" s="4"/>
       <c r="R76" s="4"/>
       <c r="S76" s="4"/>
-      <c r="T76" s="18"/>
+      <c r="T76" s="4"/>
       <c r="U76" s="4"/>
       <c r="V76" s="4"/>
       <c r="W76" s="6"/>
@@ -5948,7 +5991,7 @@
       <c r="AV76" s="48"/>
       <c r="AW76" s="48"/>
       <c r="AX76" s="48"/>
-      <c r="AY76" s="48"/>
+      <c r="AY76" s="71"/>
       <c r="AZ76" s="48"/>
       <c r="BA76" s="4"/>
       <c r="BB76" s="4"/>
@@ -5959,9 +6002,11 @@
       <c r="BG76" s="4"/>
     </row>
     <row r="77" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
+      <c r="A77" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B77" s="4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
@@ -6011,7 +6056,7 @@
       <c r="AV77" s="48"/>
       <c r="AW77" s="48"/>
       <c r="AX77" s="48"/>
-      <c r="AY77" s="48"/>
+      <c r="AY77" s="71"/>
       <c r="AZ77" s="48"/>
       <c r="BA77" s="4"/>
       <c r="BB77" s="4"/>
@@ -6023,7 +6068,9 @@
     </row>
     <row r="78" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
-      <c r="B78" s="4"/>
+      <c r="B78" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
@@ -6041,7 +6088,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
       <c r="S78" s="4"/>
-      <c r="T78" s="4"/>
+      <c r="T78" s="18"/>
       <c r="U78" s="4"/>
       <c r="V78" s="4"/>
       <c r="W78" s="6"/>
@@ -6072,7 +6119,7 @@
       <c r="AV78" s="48"/>
       <c r="AW78" s="48"/>
       <c r="AX78" s="48"/>
-      <c r="AY78" s="48"/>
+      <c r="AY78" s="71"/>
       <c r="AZ78" s="48"/>
       <c r="BA78" s="4"/>
       <c r="BB78" s="4"/>
@@ -6083,12 +6130,8 @@
       <c r="BG78" s="4"/>
     </row>
     <row r="79" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A79" s="1"/>
+      <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -6106,7 +6149,7 @@
       <c r="Q79" s="4"/>
       <c r="R79" s="4"/>
       <c r="S79" s="4"/>
-      <c r="T79" s="18"/>
+      <c r="T79" s="4"/>
       <c r="U79" s="4"/>
       <c r="V79" s="4"/>
       <c r="W79" s="6"/>
@@ -6137,7 +6180,7 @@
       <c r="AV79" s="48"/>
       <c r="AW79" s="48"/>
       <c r="AX79" s="48"/>
-      <c r="AY79" s="48"/>
+      <c r="AY79" s="71"/>
       <c r="AZ79" s="48"/>
       <c r="BA79" s="4"/>
       <c r="BB79" s="4"/>
@@ -6148,9 +6191,11 @@
       <c r="BG79" s="4"/>
     </row>
     <row r="80" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
+      <c r="A80" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B80" s="1" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -6170,13 +6215,13 @@
       <c r="R80" s="4"/>
       <c r="S80" s="4"/>
       <c r="T80" s="18"/>
-      <c r="U80" s="18"/>
-      <c r="V80" s="18"/>
-      <c r="W80" s="18"/>
-      <c r="X80" s="18"/>
-      <c r="Y80" s="18"/>
-      <c r="Z80" s="18"/>
-      <c r="AA80" s="18"/>
+      <c r="U80" s="4"/>
+      <c r="V80" s="4"/>
+      <c r="W80" s="6"/>
+      <c r="X80" s="43"/>
+      <c r="Y80" s="4"/>
+      <c r="Z80" s="4"/>
+      <c r="AA80" s="4"/>
       <c r="AB80" s="4"/>
       <c r="AC80" s="4"/>
       <c r="AD80" s="4"/>
@@ -6200,7 +6245,7 @@
       <c r="AV80" s="48"/>
       <c r="AW80" s="48"/>
       <c r="AX80" s="48"/>
-      <c r="AY80" s="48"/>
+      <c r="AY80" s="71"/>
       <c r="AZ80" s="48"/>
       <c r="BA80" s="4"/>
       <c r="BB80" s="4"/>
@@ -6213,7 +6258,7 @@
     <row r="81" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
@@ -6234,12 +6279,12 @@
       <c r="S81" s="4"/>
       <c r="T81" s="18"/>
       <c r="U81" s="18"/>
-      <c r="V81" s="4"/>
-      <c r="W81" s="6"/>
-      <c r="X81" s="43"/>
-      <c r="Y81" s="4"/>
-      <c r="Z81" s="4"/>
-      <c r="AA81" s="4"/>
+      <c r="V81" s="18"/>
+      <c r="W81" s="18"/>
+      <c r="X81" s="18"/>
+      <c r="Y81" s="18"/>
+      <c r="Z81" s="18"/>
+      <c r="AA81" s="18"/>
       <c r="AB81" s="4"/>
       <c r="AC81" s="4"/>
       <c r="AD81" s="4"/>
@@ -6263,7 +6308,7 @@
       <c r="AV81" s="48"/>
       <c r="AW81" s="48"/>
       <c r="AX81" s="48"/>
-      <c r="AY81" s="48"/>
+      <c r="AY81" s="71"/>
       <c r="AZ81" s="48"/>
       <c r="BA81" s="4"/>
       <c r="BB81" s="4"/>
@@ -6276,7 +6321,7 @@
     <row r="82" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
@@ -6296,7 +6341,7 @@
       <c r="R82" s="4"/>
       <c r="S82" s="4"/>
       <c r="T82" s="18"/>
-      <c r="U82" s="4"/>
+      <c r="U82" s="18"/>
       <c r="V82" s="4"/>
       <c r="W82" s="6"/>
       <c r="X82" s="43"/>
@@ -6326,7 +6371,7 @@
       <c r="AV82" s="48"/>
       <c r="AW82" s="48"/>
       <c r="AX82" s="48"/>
-      <c r="AY82" s="48"/>
+      <c r="AY82" s="71"/>
       <c r="AZ82" s="48"/>
       <c r="BA82" s="4"/>
       <c r="BB82" s="4"/>
@@ -6339,7 +6384,7 @@
     <row r="83" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
@@ -6358,11 +6403,11 @@
       <c r="Q83" s="4"/>
       <c r="R83" s="4"/>
       <c r="S83" s="4"/>
-      <c r="T83" s="4"/>
+      <c r="T83" s="18"/>
       <c r="U83" s="4"/>
       <c r="V83" s="4"/>
       <c r="W83" s="6"/>
-      <c r="X83" s="18"/>
+      <c r="X83" s="43"/>
       <c r="Y83" s="4"/>
       <c r="Z83" s="4"/>
       <c r="AA83" s="4"/>
@@ -6389,7 +6434,7 @@
       <c r="AV83" s="48"/>
       <c r="AW83" s="48"/>
       <c r="AX83" s="48"/>
-      <c r="AY83" s="48"/>
+      <c r="AY83" s="71"/>
       <c r="AZ83" s="48"/>
       <c r="BA83" s="4"/>
       <c r="BB83" s="4"/>
@@ -6402,7 +6447,7 @@
     <row r="84" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
@@ -6425,8 +6470,8 @@
       <c r="U84" s="4"/>
       <c r="V84" s="4"/>
       <c r="W84" s="6"/>
-      <c r="X84" s="43"/>
-      <c r="Y84" s="18"/>
+      <c r="X84" s="18"/>
+      <c r="Y84" s="4"/>
       <c r="Z84" s="4"/>
       <c r="AA84" s="4"/>
       <c r="AB84" s="4"/>
@@ -6452,7 +6497,7 @@
       <c r="AV84" s="48"/>
       <c r="AW84" s="48"/>
       <c r="AX84" s="48"/>
-      <c r="AY84" s="48"/>
+      <c r="AY84" s="71"/>
       <c r="AZ84" s="48"/>
       <c r="BA84" s="4"/>
       <c r="BB84" s="4"/>
@@ -6464,7 +6509,9 @@
     </row>
     <row r="85" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
-      <c r="B85" s="4"/>
+      <c r="B85" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
@@ -6487,7 +6534,7 @@
       <c r="V85" s="4"/>
       <c r="W85" s="6"/>
       <c r="X85" s="43"/>
-      <c r="Y85" s="4"/>
+      <c r="Y85" s="18"/>
       <c r="Z85" s="4"/>
       <c r="AA85" s="4"/>
       <c r="AB85" s="4"/>
@@ -6513,7 +6560,7 @@
       <c r="AV85" s="48"/>
       <c r="AW85" s="48"/>
       <c r="AX85" s="48"/>
-      <c r="AY85" s="48"/>
+      <c r="AY85" s="71"/>
       <c r="AZ85" s="48"/>
       <c r="BA85" s="4"/>
       <c r="BB85" s="4"/>
@@ -6574,7 +6621,7 @@
       <c r="AV86" s="48"/>
       <c r="AW86" s="48"/>
       <c r="AX86" s="48"/>
-      <c r="AY86" s="48"/>
+      <c r="AY86" s="71"/>
       <c r="AZ86" s="48"/>
       <c r="BA86" s="4"/>
       <c r="BB86" s="4"/>
@@ -6585,12 +6632,8 @@
       <c r="BG86" s="4"/>
     </row>
     <row r="87" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="A87" s="1"/>
+      <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -6616,7 +6659,7 @@
       <c r="Y87" s="4"/>
       <c r="Z87" s="4"/>
       <c r="AA87" s="4"/>
-      <c r="AB87" s="18"/>
+      <c r="AB87" s="4"/>
       <c r="AC87" s="4"/>
       <c r="AD87" s="4"/>
       <c r="AE87" s="4"/>
@@ -6639,7 +6682,7 @@
       <c r="AV87" s="48"/>
       <c r="AW87" s="48"/>
       <c r="AX87" s="48"/>
-      <c r="AY87" s="48"/>
+      <c r="AY87" s="71"/>
       <c r="AZ87" s="48"/>
       <c r="BA87" s="4"/>
       <c r="BB87" s="4"/>
@@ -6650,9 +6693,11 @@
       <c r="BG87" s="4"/>
     </row>
     <row r="88" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="4" t="s">
-        <v>43</v>
+      <c r="A88" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
@@ -6702,7 +6747,7 @@
       <c r="AV88" s="48"/>
       <c r="AW88" s="48"/>
       <c r="AX88" s="48"/>
-      <c r="AY88" s="48"/>
+      <c r="AY88" s="71"/>
       <c r="AZ88" s="48"/>
       <c r="BA88" s="4"/>
       <c r="BB88" s="4"/>
@@ -6713,139 +6758,139 @@
       <c r="BG88" s="4"/>
     </row>
     <row r="89" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="1"/>
+      <c r="B89" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="4"/>
+      <c r="M89" s="4"/>
+      <c r="N89" s="4"/>
+      <c r="O89" s="4"/>
+      <c r="P89" s="4"/>
+      <c r="Q89" s="4"/>
+      <c r="R89" s="4"/>
+      <c r="S89" s="4"/>
+      <c r="T89" s="4"/>
+      <c r="U89" s="4"/>
+      <c r="V89" s="4"/>
+      <c r="W89" s="6"/>
+      <c r="X89" s="43"/>
+      <c r="Y89" s="4"/>
+      <c r="Z89" s="4"/>
+      <c r="AA89" s="4"/>
+      <c r="AB89" s="18"/>
+      <c r="AC89" s="4"/>
+      <c r="AD89" s="4"/>
+      <c r="AE89" s="4"/>
+      <c r="AF89" s="4"/>
+      <c r="AG89" s="44"/>
+      <c r="AH89" s="9"/>
+      <c r="AI89" s="4"/>
+      <c r="AJ89" s="4"/>
+      <c r="AK89" s="4"/>
+      <c r="AL89" s="4"/>
+      <c r="AM89" s="4"/>
+      <c r="AN89" s="48"/>
+      <c r="AO89" s="48"/>
+      <c r="AP89" s="48"/>
+      <c r="AQ89" s="48"/>
+      <c r="AR89" s="48"/>
+      <c r="AS89" s="48"/>
+      <c r="AT89" s="48"/>
+      <c r="AU89" s="48"/>
+      <c r="AV89" s="48"/>
+      <c r="AW89" s="48"/>
+      <c r="AX89" s="48"/>
+      <c r="AY89" s="71"/>
+      <c r="AZ89" s="48"/>
+      <c r="BA89" s="4"/>
+      <c r="BB89" s="4"/>
+      <c r="BC89" s="4"/>
+      <c r="BD89" s="48"/>
+      <c r="BE89" s="4"/>
+      <c r="BF89" s="4"/>
+      <c r="BG89" s="4"/>
+    </row>
+    <row r="90" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B90" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="5"/>
-      <c r="H89" s="5"/>
-      <c r="I89" s="5"/>
-      <c r="J89" s="5"/>
-      <c r="K89" s="5"/>
-      <c r="L89" s="5"/>
-      <c r="M89" s="5"/>
-      <c r="N89" s="5"/>
-      <c r="O89" s="5"/>
-      <c r="P89" s="5"/>
-      <c r="Q89" s="5"/>
-      <c r="R89" s="5"/>
-      <c r="S89" s="5"/>
-      <c r="T89" s="5"/>
-      <c r="U89" s="5"/>
-      <c r="V89" s="5"/>
-      <c r="W89" s="7"/>
-      <c r="X89" s="41"/>
-      <c r="Y89" s="5"/>
-      <c r="Z89" s="5"/>
-      <c r="AA89" s="5"/>
-      <c r="AB89" s="5"/>
-      <c r="AC89" s="5"/>
-      <c r="AD89" s="5"/>
-      <c r="AE89" s="5"/>
-      <c r="AF89" s="5"/>
-      <c r="AG89" s="42"/>
-      <c r="AH89" s="21"/>
-      <c r="AI89" s="5"/>
-      <c r="AJ89" s="5"/>
-      <c r="AK89" s="5"/>
-      <c r="AL89" s="5"/>
-      <c r="AM89" s="5"/>
-      <c r="AN89" s="5"/>
-      <c r="AO89" s="5"/>
-      <c r="AP89" s="5"/>
-      <c r="AQ89" s="5"/>
-      <c r="AR89" s="5"/>
-      <c r="AS89" s="5"/>
-      <c r="AT89" s="5"/>
-      <c r="AU89" s="5"/>
-      <c r="AV89" s="5"/>
-      <c r="AW89" s="5"/>
-      <c r="AX89" s="5"/>
-      <c r="AY89" s="5"/>
-      <c r="AZ89" s="5"/>
-      <c r="BA89" s="5"/>
-      <c r="BB89" s="5"/>
-      <c r="BC89" s="5"/>
-      <c r="BD89" s="5"/>
-      <c r="BE89" s="5"/>
-      <c r="BF89" s="5"/>
-      <c r="BG89" s="5"/>
-    </row>
-    <row r="90" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+      <c r="I90" s="5"/>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
+      <c r="L90" s="5"/>
+      <c r="M90" s="5"/>
+      <c r="N90" s="5"/>
+      <c r="O90" s="5"/>
+      <c r="P90" s="5"/>
+      <c r="Q90" s="5"/>
+      <c r="R90" s="5"/>
+      <c r="S90" s="5"/>
+      <c r="T90" s="5"/>
+      <c r="U90" s="5"/>
+      <c r="V90" s="5"/>
+      <c r="W90" s="7"/>
+      <c r="X90" s="41"/>
+      <c r="Y90" s="5"/>
+      <c r="Z90" s="5"/>
+      <c r="AA90" s="5"/>
+      <c r="AB90" s="5"/>
+      <c r="AC90" s="5"/>
+      <c r="AD90" s="5"/>
+      <c r="AE90" s="5"/>
+      <c r="AF90" s="5"/>
+      <c r="AG90" s="42"/>
+      <c r="AH90" s="21"/>
+      <c r="AI90" s="5"/>
+      <c r="AJ90" s="5"/>
+      <c r="AK90" s="5"/>
+      <c r="AL90" s="5"/>
+      <c r="AM90" s="5"/>
+      <c r="AN90" s="5"/>
+      <c r="AO90" s="5"/>
+      <c r="AP90" s="5"/>
+      <c r="AQ90" s="5"/>
+      <c r="AR90" s="5"/>
+      <c r="AS90" s="5"/>
+      <c r="AT90" s="5"/>
+      <c r="AU90" s="5"/>
+      <c r="AV90" s="5"/>
+      <c r="AW90" s="5"/>
+      <c r="AX90" s="5"/>
+      <c r="AY90" s="71"/>
+      <c r="AZ90" s="5"/>
+      <c r="BA90" s="5"/>
+      <c r="BB90" s="5"/>
+      <c r="BC90" s="5"/>
+      <c r="BD90" s="5"/>
+      <c r="BE90" s="5"/>
+      <c r="BF90" s="5"/>
+      <c r="BG90" s="5"/>
+    </row>
+    <row r="91" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C90" s="4"/>
-      <c r="D90" s="4"/>
-      <c r="E90" s="4"/>
-      <c r="F90" s="4"/>
-      <c r="G90" s="4"/>
-      <c r="H90" s="4"/>
-      <c r="I90" s="4"/>
-      <c r="J90" s="4"/>
-      <c r="K90" s="4"/>
-      <c r="L90" s="4"/>
-      <c r="M90" s="4"/>
-      <c r="N90" s="4"/>
-      <c r="O90" s="4"/>
-      <c r="P90" s="4"/>
-      <c r="Q90" s="4"/>
-      <c r="R90" s="4"/>
-      <c r="S90" s="4"/>
-      <c r="T90" s="4"/>
-      <c r="U90" s="4"/>
-      <c r="V90" s="4"/>
-      <c r="W90" s="6"/>
-      <c r="X90" s="43"/>
-      <c r="Y90" s="4"/>
-      <c r="Z90" s="4"/>
-      <c r="AA90" s="4"/>
-      <c r="AB90" s="4"/>
-      <c r="AC90" s="18"/>
-      <c r="AD90" s="4"/>
-      <c r="AE90" s="4"/>
-      <c r="AF90" s="4"/>
-      <c r="AG90" s="44"/>
-      <c r="AH90" s="9"/>
-      <c r="AI90" s="4"/>
-      <c r="AJ90" s="4"/>
-      <c r="AK90" s="4"/>
-      <c r="AL90" s="4"/>
-      <c r="AM90" s="4"/>
-      <c r="AN90" s="48"/>
-      <c r="AO90" s="48"/>
-      <c r="AP90" s="48"/>
-      <c r="AQ90" s="48"/>
-      <c r="AR90" s="48"/>
-      <c r="AS90" s="48"/>
-      <c r="AT90" s="48"/>
-      <c r="AU90" s="48"/>
-      <c r="AV90" s="48"/>
-      <c r="AW90" s="48"/>
-      <c r="AX90" s="48"/>
-      <c r="AY90" s="48"/>
-      <c r="AZ90" s="48"/>
-      <c r="BA90" s="4"/>
-      <c r="BB90" s="4"/>
-      <c r="BC90" s="4"/>
-      <c r="BD90" s="48"/>
-      <c r="BE90" s="4"/>
-      <c r="BF90" s="4"/>
-      <c r="BG90" s="4"/>
-    </row>
-    <row r="91" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-      <c r="B91" t="s">
-        <v>54</v>
       </c>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
@@ -6895,7 +6940,7 @@
       <c r="AV91" s="48"/>
       <c r="AW91" s="48"/>
       <c r="AX91" s="48"/>
-      <c r="AY91" s="48"/>
+      <c r="AY91" s="71"/>
       <c r="AZ91" s="48"/>
       <c r="BA91" s="4"/>
       <c r="BB91" s="4"/>
@@ -6907,8 +6952,8 @@
     </row>
     <row r="92" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
-      <c r="B92" s="1" t="s">
-        <v>40</v>
+      <c r="B92" t="s">
+        <v>54</v>
       </c>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
@@ -6958,7 +7003,7 @@
       <c r="AV92" s="48"/>
       <c r="AW92" s="48"/>
       <c r="AX92" s="48"/>
-      <c r="AY92" s="48"/>
+      <c r="AY92" s="71"/>
       <c r="AZ92" s="48"/>
       <c r="BA92" s="4"/>
       <c r="BB92" s="4"/>
@@ -6970,6 +7015,9 @@
     </row>
     <row r="93" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
+      <c r="B93" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
@@ -6996,7 +7044,7 @@
       <c r="Z93" s="4"/>
       <c r="AA93" s="4"/>
       <c r="AB93" s="4"/>
-      <c r="AC93" s="4"/>
+      <c r="AC93" s="18"/>
       <c r="AD93" s="4"/>
       <c r="AE93" s="4"/>
       <c r="AF93" s="4"/>
@@ -7018,7 +7066,7 @@
       <c r="AV93" s="48"/>
       <c r="AW93" s="48"/>
       <c r="AX93" s="48"/>
-      <c r="AY93" s="48"/>
+      <c r="AY93" s="71"/>
       <c r="AZ93" s="48"/>
       <c r="BA93" s="4"/>
       <c r="BB93" s="4"/>
@@ -7030,7 +7078,6 @@
     </row>
     <row r="94" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
@@ -7079,7 +7126,7 @@
       <c r="AV94" s="48"/>
       <c r="AW94" s="48"/>
       <c r="AX94" s="48"/>
-      <c r="AY94" s="48"/>
+      <c r="AY94" s="71"/>
       <c r="AZ94" s="48"/>
       <c r="BA94" s="4"/>
       <c r="BB94" s="4"/>
@@ -7090,12 +7137,8 @@
       <c r="BG94" s="4"/>
     </row>
     <row r="95" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
@@ -7123,7 +7166,7 @@
       <c r="AA95" s="4"/>
       <c r="AB95" s="4"/>
       <c r="AC95" s="4"/>
-      <c r="AD95" s="18"/>
+      <c r="AD95" s="4"/>
       <c r="AE95" s="4"/>
       <c r="AF95" s="4"/>
       <c r="AG95" s="44"/>
@@ -7144,7 +7187,7 @@
       <c r="AV95" s="48"/>
       <c r="AW95" s="48"/>
       <c r="AX95" s="48"/>
-      <c r="AY95" s="48"/>
+      <c r="AY95" s="71"/>
       <c r="AZ95" s="48"/>
       <c r="BA95" s="4"/>
       <c r="BB95" s="4"/>
@@ -7155,8 +7198,12 @@
       <c r="BG95" s="4"/>
     </row>
     <row r="96" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
+      <c r="A96" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
@@ -7184,7 +7231,7 @@
       <c r="AA96" s="4"/>
       <c r="AB96" s="4"/>
       <c r="AC96" s="4"/>
-      <c r="AD96" s="4"/>
+      <c r="AD96" s="18"/>
       <c r="AE96" s="4"/>
       <c r="AF96" s="4"/>
       <c r="AG96" s="44"/>
@@ -7205,7 +7252,7 @@
       <c r="AV96" s="48"/>
       <c r="AW96" s="48"/>
       <c r="AX96" s="48"/>
-      <c r="AY96" s="48"/>
+      <c r="AY96" s="71"/>
       <c r="AZ96" s="48"/>
       <c r="BA96" s="4"/>
       <c r="BB96" s="4"/>
@@ -7266,7 +7313,7 @@
       <c r="AV97" s="48"/>
       <c r="AW97" s="48"/>
       <c r="AX97" s="48"/>
-      <c r="AY97" s="48"/>
+      <c r="AY97" s="71"/>
       <c r="AZ97" s="48"/>
       <c r="BA97" s="4"/>
       <c r="BB97" s="4"/>
@@ -7277,12 +7324,8 @@
       <c r="BG97" s="4"/>
     </row>
     <row r="98" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
@@ -7310,13 +7353,13 @@
       <c r="AA98" s="4"/>
       <c r="AB98" s="4"/>
       <c r="AC98" s="4"/>
-      <c r="AD98" s="18"/>
-      <c r="AE98" s="18"/>
-      <c r="AF98" s="18"/>
-      <c r="AG98" s="18"/>
-      <c r="AH98" s="18"/>
-      <c r="AI98" s="18"/>
-      <c r="AJ98" s="18"/>
+      <c r="AD98" s="4"/>
+      <c r="AE98" s="4"/>
+      <c r="AF98" s="4"/>
+      <c r="AG98" s="44"/>
+      <c r="AH98" s="9"/>
+      <c r="AI98" s="4"/>
+      <c r="AJ98" s="4"/>
       <c r="AK98" s="4"/>
       <c r="AL98" s="4"/>
       <c r="AM98" s="4"/>
@@ -7331,7 +7374,7 @@
       <c r="AV98" s="48"/>
       <c r="AW98" s="48"/>
       <c r="AX98" s="48"/>
-      <c r="AY98" s="48"/>
+      <c r="AY98" s="71"/>
       <c r="AZ98" s="48"/>
       <c r="BA98" s="4"/>
       <c r="BB98" s="4"/>
@@ -7342,8 +7385,12 @@
       <c r="BG98" s="4"/>
     </row>
     <row r="99" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
+      <c r="A99" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
@@ -7371,13 +7418,13 @@
       <c r="AA99" s="4"/>
       <c r="AB99" s="4"/>
       <c r="AC99" s="4"/>
-      <c r="AD99" s="4"/>
-      <c r="AE99" s="4"/>
-      <c r="AF99" s="4"/>
-      <c r="AG99" s="44"/>
-      <c r="AH99" s="9"/>
-      <c r="AI99" s="4"/>
-      <c r="AJ99" s="4"/>
+      <c r="AD99" s="18"/>
+      <c r="AE99" s="18"/>
+      <c r="AF99" s="18"/>
+      <c r="AG99" s="18"/>
+      <c r="AH99" s="18"/>
+      <c r="AI99" s="18"/>
+      <c r="AJ99" s="18"/>
       <c r="AK99" s="4"/>
       <c r="AL99" s="4"/>
       <c r="AM99" s="4"/>
@@ -7392,7 +7439,7 @@
       <c r="AV99" s="48"/>
       <c r="AW99" s="48"/>
       <c r="AX99" s="48"/>
-      <c r="AY99" s="48"/>
+      <c r="AY99" s="71"/>
       <c r="AZ99" s="48"/>
       <c r="BA99" s="4"/>
       <c r="BB99" s="4"/>
@@ -7453,7 +7500,7 @@
       <c r="AV100" s="48"/>
       <c r="AW100" s="48"/>
       <c r="AX100" s="48"/>
-      <c r="AY100" s="48"/>
+      <c r="AY100" s="71"/>
       <c r="AZ100" s="48"/>
       <c r="BA100" s="4"/>
       <c r="BB100" s="4"/>
@@ -7514,7 +7561,7 @@
       <c r="AV101" s="48"/>
       <c r="AW101" s="48"/>
       <c r="AX101" s="48"/>
-      <c r="AY101" s="48"/>
+      <c r="AY101" s="71"/>
       <c r="AZ101" s="48"/>
       <c r="BA101" s="4"/>
       <c r="BB101" s="4"/>
@@ -7525,12 +7572,8 @@
       <c r="BG101" s="4"/>
     </row>
     <row r="102" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
@@ -7565,9 +7608,9 @@
       <c r="AH102" s="9"/>
       <c r="AI102" s="4"/>
       <c r="AJ102" s="4"/>
-      <c r="AK102" s="18"/>
-      <c r="AL102" s="18"/>
-      <c r="AM102" s="18"/>
+      <c r="AK102" s="4"/>
+      <c r="AL102" s="4"/>
+      <c r="AM102" s="4"/>
       <c r="AN102" s="48"/>
       <c r="AO102" s="48"/>
       <c r="AP102" s="48"/>
@@ -7579,7 +7622,7 @@
       <c r="AV102" s="48"/>
       <c r="AW102" s="48"/>
       <c r="AX102" s="48"/>
-      <c r="AY102" s="48"/>
+      <c r="AY102" s="71"/>
       <c r="AZ102" s="48"/>
       <c r="BA102" s="4"/>
       <c r="BB102" s="4"/>
@@ -7590,9 +7633,11 @@
       <c r="BG102" s="4"/>
     </row>
     <row r="103" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
-      <c r="B103" s="4" t="s">
-        <v>43</v>
+      <c r="A103" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
@@ -7628,7 +7673,7 @@
       <c r="AH103" s="9"/>
       <c r="AI103" s="4"/>
       <c r="AJ103" s="4"/>
-      <c r="AK103" s="4"/>
+      <c r="AK103" s="18"/>
       <c r="AL103" s="18"/>
       <c r="AM103" s="18"/>
       <c r="AN103" s="48"/>
@@ -7642,7 +7687,7 @@
       <c r="AV103" s="48"/>
       <c r="AW103" s="48"/>
       <c r="AX103" s="48"/>
-      <c r="AY103" s="48"/>
+      <c r="AY103" s="71"/>
       <c r="AZ103" s="48"/>
       <c r="BA103" s="4"/>
       <c r="BB103" s="4"/>
@@ -7653,138 +7698,140 @@
       <c r="BG103" s="4"/>
     </row>
     <row r="104" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
+      <c r="A104" s="1"/>
+      <c r="B104" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
+      <c r="H104" s="4"/>
+      <c r="I104" s="4"/>
+      <c r="J104" s="4"/>
+      <c r="K104" s="4"/>
+      <c r="L104" s="4"/>
+      <c r="M104" s="4"/>
+      <c r="N104" s="4"/>
+      <c r="O104" s="4"/>
+      <c r="P104" s="4"/>
+      <c r="Q104" s="4"/>
+      <c r="R104" s="4"/>
+      <c r="S104" s="4"/>
+      <c r="T104" s="4"/>
+      <c r="U104" s="4"/>
+      <c r="V104" s="4"/>
+      <c r="W104" s="6"/>
+      <c r="X104" s="43"/>
+      <c r="Y104" s="4"/>
+      <c r="Z104" s="4"/>
+      <c r="AA104" s="4"/>
+      <c r="AB104" s="4"/>
+      <c r="AC104" s="4"/>
+      <c r="AD104" s="4"/>
+      <c r="AE104" s="4"/>
+      <c r="AF104" s="4"/>
+      <c r="AG104" s="44"/>
+      <c r="AH104" s="9"/>
+      <c r="AI104" s="4"/>
+      <c r="AJ104" s="4"/>
+      <c r="AK104" s="4"/>
+      <c r="AL104" s="18"/>
+      <c r="AM104" s="18"/>
+      <c r="AN104" s="48"/>
+      <c r="AO104" s="48"/>
+      <c r="AP104" s="48"/>
+      <c r="AQ104" s="48"/>
+      <c r="AR104" s="48"/>
+      <c r="AS104" s="48"/>
+      <c r="AT104" s="48"/>
+      <c r="AU104" s="48"/>
+      <c r="AV104" s="48"/>
+      <c r="AW104" s="48"/>
+      <c r="AX104" s="48"/>
+      <c r="AY104" s="71"/>
+      <c r="AZ104" s="48"/>
+      <c r="BA104" s="4"/>
+      <c r="BB104" s="4"/>
+      <c r="BC104" s="4"/>
+      <c r="BD104" s="48"/>
+      <c r="BE104" s="4"/>
+      <c r="BF104" s="4"/>
+      <c r="BG104" s="4"/>
+    </row>
+    <row r="105" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B105" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
-      <c r="H104" s="5"/>
-      <c r="I104" s="5"/>
-      <c r="J104" s="5"/>
-      <c r="K104" s="5"/>
-      <c r="L104" s="5"/>
-      <c r="M104" s="5"/>
-      <c r="N104" s="5"/>
-      <c r="O104" s="5"/>
-      <c r="P104" s="5"/>
-      <c r="Q104" s="5"/>
-      <c r="R104" s="5"/>
-      <c r="S104" s="5"/>
-      <c r="T104" s="5"/>
-      <c r="U104" s="5"/>
-      <c r="V104" s="5"/>
-      <c r="W104" s="7"/>
-      <c r="X104" s="41"/>
-      <c r="Y104" s="5"/>
-      <c r="Z104" s="5"/>
-      <c r="AA104" s="5"/>
-      <c r="AB104" s="5"/>
-      <c r="AC104" s="5"/>
-      <c r="AD104" s="5"/>
-      <c r="AE104" s="5"/>
-      <c r="AF104" s="5"/>
-      <c r="AG104" s="42"/>
-      <c r="AH104" s="21"/>
-      <c r="AI104" s="5"/>
-      <c r="AJ104" s="5"/>
-      <c r="AK104" s="5"/>
-      <c r="AL104" s="5"/>
-      <c r="AM104" s="5"/>
-      <c r="AN104" s="5"/>
-      <c r="AO104" s="5"/>
-      <c r="AP104" s="5"/>
-      <c r="AQ104" s="5"/>
-      <c r="AR104" s="5"/>
-      <c r="AS104" s="5"/>
-      <c r="AT104" s="5"/>
-      <c r="AU104" s="5"/>
-      <c r="AV104" s="5"/>
-      <c r="AW104" s="5"/>
-      <c r="AX104" s="5"/>
-      <c r="AY104" s="5"/>
-      <c r="AZ104" s="5"/>
-      <c r="BA104" s="5"/>
-      <c r="BB104" s="5"/>
-      <c r="BC104" s="5"/>
-      <c r="BD104" s="5"/>
-      <c r="BE104" s="5"/>
-      <c r="BF104" s="5"/>
-      <c r="BG104" s="5"/>
-    </row>
-    <row r="105" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="5"/>
+      <c r="H105" s="5"/>
+      <c r="I105" s="5"/>
+      <c r="J105" s="5"/>
+      <c r="K105" s="5"/>
+      <c r="L105" s="5"/>
+      <c r="M105" s="5"/>
+      <c r="N105" s="5"/>
+      <c r="O105" s="5"/>
+      <c r="P105" s="5"/>
+      <c r="Q105" s="5"/>
+      <c r="R105" s="5"/>
+      <c r="S105" s="5"/>
+      <c r="T105" s="5"/>
+      <c r="U105" s="5"/>
+      <c r="V105" s="5"/>
+      <c r="W105" s="7"/>
+      <c r="X105" s="41"/>
+      <c r="Y105" s="5"/>
+      <c r="Z105" s="5"/>
+      <c r="AA105" s="5"/>
+      <c r="AB105" s="5"/>
+      <c r="AC105" s="5"/>
+      <c r="AD105" s="5"/>
+      <c r="AE105" s="5"/>
+      <c r="AF105" s="5"/>
+      <c r="AG105" s="42"/>
+      <c r="AH105" s="21"/>
+      <c r="AI105" s="5"/>
+      <c r="AJ105" s="5"/>
+      <c r="AK105" s="5"/>
+      <c r="AL105" s="5"/>
+      <c r="AM105" s="5"/>
+      <c r="AN105" s="5"/>
+      <c r="AO105" s="5"/>
+      <c r="AP105" s="5"/>
+      <c r="AQ105" s="5"/>
+      <c r="AR105" s="5"/>
+      <c r="AS105" s="5"/>
+      <c r="AT105" s="5"/>
+      <c r="AU105" s="5"/>
+      <c r="AV105" s="5"/>
+      <c r="AW105" s="5"/>
+      <c r="AX105" s="5"/>
+      <c r="AY105" s="71"/>
+      <c r="AZ105" s="5"/>
+      <c r="BA105" s="5"/>
+      <c r="BB105" s="5"/>
+      <c r="BC105" s="5"/>
+      <c r="BD105" s="5"/>
+      <c r="BE105" s="5"/>
+      <c r="BF105" s="5"/>
+      <c r="BG105" s="5"/>
+    </row>
+    <row r="106" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C105" s="4"/>
-      <c r="D105" s="4"/>
-      <c r="E105" s="4"/>
-      <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
-      <c r="H105" s="4"/>
-      <c r="I105" s="4"/>
-      <c r="J105" s="4"/>
-      <c r="K105" s="4"/>
-      <c r="L105" s="4"/>
-      <c r="M105" s="4"/>
-      <c r="N105" s="4"/>
-      <c r="O105" s="4"/>
-      <c r="P105" s="4"/>
-      <c r="Q105" s="4"/>
-      <c r="R105" s="4"/>
-      <c r="S105" s="4"/>
-      <c r="T105" s="4"/>
-      <c r="U105" s="4"/>
-      <c r="V105" s="4"/>
-      <c r="W105" s="6"/>
-      <c r="X105" s="43"/>
-      <c r="Y105" s="4"/>
-      <c r="Z105" s="4"/>
-      <c r="AA105" s="4"/>
-      <c r="AB105" s="4"/>
-      <c r="AC105" s="4"/>
-      <c r="AD105" s="4"/>
-      <c r="AE105" s="4"/>
-      <c r="AF105" s="4"/>
-      <c r="AG105" s="44"/>
-      <c r="AH105" s="9"/>
-      <c r="AI105" s="4"/>
-      <c r="AJ105" s="4"/>
-      <c r="AK105" s="4"/>
-      <c r="AL105" s="4"/>
-      <c r="AM105" s="18"/>
-      <c r="AN105" s="18"/>
-      <c r="AO105" s="18"/>
-      <c r="AP105" s="18"/>
-      <c r="AQ105" s="48"/>
-      <c r="AR105" s="48"/>
-      <c r="AS105" s="48"/>
-      <c r="AT105" s="48"/>
-      <c r="AU105" s="48"/>
-      <c r="AV105" s="48"/>
-      <c r="AW105" s="48"/>
-      <c r="AX105" s="48"/>
-      <c r="AY105" s="48"/>
-      <c r="AZ105" s="48"/>
-      <c r="BA105" s="4"/>
-      <c r="BB105" s="4"/>
-      <c r="BC105" s="4"/>
-      <c r="BD105" s="48"/>
-      <c r="BE105" s="4"/>
-      <c r="BF105" s="4"/>
-      <c r="BG105" s="4"/>
-    </row>
-    <row r="106" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
-      <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
@@ -7821,10 +7868,10 @@
       <c r="AJ106" s="4"/>
       <c r="AK106" s="4"/>
       <c r="AL106" s="4"/>
-      <c r="AM106" s="4"/>
-      <c r="AN106" s="48"/>
-      <c r="AO106" s="48"/>
-      <c r="AP106" s="48"/>
+      <c r="AM106" s="18"/>
+      <c r="AN106" s="18"/>
+      <c r="AO106" s="18"/>
+      <c r="AP106" s="18"/>
       <c r="AQ106" s="48"/>
       <c r="AR106" s="48"/>
       <c r="AS106" s="48"/>
@@ -7833,7 +7880,7 @@
       <c r="AV106" s="48"/>
       <c r="AW106" s="48"/>
       <c r="AX106" s="48"/>
-      <c r="AY106" s="48"/>
+      <c r="AY106" s="71"/>
       <c r="AZ106" s="48"/>
       <c r="BA106" s="4"/>
       <c r="BB106" s="4"/>
@@ -7894,7 +7941,7 @@
       <c r="AV107" s="48"/>
       <c r="AW107" s="48"/>
       <c r="AX107" s="48"/>
-      <c r="AY107" s="48"/>
+      <c r="AY107" s="71"/>
       <c r="AZ107" s="48"/>
       <c r="BA107" s="4"/>
       <c r="BB107" s="4"/>
@@ -7955,7 +8002,7 @@
       <c r="AV108" s="48"/>
       <c r="AW108" s="48"/>
       <c r="AX108" s="48"/>
-      <c r="AY108" s="48"/>
+      <c r="AY108" s="71"/>
       <c r="AZ108" s="48"/>
       <c r="BA108" s="4"/>
       <c r="BB108" s="4"/>
@@ -8016,7 +8063,7 @@
       <c r="AV109" s="48"/>
       <c r="AW109" s="48"/>
       <c r="AX109" s="48"/>
-      <c r="AY109" s="48"/>
+      <c r="AY109" s="71"/>
       <c r="AZ109" s="48"/>
       <c r="BA109" s="4"/>
       <c r="BB109" s="4"/>
@@ -8027,12 +8074,8 @@
       <c r="BG109" s="4"/>
     </row>
     <row r="110" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>67</v>
-      </c>
+      <c r="A110" s="1"/>
+      <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -8071,8 +8114,8 @@
       <c r="AL110" s="4"/>
       <c r="AM110" s="4"/>
       <c r="AN110" s="48"/>
-      <c r="AO110" s="18"/>
-      <c r="AP110" s="18"/>
+      <c r="AO110" s="48"/>
+      <c r="AP110" s="48"/>
       <c r="AQ110" s="48"/>
       <c r="AR110" s="48"/>
       <c r="AS110" s="48"/>
@@ -8081,7 +8124,7 @@
       <c r="AV110" s="48"/>
       <c r="AW110" s="48"/>
       <c r="AX110" s="48"/>
-      <c r="AY110" s="48"/>
+      <c r="AY110" s="71"/>
       <c r="AZ110" s="48"/>
       <c r="BA110" s="4"/>
       <c r="BB110" s="4"/>
@@ -8092,8 +8135,12 @@
       <c r="BG110" s="4"/>
     </row>
     <row r="111" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-      <c r="B111" s="4"/>
+      <c r="A111" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -8132,8 +8179,8 @@
       <c r="AL111" s="4"/>
       <c r="AM111" s="4"/>
       <c r="AN111" s="48"/>
-      <c r="AO111" s="48"/>
-      <c r="AP111" s="48"/>
+      <c r="AO111" s="18"/>
+      <c r="AP111" s="18"/>
       <c r="AQ111" s="48"/>
       <c r="AR111" s="48"/>
       <c r="AS111" s="48"/>
@@ -8142,7 +8189,7 @@
       <c r="AV111" s="48"/>
       <c r="AW111" s="48"/>
       <c r="AX111" s="48"/>
-      <c r="AY111" s="48"/>
+      <c r="AY111" s="71"/>
       <c r="AZ111" s="48"/>
       <c r="BA111" s="4"/>
       <c r="BB111" s="4"/>
@@ -8203,7 +8250,7 @@
       <c r="AV112" s="48"/>
       <c r="AW112" s="48"/>
       <c r="AX112" s="48"/>
-      <c r="AY112" s="48"/>
+      <c r="AY112" s="71"/>
       <c r="AZ112" s="48"/>
       <c r="BA112" s="4"/>
       <c r="BB112" s="4"/>
@@ -8214,12 +8261,8 @@
       <c r="BG112" s="4"/>
     </row>
     <row r="113" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B113" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="A113" s="1"/>
+      <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -8260,15 +8303,15 @@
       <c r="AN113" s="48"/>
       <c r="AO113" s="48"/>
       <c r="AP113" s="48"/>
-      <c r="AQ113" s="18"/>
-      <c r="AR113" s="18"/>
-      <c r="AS113" s="18"/>
-      <c r="AT113" s="18"/>
-      <c r="AU113" s="18"/>
-      <c r="AV113" s="18"/>
+      <c r="AQ113" s="48"/>
+      <c r="AR113" s="48"/>
+      <c r="AS113" s="48"/>
+      <c r="AT113" s="48"/>
+      <c r="AU113" s="48"/>
+      <c r="AV113" s="48"/>
       <c r="AW113" s="48"/>
       <c r="AX113" s="48"/>
-      <c r="AY113" s="48"/>
+      <c r="AY113" s="71"/>
       <c r="AZ113" s="48"/>
       <c r="BA113" s="4"/>
       <c r="BB113" s="4"/>
@@ -8279,9 +8322,11 @@
       <c r="BG113" s="4"/>
     </row>
     <row r="114" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
+      <c r="A114" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B114" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
@@ -8323,16 +8368,16 @@
       <c r="AN114" s="48"/>
       <c r="AO114" s="48"/>
       <c r="AP114" s="48"/>
-      <c r="AQ114" s="48"/>
-      <c r="AR114" s="48"/>
-      <c r="AS114" s="48"/>
-      <c r="AT114" s="48"/>
-      <c r="AU114" s="48"/>
-      <c r="AV114" s="48"/>
-      <c r="AW114" s="18"/>
-      <c r="AX114" s="18"/>
-      <c r="AY114" s="18"/>
-      <c r="AZ114" s="18"/>
+      <c r="AQ114" s="18"/>
+      <c r="AR114" s="18"/>
+      <c r="AS114" s="18"/>
+      <c r="AT114" s="18"/>
+      <c r="AU114" s="18"/>
+      <c r="AV114" s="18"/>
+      <c r="AW114" s="48"/>
+      <c r="AX114" s="48"/>
+      <c r="AY114" s="71"/>
+      <c r="AZ114" s="48"/>
       <c r="BA114" s="4"/>
       <c r="BB114" s="4"/>
       <c r="BC114" s="4"/>
@@ -8343,7 +8388,9 @@
     </row>
     <row r="115" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
-      <c r="B115" s="4"/>
+      <c r="B115" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
@@ -8390,9 +8437,9 @@
       <c r="AT115" s="48"/>
       <c r="AU115" s="48"/>
       <c r="AV115" s="48"/>
-      <c r="AW115" s="48"/>
-      <c r="AX115" s="48"/>
-      <c r="AY115" s="48"/>
+      <c r="AW115" s="18"/>
+      <c r="AX115" s="18"/>
+      <c r="AY115" s="71"/>
       <c r="AZ115" s="48"/>
       <c r="BA115" s="4"/>
       <c r="BB115" s="4"/>
@@ -8453,7 +8500,7 @@
       <c r="AV116" s="48"/>
       <c r="AW116" s="48"/>
       <c r="AX116" s="48"/>
-      <c r="AY116" s="48"/>
+      <c r="AY116" s="71"/>
       <c r="AZ116" s="48"/>
       <c r="BA116" s="4"/>
       <c r="BB116" s="4"/>
@@ -8464,10 +8511,8 @@
       <c r="BG116" s="4"/>
     </row>
     <row r="117" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B117" s="1"/>
+      <c r="A117" s="1"/>
+      <c r="B117" s="4"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -8516,7 +8561,7 @@
       <c r="AV117" s="48"/>
       <c r="AW117" s="48"/>
       <c r="AX117" s="48"/>
-      <c r="AY117" s="48"/>
+      <c r="AY117" s="71"/>
       <c r="AZ117" s="48"/>
       <c r="BA117" s="4"/>
       <c r="BB117" s="4"/>
@@ -8527,8 +8572,10 @@
       <c r="BG117" s="4"/>
     </row>
     <row r="118" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
-      <c r="B118" s="4"/>
+      <c r="A118" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B118" s="1"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -8577,7 +8624,7 @@
       <c r="AV118" s="48"/>
       <c r="AW118" s="48"/>
       <c r="AX118" s="48"/>
-      <c r="AY118" s="48"/>
+      <c r="AY118" s="71"/>
       <c r="AZ118" s="48"/>
       <c r="BA118" s="4"/>
       <c r="BB118" s="4"/>
@@ -8587,10 +8634,8 @@
       <c r="BF118" s="4"/>
       <c r="BG118" s="4"/>
     </row>
-    <row r="119" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
-        <v>29</v>
-      </c>
+    <row r="119" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A119" s="1"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
@@ -8613,16 +8658,16 @@
       <c r="U119" s="4"/>
       <c r="V119" s="4"/>
       <c r="W119" s="6"/>
-      <c r="X119" s="45"/>
-      <c r="Y119" s="46"/>
-      <c r="Z119" s="46"/>
-      <c r="AA119" s="46"/>
-      <c r="AB119" s="46"/>
-      <c r="AC119" s="46"/>
-      <c r="AD119" s="46"/>
-      <c r="AE119" s="46"/>
-      <c r="AF119" s="46"/>
-      <c r="AG119" s="47"/>
+      <c r="X119" s="43"/>
+      <c r="Y119" s="4"/>
+      <c r="Z119" s="4"/>
+      <c r="AA119" s="4"/>
+      <c r="AB119" s="4"/>
+      <c r="AC119" s="4"/>
+      <c r="AD119" s="4"/>
+      <c r="AE119" s="4"/>
+      <c r="AF119" s="4"/>
+      <c r="AG119" s="44"/>
       <c r="AH119" s="9"/>
       <c r="AI119" s="4"/>
       <c r="AJ119" s="4"/>
@@ -8640,7 +8685,7 @@
       <c r="AV119" s="48"/>
       <c r="AW119" s="48"/>
       <c r="AX119" s="48"/>
-      <c r="AY119" s="48"/>
+      <c r="AY119" s="71"/>
       <c r="AZ119" s="48"/>
       <c r="BA119" s="4"/>
       <c r="BB119" s="4"/>
@@ -8650,24 +8695,94 @@
       <c r="BF119" s="4"/>
       <c r="BG119" s="4"/>
     </row>
-    <row r="120" spans="1:59" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
+    <row r="120" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B120" s="4"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="4"/>
+      <c r="J120" s="4"/>
+      <c r="K120" s="4"/>
+      <c r="L120" s="4"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="4"/>
+      <c r="O120" s="4"/>
+      <c r="P120" s="4"/>
+      <c r="Q120" s="4"/>
+      <c r="R120" s="4"/>
+      <c r="S120" s="4"/>
+      <c r="T120" s="4"/>
+      <c r="U120" s="4"/>
+      <c r="V120" s="4"/>
+      <c r="W120" s="6"/>
+      <c r="X120" s="45"/>
+      <c r="Y120" s="46"/>
+      <c r="Z120" s="46"/>
+      <c r="AA120" s="46"/>
+      <c r="AB120" s="46"/>
+      <c r="AC120" s="46"/>
+      <c r="AD120" s="46"/>
+      <c r="AE120" s="46"/>
+      <c r="AF120" s="46"/>
+      <c r="AG120" s="47"/>
+      <c r="AH120" s="9"/>
+      <c r="AI120" s="4"/>
+      <c r="AJ120" s="4"/>
+      <c r="AK120" s="4"/>
+      <c r="AL120" s="4"/>
+      <c r="AM120" s="4"/>
+      <c r="AN120" s="48"/>
+      <c r="AO120" s="48"/>
+      <c r="AP120" s="48"/>
+      <c r="AQ120" s="48"/>
+      <c r="AR120" s="48"/>
+      <c r="AS120" s="48"/>
+      <c r="AT120" s="48"/>
+      <c r="AU120" s="48"/>
+      <c r="AV120" s="48"/>
+      <c r="AW120" s="48"/>
+      <c r="AX120" s="48"/>
+      <c r="AY120" s="71"/>
+      <c r="BA120" s="4"/>
+      <c r="BB120" s="4"/>
+      <c r="BC120" s="4"/>
+      <c r="BD120" s="48"/>
+      <c r="BE120" s="4"/>
+      <c r="BF120" s="4"/>
+      <c r="BG120" s="4"/>
+    </row>
+    <row r="121" spans="1:59" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:59" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A123" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B123" s="74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="126" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="127" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A127" s="2" t="s">
+    <row r="128" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="128" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A128" s="40" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="40" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add text to Metodology Chapter.
Add text and images to metodology chapter.
Moved class of hydraulic simulation to other package.
Re-generated the javadoc.
Add a new diagram and modified others.
</commit_message>
<xml_diff>
--- a/planificacion/planificacion.xlsx
+++ b/planificacion/planificacion.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EFCF70-1AC8-48A8-BE8A-D623E33D6AA0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540E6376-6A79-48F3-ADCE-ABAE6F96E3E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version anterior" sheetId="5" r:id="rId1"/>
@@ -8980,8 +8980,8 @@
   <dimension ref="A1:BG156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AV128" sqref="AV128"/>
+      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18239,12 +18239,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:T1"/>
-    <mergeCell ref="U1:Y1"/>
     <mergeCell ref="BD1:BG1"/>
     <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="AH1:AL1"/>
@@ -18252,6 +18246,12 @@
     <mergeCell ref="AQ1:AT1"/>
     <mergeCell ref="AU1:AY1"/>
     <mergeCell ref="AZ1:BC1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished documents of test cases.
Modified tooltip of buttons in MainWindow.
Litte changes in documents.
</commit_message>
<xml_diff>
--- a/planificacion/planificacion.xlsx
+++ b/planificacion/planificacion.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540E6376-6A79-48F3-ADCE-ABAE6F96E3E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA6EC07-1EE4-48B9-A968-25FB8B469322}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version anterior" sheetId="5" r:id="rId1"/>
@@ -8979,8 +8979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5ADF685-79E0-48B0-8EE7-248F90EF2AB1}">
   <dimension ref="A1:BG156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
@@ -18239,6 +18239,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:Y1"/>
     <mergeCell ref="BD1:BG1"/>
     <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="AH1:AL1"/>
@@ -18246,12 +18252,6 @@
     <mergeCell ref="AQ1:AT1"/>
     <mergeCell ref="AU1:AY1"/>
     <mergeCell ref="AZ1:BC1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:T1"/>
-    <mergeCell ref="U1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>